<commit_message>
Template: Update all hyperlinks
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_Data_Pack_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5327205C-7489-AE4C-B0FF-011DB434A7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D279E282-0D04-BF45-AFD0-D1FD86EADBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10480" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="13" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
+    <workbookView xWindow="-10480" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -7135,7 +7135,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="480">
+  <cellXfs count="478">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -7973,9 +7973,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="35" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="29" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8043,9 +8040,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="34" fillId="7" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="28" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="15" fillId="7" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13455,16 +13449,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E004659-5EB2-2446-982F-56BEFF173113}">
-  <sheetPr codeName="Sheet18">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:AN15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="14" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -13477,30 +13468,30 @@
     <col min="5" max="5" width="11.83203125" style="122" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" style="72" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" style="197" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" style="417" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="416" customWidth="1"/>
     <col min="9" max="9" width="11.83203125" style="72" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="417" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" style="416" customWidth="1"/>
     <col min="11" max="11" width="11.83203125" style="72" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" style="417" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" style="416" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" style="72" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" style="417" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="416" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" style="295" customWidth="1"/>
     <col min="16" max="17" width="11.83203125" style="72" customWidth="1"/>
-    <col min="18" max="18" width="11.83203125" style="417" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" style="416" customWidth="1"/>
     <col min="19" max="21" width="11.83203125" style="294" customWidth="1"/>
     <col min="22" max="22" width="11.83203125" style="72" customWidth="1"/>
-    <col min="23" max="23" width="11.83203125" style="420" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" style="419" customWidth="1"/>
     <col min="24" max="24" width="11.83203125" style="294" customWidth="1"/>
     <col min="25" max="25" width="11.83203125" style="72" customWidth="1"/>
-    <col min="26" max="26" width="11.83203125" style="420" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" style="419" customWidth="1"/>
     <col min="27" max="27" width="11.83203125" style="72" customWidth="1"/>
-    <col min="28" max="28" width="11.83203125" style="420" customWidth="1"/>
+    <col min="28" max="28" width="11.83203125" style="419" customWidth="1"/>
     <col min="29" max="32" width="11.83203125" style="295" customWidth="1"/>
     <col min="33" max="34" width="11.83203125" style="294" customWidth="1"/>
     <col min="35" max="36" width="11.83203125" style="72" customWidth="1"/>
-    <col min="37" max="37" width="11.83203125" style="420" customWidth="1"/>
+    <col min="37" max="37" width="11.83203125" style="419" customWidth="1"/>
     <col min="38" max="38" width="11.83203125" style="72" customWidth="1"/>
-    <col min="39" max="39" width="11.83203125" style="417" customWidth="1"/>
+    <col min="39" max="39" width="11.83203125" style="416" customWidth="1"/>
     <col min="40" max="40" width="11.83203125" style="72" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13515,7 +13506,7 @@
         <v>43</v>
       </c>
       <c r="F1" s="67"/>
-      <c r="G1" s="421"/>
+      <c r="G1" s="420"/>
       <c r="H1" s="107" t="s">
         <v>897</v>
       </c>
@@ -13715,7 +13706,7 @@
       <c r="V3" s="138" t="s">
         <v>833</v>
       </c>
-      <c r="W3" s="418" t="s">
+      <c r="W3" s="417" t="s">
         <v>834</v>
       </c>
       <c r="X3" s="351" t="s">
@@ -13724,7 +13715,7 @@
       <c r="Y3" s="138" t="s">
         <v>836</v>
       </c>
-      <c r="Z3" s="418" t="s">
+      <c r="Z3" s="417" t="s">
         <v>837</v>
       </c>
       <c r="AA3" s="138" t="s">
@@ -13843,13 +13834,13 @@
         <f>SUBTOTAL(109,V$15:INDEX(V:V,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="W4" s="419"/>
+      <c r="W4" s="418"/>
       <c r="X4" s="206"/>
       <c r="Y4" s="71">
         <f>SUBTOTAL(109,Y$15:INDEX(Y:Y,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="419" t="str">
+      <c r="Z4" s="418" t="str">
         <f>IF($Y$4=0,"",$AA$4/$Y$4)</f>
         <v/>
       </c>
@@ -13893,7 +13884,7 @@
         <f>SUBTOTAL(109,AJ$15:INDEX(AJ:AJ,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="AK4" s="419" t="str">
+      <c r="AK4" s="418" t="str">
         <f>IF($AI$4=0,"",$AL$4/$AI$4)</f>
         <v/>
       </c>
@@ -13977,7 +13968,7 @@
       <c r="V5" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="W5" s="415" t="s">
+      <c r="W5" s="414" t="s">
         <v>99</v>
       </c>
       <c r="X5" s="208" t="s">
@@ -13986,7 +13977,7 @@
       <c r="Y5" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="Z5" s="415" t="s">
+      <c r="Z5" s="414" t="s">
         <v>99</v>
       </c>
       <c r="AA5" s="72" t="s">
@@ -14019,7 +14010,7 @@
       <c r="AJ5" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="AK5" s="415" t="s">
+      <c r="AK5" s="414" t="s">
         <v>99</v>
       </c>
       <c r="AL5" s="72" t="s">
@@ -14099,7 +14090,7 @@
       <c r="V6" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="W6" s="415" t="s">
+      <c r="W6" s="414" t="s">
         <v>113</v>
       </c>
       <c r="X6" s="208" t="s">
@@ -14108,7 +14099,7 @@
       <c r="Y6" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="Z6" s="415" t="s">
+      <c r="Z6" s="414" t="s">
         <v>113</v>
       </c>
       <c r="AA6" s="72" t="s">
@@ -14141,7 +14132,7 @@
       <c r="AJ6" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="AK6" s="415" t="s">
+      <c r="AK6" s="414" t="s">
         <v>113</v>
       </c>
       <c r="AL6" s="72" t="s">
@@ -14221,7 +14212,7 @@
       <c r="V7" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="W7" s="415" t="s">
+      <c r="W7" s="414" t="s">
         <v>96</v>
       </c>
       <c r="X7" s="208" t="s">
@@ -14230,7 +14221,7 @@
       <c r="Y7" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="Z7" s="415" t="s">
+      <c r="Z7" s="414" t="s">
         <v>96</v>
       </c>
       <c r="AA7" s="72" t="s">
@@ -14263,7 +14254,7 @@
       <c r="AJ7" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="AK7" s="415" t="s">
+      <c r="AK7" s="414" t="s">
         <v>96</v>
       </c>
       <c r="AL7" s="72" t="s">
@@ -14287,7 +14278,7 @@
       <c r="F8" s="309" t="s">
         <v>286</v>
       </c>
-      <c r="G8" s="422" t="s">
+      <c r="G8" s="421" t="s">
         <v>287</v>
       </c>
       <c r="H8" s="314" t="s">
@@ -14327,12 +14318,12 @@
       <c r="V8" s="309" t="s">
         <v>185</v>
       </c>
-      <c r="W8" s="415"/>
+      <c r="W8" s="414"/>
       <c r="X8" s="208"/>
       <c r="Y8" s="309" t="s">
         <v>252</v>
       </c>
-      <c r="Z8" s="415"/>
+      <c r="Z8" s="414"/>
       <c r="AA8" s="309" t="s">
         <v>251</v>
       </c>
@@ -14353,7 +14344,7 @@
       <c r="AJ8" s="309" t="s">
         <v>183</v>
       </c>
-      <c r="AK8" s="415"/>
+      <c r="AK8" s="414"/>
       <c r="AL8" s="309" t="s">
         <v>248</v>
       </c>
@@ -14371,7 +14362,7 @@
       <c r="D9" s="66"/>
       <c r="E9" s="311"/>
       <c r="F9" s="309"/>
-      <c r="G9" s="422"/>
+      <c r="G9" s="421"/>
       <c r="H9" s="314" t="s">
         <v>188</v>
       </c>
@@ -14409,12 +14400,12 @@
       <c r="V9" s="309" t="s">
         <v>186</v>
       </c>
-      <c r="W9" s="415"/>
+      <c r="W9" s="414"/>
       <c r="X9" s="208"/>
       <c r="Y9" s="309" t="s">
         <v>253</v>
       </c>
-      <c r="Z9" s="415"/>
+      <c r="Z9" s="414"/>
       <c r="AA9" s="309" t="s">
         <v>250</v>
       </c>
@@ -14435,7 +14426,7 @@
       <c r="AJ9" s="309" t="s">
         <v>184</v>
       </c>
-      <c r="AK9" s="415"/>
+      <c r="AK9" s="414"/>
       <c r="AL9" s="309" t="s">
         <v>289</v>
       </c>
@@ -14455,7 +14446,7 @@
       <c r="F10" s="309" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="422" t="s">
+      <c r="G10" s="421" t="s">
         <v>105</v>
       </c>
       <c r="H10" s="314"/>
@@ -14483,12 +14474,12 @@
       <c r="V10" s="309" t="s">
         <v>105</v>
       </c>
-      <c r="W10" s="415"/>
+      <c r="W10" s="414"/>
       <c r="X10" s="208"/>
       <c r="Y10" s="309" t="s">
         <v>105</v>
       </c>
-      <c r="Z10" s="415"/>
+      <c r="Z10" s="414"/>
       <c r="AA10" s="309" t="s">
         <v>105</v>
       </c>
@@ -14509,7 +14500,7 @@
       <c r="AJ10" s="309" t="s">
         <v>122</v>
       </c>
-      <c r="AK10" s="415"/>
+      <c r="AK10" s="414"/>
       <c r="AL10" s="309" t="s">
         <v>105</v>
       </c>
@@ -14523,7 +14514,7 @@
       <c r="D11" s="66"/>
       <c r="E11" s="122"/>
       <c r="F11" s="119"/>
-      <c r="G11" s="423"/>
+      <c r="G11" s="422"/>
       <c r="H11" s="98"/>
       <c r="I11" s="72"/>
       <c r="J11" s="233"/>
@@ -14539,10 +14530,10 @@
       <c r="T11" s="208"/>
       <c r="U11" s="208"/>
       <c r="V11" s="72"/>
-      <c r="W11" s="415"/>
+      <c r="W11" s="414"/>
       <c r="X11" s="208"/>
       <c r="Y11" s="72"/>
-      <c r="Z11" s="415"/>
+      <c r="Z11" s="414"/>
       <c r="AA11" s="72"/>
       <c r="AB11" s="161"/>
       <c r="AC11" s="75"/>
@@ -14553,7 +14544,7 @@
       <c r="AH11" s="208"/>
       <c r="AI11" s="72"/>
       <c r="AJ11" s="72"/>
-      <c r="AK11" s="415"/>
+      <c r="AK11" s="414"/>
       <c r="AL11" s="72"/>
       <c r="AM11" s="98"/>
       <c r="AN11" s="72"/>
@@ -14581,10 +14572,10 @@
       <c r="T12" s="208"/>
       <c r="U12" s="208"/>
       <c r="V12" s="72"/>
-      <c r="W12" s="415"/>
+      <c r="W12" s="414"/>
       <c r="X12" s="208"/>
       <c r="Y12" s="72"/>
-      <c r="Z12" s="415"/>
+      <c r="Z12" s="414"/>
       <c r="AA12" s="72"/>
       <c r="AB12" s="161"/>
       <c r="AC12" s="75"/>
@@ -14595,7 +14586,7 @@
       <c r="AH12" s="208"/>
       <c r="AI12" s="72"/>
       <c r="AJ12" s="72"/>
-      <c r="AK12" s="415"/>
+      <c r="AK12" s="414"/>
       <c r="AL12" s="72"/>
       <c r="AM12" s="98"/>
       <c r="AN12" s="72"/>
@@ -14659,7 +14650,7 @@
       <c r="V13" s="72" t="s">
         <v>697</v>
       </c>
-      <c r="W13" s="415" t="s">
+      <c r="W13" s="414" t="s">
         <v>697</v>
       </c>
       <c r="X13" s="208" t="s">
@@ -14668,7 +14659,7 @@
       <c r="Y13" s="72" t="s">
         <v>697</v>
       </c>
-      <c r="Z13" s="415" t="s">
+      <c r="Z13" s="414" t="s">
         <v>697</v>
       </c>
       <c r="AA13" s="72" t="s">
@@ -14701,7 +14692,7 @@
       <c r="AJ13" s="72" t="s">
         <v>697</v>
       </c>
-      <c r="AK13" s="415" t="s">
+      <c r="AK13" s="414" t="s">
         <v>697</v>
       </c>
       <c r="AL13" s="72" t="s">
@@ -15002,16 +14993,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B895D15E-C6E2-A247-9FD1-CA32101F4B03}">
-  <sheetPr codeName="Sheet15">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:CC15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -15022,35 +15010,35 @@
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" customWidth="1"/>
     <col min="5" max="5" width="7" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="416" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="415" customWidth="1"/>
     <col min="7" max="15" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" style="416" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" style="415" customWidth="1"/>
     <col min="17" max="33" width="11.83203125" customWidth="1"/>
-    <col min="34" max="34" width="11.83203125" style="416" customWidth="1"/>
+    <col min="34" max="34" width="11.83203125" style="415" customWidth="1"/>
     <col min="35" max="36" width="11.83203125" customWidth="1"/>
-    <col min="37" max="37" width="11.83203125" style="416" customWidth="1"/>
+    <col min="37" max="37" width="11.83203125" style="415" customWidth="1"/>
     <col min="38" max="39" width="11.83203125" customWidth="1"/>
-    <col min="40" max="40" width="11.83203125" style="416" customWidth="1"/>
+    <col min="40" max="40" width="11.83203125" style="415" customWidth="1"/>
     <col min="41" max="42" width="11.83203125" customWidth="1"/>
-    <col min="43" max="43" width="11.83203125" style="416" customWidth="1"/>
+    <col min="43" max="43" width="11.83203125" style="415" customWidth="1"/>
     <col min="44" max="45" width="11.83203125" customWidth="1"/>
-    <col min="46" max="46" width="11.83203125" style="416" customWidth="1"/>
+    <col min="46" max="46" width="11.83203125" style="415" customWidth="1"/>
     <col min="47" max="48" width="11.83203125" customWidth="1"/>
-    <col min="49" max="49" width="11.83203125" style="416" customWidth="1"/>
+    <col min="49" max="49" width="11.83203125" style="415" customWidth="1"/>
     <col min="50" max="51" width="11.83203125" customWidth="1"/>
-    <col min="52" max="52" width="11.83203125" style="416" customWidth="1"/>
+    <col min="52" max="52" width="11.83203125" style="415" customWidth="1"/>
     <col min="53" max="54" width="11.83203125" customWidth="1"/>
-    <col min="55" max="55" width="11.83203125" style="416" customWidth="1"/>
+    <col min="55" max="55" width="11.83203125" style="415" customWidth="1"/>
     <col min="56" max="57" width="11.83203125" customWidth="1"/>
-    <col min="58" max="58" width="11.83203125" style="416" customWidth="1"/>
+    <col min="58" max="58" width="11.83203125" style="415" customWidth="1"/>
     <col min="59" max="60" width="11.83203125" customWidth="1"/>
-    <col min="61" max="61" width="11.83203125" style="416" customWidth="1"/>
+    <col min="61" max="61" width="11.83203125" style="415" customWidth="1"/>
     <col min="62" max="63" width="11.83203125" customWidth="1"/>
-    <col min="64" max="64" width="11.83203125" style="416" customWidth="1"/>
+    <col min="64" max="64" width="11.83203125" style="415" customWidth="1"/>
     <col min="65" max="66" width="11.83203125" customWidth="1"/>
-    <col min="67" max="67" width="11.83203125" style="416" customWidth="1"/>
+    <col min="67" max="67" width="11.83203125" style="415" customWidth="1"/>
     <col min="68" max="78" width="11.83203125" customWidth="1"/>
-    <col min="79" max="79" width="11.83203125" style="416" customWidth="1"/>
+    <col min="79" max="79" width="11.83203125" style="415" customWidth="1"/>
     <col min="80" max="81" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15170,10 +15158,10 @@
       <c r="CC1" s="67"/>
     </row>
     <row r="2" spans="1:81" s="56" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="479" t="s">
+      <c r="A2" s="477" t="s">
         <v>770</v>
       </c>
-      <c r="B2" s="476"/>
+      <c r="B2" s="474"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -15319,8 +15307,8 @@
       </c>
     </row>
     <row r="3" spans="1:81" s="40" customFormat="1" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477"/>
-      <c r="B3" s="478"/>
+      <c r="A3" s="475"/>
+      <c r="B3" s="476"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
@@ -17812,19 +17800,19 @@
         <v/>
       </c>
       <c r="K15" s="118" t="str" cm="1">
-        <f t="array" ref="K15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CB:$CB,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CB:$CB,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="K15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(PMTCT!$AF:$AF,PMTCT!$B:$B,$B15,PMTCT!$C:$C,{"50-54","55-59","60-64","65+"},PMTCT!$D:$D,$D15)),INDEX(PMTCT!$AF:$AF,MATCH($E15,PMTCT!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="L15" s="118" t="str" cm="1">
-        <f t="array" ref="L15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CC:$CC,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CC:$CC,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="L15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(PMTCT!$AV:$AV,PMTCT!$B:$B,$B15,PMTCT!$C:$C,{"50-54","55-59","60-64","65+"},PMTCT!$D:$D,$D15)),INDEX(PMTCT!$AV:$AV,MATCH($E15,PMTCT!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="M15" s="118" t="str" cm="1">
-        <f t="array" ref="M15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CD:$CD,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CD:$CD,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="M15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(TB!$Q:$Q,TB!$B:$B,$B15,TB!$C:$C,{"50-54","55-59","60-64","65+"},TB!$D:$D,$D15)),INDEX(TB!$Q:$Q,MATCH($E15,TB!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="N15" s="118" t="str" cm="1">
-        <f t="array" ref="N15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CE:$CE,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CE:$CE,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="N15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(VMMC!$AC:$AC,VMMC!$B:$B,$B15,VMMC!$C:$C,{"50-54","55-59","60-64","65+"},VMMC!$D:$D,$D15)),INDEX(VMMC!$AC:$AC,MATCH($E15,VMMC!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="O15" s="118" t="str" cm="1">
@@ -18103,14 +18091,14 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="AD3" location="HTS!BH:BJ" display="Community - Mobile (%)" xr:uid="{E006FFAE-7A20-8446-BB9D-C5A63ED5CBAE}"/>
-    <hyperlink ref="AF3" location="HTS!BK:BM" display="Community - Other (%)" xr:uid="{7A0718ED-A870-5F4A-982F-22250833ED99}"/>
-    <hyperlink ref="Z3" location="HTS!AY:BA" display="Facility - Emergency (%)" xr:uid="{F8868817-83DA-1041-91DD-0FC127E99A1C}"/>
-    <hyperlink ref="V3" location="HTS!AM:AO" display="Facility - Inpatient (%)" xr:uid="{BED9E3C6-D94E-C84E-AEAC-BAD225ACA845}"/>
-    <hyperlink ref="X3" location="HTS!AS:AU" display="Facility - Malnutrition (%)" xr:uid="{5F946879-2C14-D84E-8357-DCB4BEBFB4BC}"/>
-    <hyperlink ref="W3" location="HTS!AP:AR" display="Facility - Pediatric (%)" xr:uid="{F80E706B-39B3-EA45-82C1-8666C2766CD2}"/>
-    <hyperlink ref="AB3" location="HTS!BE:BG" display="Facility - VCT (%)" xr:uid="{96AFECA4-8D1E-9143-A4C2-035297061790}"/>
-    <hyperlink ref="AA3" location="HTS!BB:BD" display="Facility - Other PITC (%)" xr:uid="{A6056D15-DE6D-9D43-9343-4416F177D27E}"/>
+    <hyperlink ref="AD3" location="HTS!BG:BG" display="Community - Mobile (%)" xr:uid="{E006FFAE-7A20-8446-BB9D-C5A63ED5CBAE}"/>
+    <hyperlink ref="AF3" location="HTS!BM:BM" display="Community - Other (%)" xr:uid="{7A0718ED-A870-5F4A-982F-22250833ED99}"/>
+    <hyperlink ref="Z3" location="HTS!AU:AU" display="Facility - Emergency (%)" xr:uid="{F8868817-83DA-1041-91DD-0FC127E99A1C}"/>
+    <hyperlink ref="V3" location="HTS!AI:AI" display="Facility - Inpatient (%)" xr:uid="{BED9E3C6-D94E-C84E-AEAC-BAD225ACA845}"/>
+    <hyperlink ref="X3" location="HTS!AO:AO" display="Facility - Malnutrition (%)" xr:uid="{5F946879-2C14-D84E-8357-DCB4BEBFB4BC}"/>
+    <hyperlink ref="W3" location="HTS!AL:AL" display="Facility - Pediatric (%)" xr:uid="{F80E706B-39B3-EA45-82C1-8666C2766CD2}"/>
+    <hyperlink ref="AB3" location="HTS!BA:BA" display="Facility - VCT (%)" xr:uid="{96AFECA4-8D1E-9143-A4C2-035297061790}"/>
+    <hyperlink ref="AA3" location="HTS!AX:AX" display="Facility - Other PITC (%)" xr:uid="{A6056D15-DE6D-9D43-9343-4416F177D27E}"/>
     <hyperlink ref="BG3" location="HTS!AD:AD" display="Positive" xr:uid="{B6561B91-32AC-4E43-909B-006C5857E9D3}"/>
     <hyperlink ref="BM3" location="HTS!AF:AF" display="Positive" xr:uid="{36F19663-692F-0B4E-A735-36B1A8B45174}"/>
     <hyperlink ref="AU3" location="HTS!Z:Z" display="Positive" xr:uid="{5F925F42-4472-D64A-B673-9242301DC80B}"/>
@@ -18120,32 +18108,34 @@
     <hyperlink ref="AR3" location="HTS!Y:Y" display="Positive" xr:uid="{A6D67445-60DB-7B4D-BE45-D8028AC6C038}"/>
     <hyperlink ref="BA3" location="HTS!AB:AB" display="Positive" xr:uid="{47D345C0-E172-384E-9A54-1662548C7E60}"/>
     <hyperlink ref="AX3" location="HTS!AA:AA" display="Positive" xr:uid="{3BC8C9A7-8313-D648-B559-71BED3A00FD5}"/>
-    <hyperlink ref="Q3" location="Cascade!CH:CH" display="HTS_INDEX_FAC: Positive (%)" xr:uid="{1FD13CB4-2815-714C-9E0D-BFA34EC9A074}"/>
-    <hyperlink ref="Y3" location="HTS!AV:AX" display="Facility - STI Clinic (%)" xr:uid="{43C8E104-EDFB-E34B-97AD-5266A520E66C}"/>
-    <hyperlink ref="P3" location="Cascade!CG:CG" display="HTS_INDEX_COM: Positive (%)" xr:uid="{2BA35798-2920-0047-9263-AE9138D115BC}"/>
+    <hyperlink ref="Q3" location="HTS!J:J" display="HTS_INDEX_FAC: Positive (%)" xr:uid="{1FD13CB4-2815-714C-9E0D-BFA34EC9A074}"/>
+    <hyperlink ref="Y3" location="HTS!AR:AR" display="Facility - STI Clinic (%)" xr:uid="{43C8E104-EDFB-E34B-97AD-5266A520E66C}"/>
+    <hyperlink ref="P3" location="HTS!I:I" display="HTS_INDEX_COM: Positive (%)" xr:uid="{2BA35798-2920-0047-9263-AE9138D115BC}"/>
     <hyperlink ref="BO3" location="HTS!H:H" display="Original HTS_TST_POS (FY23)" xr:uid="{7CF79D4A-82ED-0A43-A4E4-43F4ED251182}"/>
-    <hyperlink ref="T3" location="Cascade!BS:BS" display="TB_STAT: New Positive (%)" xr:uid="{18C28BD3-FAC2-974A-A3D5-9CF1B26C23FA}"/>
-    <hyperlink ref="S3" location="Cascade!BR:BR" display="HTS_TST PMTCT Post ANC1: Positive (%)" xr:uid="{F1FC89C1-DC5F-B840-AAF9-44A1F4477F09}"/>
-    <hyperlink ref="U3" location="Cascade!BT:BT" display="VMMC_CIRC: HIV Positive (%)" xr:uid="{B1FE978A-966A-8843-8592-43CD0B9E86E3}"/>
-    <hyperlink ref="F3" location="Cascade!Z:Z" display="Host Country Est. ART Coverage (FY22) (%)" xr:uid="{62E0A0AF-20D9-6845-8B29-307EB64A2270}"/>
-    <hyperlink ref="H3" location="Cascade!BO:BO" display="Total HTS_TST_POS (FY23)" xr:uid="{4F5D648D-D7C2-5348-BC20-3F43FA74D673}"/>
-    <hyperlink ref="I3" location="Cascade!CI:CI" display="HTS_INDEX Community Positives (FY23)" xr:uid="{F10D394A-A559-CD44-A6BB-3657FE272021}"/>
-    <hyperlink ref="K3" location="Cascade!BQ:BQ" display="PMTCT_STAT New Positives (FY23)" xr:uid="{812A1C32-C461-DA45-A52E-F20D4356FFAA}"/>
-    <hyperlink ref="L3" location="Cascade!BR:BR" display="HTS_TST Post ANC1 New Positives (FY23)" xr:uid="{D8D811EC-2ACC-F544-8B0B-9B3CA11DE028}"/>
-    <hyperlink ref="M3" location="Cascade!BS:BS" display="TB_STAT New Positives (FY23)" xr:uid="{E57FF0A3-0CCA-514F-A80D-BBE50EC0318F}"/>
-    <hyperlink ref="N3" location="Cascade!BT:BT" display="VMMC_CIRC New Positives (FY23)" xr:uid="{844A055A-478B-6640-9164-F1EA9117BE57}"/>
-    <hyperlink ref="O3" location="Cascade!BV:BV" display="HTS_TST_POS from All Other Modalities (FY23)" xr:uid="{C5277E53-10C0-2243-A9D4-1D88FF90A312}"/>
+    <hyperlink ref="T3" location="HTS!M:M" display="TB_STAT: New Positive (%)" xr:uid="{18C28BD3-FAC2-974A-A3D5-9CF1B26C23FA}"/>
+    <hyperlink ref="S3" location="HTS!L:L" display="HTS_TST PMTCT Post ANC1: Positive (%)" xr:uid="{F1FC89C1-DC5F-B840-AAF9-44A1F4477F09}"/>
+    <hyperlink ref="U3" location="HTS!N:N" display="VMMC_CIRC: HIV Positive (%)" xr:uid="{B1FE978A-966A-8843-8592-43CD0B9E86E3}"/>
+    <hyperlink ref="F3" location="Cascade!BS:BS" display="Host Country Est. ART Coverage (FY22) (%)" xr:uid="{62E0A0AF-20D9-6845-8B29-307EB64A2270}"/>
+    <hyperlink ref="H3" location="Cascade!BZ:BZ" display="Total HTS_TST_POS (FY23)" xr:uid="{4F5D648D-D7C2-5348-BC20-3F43FA74D673}"/>
+    <hyperlink ref="I3" location="Cascade!CR:CR" display="HTS_INDEX Community Positives (FY23)" xr:uid="{F10D394A-A559-CD44-A6BB-3657FE272021}"/>
+    <hyperlink ref="K3" location="PMTCT!AF:AF" display="PMTCT_STAT New Positives (FY23)" xr:uid="{812A1C32-C461-DA45-A52E-F20D4356FFAA}"/>
+    <hyperlink ref="L3" location="PMTCT!AV:AV" display="HTS_TST Post ANC1 New Positives (FY23)" xr:uid="{D8D811EC-2ACC-F544-8B0B-9B3CA11DE028}"/>
+    <hyperlink ref="M3" location="TB!Q:Q" display="TB_STAT New Positives (FY23)" xr:uid="{E57FF0A3-0CCA-514F-A80D-BBE50EC0318F}"/>
+    <hyperlink ref="N3" location="VMMC!AC:AC" display="VMMC_CIRC New Positives (FY23)" xr:uid="{844A055A-478B-6640-9164-F1EA9117BE57}"/>
+    <hyperlink ref="O3" location="Cascade!CG:CG" display="HTS_TST_POS from All Other Modalities (FY23)" xr:uid="{C5277E53-10C0-2243-A9D4-1D88FF90A312}"/>
     <hyperlink ref="BT3" location="PMTCT!AG:AG" display="PMTCT_STAT New Negatives (FY23)" xr:uid="{59410773-B3DC-854C-945D-B45072CA61F7}"/>
     <hyperlink ref="BU3" location="PMTCT!AW:AW" display="HTS_TST Post ANC1 Negatives (FY23)" xr:uid="{C61C3228-0418-F04A-A70D-6531131C0C12}"/>
     <hyperlink ref="BV3" location="TB!R:R" display="TB_STAT New Negatives (FY22)" xr:uid="{86527BC9-57C0-1640-BE6B-CB6BEA15D2D3}"/>
     <hyperlink ref="BW3" location="VMMC!AD:AD" display="VMMC_CIRC Negatives (FY22)" xr:uid="{3AD47724-6BB1-D148-BE45-144B25A52781}"/>
-    <hyperlink ref="J3" location="Cascade!CK:CK" display="HTS_INDEX Facility Positives (FY23)" xr:uid="{F530B28A-AF9A-CF45-8C43-7C26547A0809}"/>
-    <hyperlink ref="BR3" location="Cascade!CJ:CJ" display="HTS_INDEX Community New Negatives (FY23)" xr:uid="{7614C962-EB54-114D-8144-33CC1CCC8A19}"/>
-    <hyperlink ref="BS3" location="Cascade!CL:CL" display="HTS_INDEX Facility New Negatives (FY23)" xr:uid="{9F773D86-C36C-D14F-AD2D-78557CF866D2}"/>
-    <hyperlink ref="G3" location="Cascade!AA:AA" display="Host Country Est. Population VLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{F30F0EE7-FFA9-BF42-AF25-EB64195A4AA3}"/>
-    <hyperlink ref="R3" location="Cascade!BQ:BQ" display="PMTCT_STAT: New Positive (%)" xr:uid="{92A92D18-3020-A74B-ACBE-46783EF61EC0}"/>
+    <hyperlink ref="J3" location="Cascade!CT:CT" display="HTS_INDEX Facility Positives (FY23)" xr:uid="{F530B28A-AF9A-CF45-8C43-7C26547A0809}"/>
+    <hyperlink ref="BR3" location="Cascade!CS:CS" display="HTS_INDEX Community New Negatives (FY23)" xr:uid="{7614C962-EB54-114D-8144-33CC1CCC8A19}"/>
+    <hyperlink ref="BS3" location="Cascade!CU:CU" display="HTS_INDEX Facility New Negatives (FY23)" xr:uid="{9F773D86-C36C-D14F-AD2D-78557CF866D2}"/>
+    <hyperlink ref="G3" location="Cascade!AL:AL" display="Host Country Est. PopVLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{F30F0EE7-FFA9-BF42-AF25-EB64195A4AA3}"/>
+    <hyperlink ref="R3" location="HTS!K:K" display="PMTCT_STAT: New Positive (%)" xr:uid="{92A92D18-3020-A74B-ACBE-46783EF61EC0}"/>
     <hyperlink ref="BD3" location="HTS!AC:AC" display="Positive" xr:uid="{0268EFB4-1FE0-9648-AF9F-08E2D9DE337E}"/>
     <hyperlink ref="BJ3" location="HTS!AE:AE" display="Positive" xr:uid="{B454ED51-6EC1-7B42-9E3A-5E8EDC3280D5}"/>
+    <hyperlink ref="AC3" location="HTS!BD:BD" display="Facility - SNS (%)" xr:uid="{9C6B8EB4-E4CD-324E-A7F8-FFA83D1EE966}"/>
+    <hyperlink ref="AE3" location="HTS!BJ:BJ" display="Community - SNS (%)" xr:uid="{84A2FAC0-0B4D-F443-89ED-C6285FAEB9CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18155,16 +18145,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F12E676-4E0B-9F4C-AD46-AC4FAA82FFF4}">
-  <sheetPr codeName="Sheet14">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -18200,10 +18187,10 @@
       <c r="K1" s="67"/>
     </row>
     <row r="2" spans="1:11" s="56" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="479" t="s">
+      <c r="A2" s="477" t="s">
         <v>759</v>
       </c>
-      <c r="B2" s="476"/>
+      <c r="B2" s="474"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -18221,8 +18208,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477"/>
-      <c r="B3" s="478"/>
+      <c r="A3" s="475"/>
+      <c r="B3" s="476"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
@@ -18235,7 +18222,7 @@
       <c r="H3" s="256" t="s">
         <v>789</v>
       </c>
-      <c r="I3" s="424" t="s">
+      <c r="I3" s="423" t="s">
         <v>864</v>
       </c>
       <c r="J3" s="48" t="s">
@@ -18525,7 +18512,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H3" location="Cascade!BF:BF" display="TX_CURR (FY23)" xr:uid="{C5312933-D9B2-F74B-8895-8CDF64C56415}"/>
+    <hyperlink ref="H3" location="Cascade!BQ:BQ" display="TX_CURR (FY23)" xr:uid="{C5312933-D9B2-F74B-8895-8CDF64C56415}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18535,16 +18522,12 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8E0FAD-753E-5846-9F49-2165927EA2B9}">
-  <sheetPr>
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
   <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -19344,7 +19327,7 @@
         <v>222</v>
       </c>
       <c r="R8" s="331"/>
-      <c r="S8" s="425" t="s">
+      <c r="S8" s="424" t="s">
         <v>224</v>
       </c>
       <c r="T8" s="331"/>
@@ -20000,9 +19983,9 @@
   <hyperlinks>
     <hyperlink ref="J3" location="TB!Q:Q" display="% of Positives" xr:uid="{C240581F-0312-414F-99B5-7DC0EEDCE2D4}"/>
     <hyperlink ref="R3" location="HTS!AI:AI" display="% of Positives" xr:uid="{BCB03ADB-EB0F-9449-B4AD-8CCCC65196F5}"/>
-    <hyperlink ref="P3" location="Cascade!CK:CK" display="% of Positives" xr:uid="{F5E990DE-DF37-E84A-B2EC-94F34D61814F}"/>
-    <hyperlink ref="N3" location="Cascade!CI:CI" display="% of Positives" xr:uid="{8E652247-ECD7-3148-9B98-BE20BACDD9E8}"/>
-    <hyperlink ref="F3" location="PMTCT!AC:AC" display="% of Positives" xr:uid="{F2B49097-C594-1242-BE6B-4FE63474113E}"/>
+    <hyperlink ref="P3" location="Cascade!CT:CT" display="% of Positives" xr:uid="{F5E990DE-DF37-E84A-B2EC-94F34D61814F}"/>
+    <hyperlink ref="N3" location="Cascade!CR:CR" display="% of Positives" xr:uid="{8E652247-ECD7-3148-9B98-BE20BACDD9E8}"/>
+    <hyperlink ref="F3" location="PMTCT!AF:AF" display="% of Positives" xr:uid="{F2B49097-C594-1242-BE6B-4FE63474113E}"/>
     <hyperlink ref="H3" location="PMTCT!AV:AV" display="% of Positives" xr:uid="{564F8A9F-7394-CC4D-8071-B2C639592C77}"/>
     <hyperlink ref="L3" location="VMMC!AC:AC" display="% of Positives" xr:uid="{475FB800-421E-EC40-BC04-9B9751E0C7DD}"/>
     <hyperlink ref="T3" location="HTS!AR:AR" display="% of Positives" xr:uid="{FD6CB84C-216C-654C-BB3E-E6A97699BD36}"/>
@@ -20010,9 +19993,9 @@
     <hyperlink ref="X3" location="HTS!AX:AX" display="% of Positives" xr:uid="{BF7AE90C-BE91-3747-B0FE-18CFAFCA5903}"/>
     <hyperlink ref="Z3" location="HTS!BA:BA" display="% of Positives" xr:uid="{F60E015E-CE75-8F41-BA1B-C29B78A260DE}"/>
     <hyperlink ref="AD3" location="HTS!BG:BG" display="% of Positives" xr:uid="{20E22653-A2B8-F54C-8011-D998703856A1}"/>
-    <hyperlink ref="AH3" location="HTS!BJ:BJ" display="% of Positives" xr:uid="{94ACC59F-8D64-8345-AB6E-13194DAC8C67}"/>
+    <hyperlink ref="AH3" location="HTS!BM:BM" display="% of Positives" xr:uid="{94ACC59F-8D64-8345-AB6E-13194DAC8C67}"/>
     <hyperlink ref="AK3" location="HTS!BP:BP" display="Final HTS_TST_POS (FY23)" xr:uid="{0E85C024-3561-CF4E-9219-3D965CFB99EF}"/>
-    <hyperlink ref="AF3" location="HTS!BM:BM" display="% of Positives" xr:uid="{DA0A7933-ED09-FA43-85EA-CBB3FC01514D}"/>
+    <hyperlink ref="AF3" location="HTS!BJ:BJ" display="% of Positives" xr:uid="{DA0A7933-ED09-FA43-85EA-CBB3FC01514D}"/>
     <hyperlink ref="AB3" location="HTS!BD:BD" display="% of Positives" xr:uid="{C9C1977D-B4BA-D94C-8FED-05182F234A59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20023,16 +20006,13 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF8812F-6C9B-A843-9B36-4ED7666FB762}">
-  <sheetPr codeName="Sheet16">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:AC15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -21059,8 +21039,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F3" location="Cascade!BB:BB" display="TX_NEW (FY23)" xr:uid="{27BB3583-6C2F-684A-B303-5786DBB117DD}"/>
-    <hyperlink ref="G3" location="Cascade!AL:AL" display="TX_CURR (FY22)" xr:uid="{B1CE3692-2A00-864A-BB76-1FA9031F16FD}"/>
+    <hyperlink ref="F3" location="Cascade!BN:BN" display="TX_NEW (FY23)" xr:uid="{27BB3583-6C2F-684A-B303-5786DBB117DD}"/>
+    <hyperlink ref="G3" location="Cascade!AG:AG" display="TX_CURR (FY22)" xr:uid="{B1CE3692-2A00-864A-BB76-1FA9031F16FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -21070,16 +21050,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93744E4D-1895-6D4A-964C-B9B7D995502D}">
-  <sheetPr codeName="Sheet19">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -21336,16 +21313,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB1BDFE-6D2F-9B4B-8CDF-D9B4D3891FD5}">
-  <sheetPr codeName="Sheet17">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -22046,7 +22020,7 @@
         <v>||</v>
       </c>
       <c r="F15" s="75" t="str" cm="1">
-        <f t="array" ref="F15">IFERROR(1/(1/IF(OR($C15="15-17",$C15="18-20"),INDEX(Cascade!$F:$F,MATCH($B15&amp;"|"&amp;"15-19"&amp;"|"&amp;$D15,Cascade!$E:$E,0))/2,IF($C15="18+",SUM(SUMIFS(Cascade!$F:$F,Cascade!$B:$B,$B15,Cascade!$C:$C,{"20-24","25-29","30-34","35-39","40-44","45-49","50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$F:$F,MATCH($E15,Cascade!$E:$E,0))))),"")</f>
+        <f t="array" ref="F15">IFERROR(1/(1/IF(OR($C15="15-17",$C15="18-20"),ROUND(INDEX(Cascade!$H:$H,MATCH($B15&amp;"|"&amp;"15-19"&amp;"|"&amp;$D15,Cascade!$E:$E,0))/2,0),IF($C15="18+",SUM(SUMIFS(Cascade!$H:$H,Cascade!$B:$B,$B15,Cascade!$C:$C,{"20-24","25-29","30-34","35-39","40-44","45-49","50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$H:$H,MATCH($E15,Cascade!$E:$E,0))))),"")</f>
         <v/>
       </c>
       <c r="G15" s="181"/>
@@ -22147,16 +22121,12 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57791FBB-5296-C84C-951A-EBCEC0739F22}">
-  <sheetPr>
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="14" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -22176,12 +22146,12 @@
         <v>14</v>
       </c>
       <c r="B1" s="46"/>
-      <c r="C1" s="427" t="s">
+      <c r="C1" s="426" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="142"/>
-      <c r="E1" s="426"/>
-      <c r="F1" s="426"/>
+      <c r="E1" s="425"/>
+      <c r="F1" s="425"/>
       <c r="G1" s="142"/>
       <c r="H1" s="142"/>
     </row>
@@ -22446,16 +22416,12 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8D3DDC-1471-8141-9FF6-8D47FF9D86B6}">
-  <sheetPr>
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -22502,10 +22468,10 @@
       <c r="V1" s="67"/>
     </row>
     <row r="2" spans="1:22" s="56" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="479" t="s">
+      <c r="A2" s="477" t="s">
         <v>1027</v>
       </c>
-      <c r="B2" s="476"/>
+      <c r="B2" s="474"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -22534,12 +22500,12 @@
       <c r="V2" s="68"/>
     </row>
     <row r="3" spans="1:22" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477"/>
-      <c r="B3" s="478"/>
+      <c r="A3" s="475"/>
+      <c r="B3" s="476"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
-      <c r="F3" s="430" t="s">
+      <c r="F3" s="429" t="s">
         <v>809</v>
       </c>
       <c r="G3" s="76" t="s">
@@ -22886,7 +22852,7 @@
         <v>487</v>
       </c>
       <c r="Q8" s="173"/>
-      <c r="R8" s="429"/>
+      <c r="R8" s="428"/>
       <c r="U8" s="309" t="s">
         <v>707</v>
       </c>
@@ -22907,7 +22873,7 @@
       <c r="O9" s="317"/>
       <c r="P9" s="317"/>
       <c r="Q9" s="215"/>
-      <c r="R9" s="428"/>
+      <c r="R9" s="427"/>
       <c r="U9" s="309"/>
       <c r="V9" s="309"/>
     </row>
@@ -22932,9 +22898,9 @@
         <v>1033</v>
       </c>
       <c r="Q10" s="173"/>
-      <c r="R10" s="429"/>
-      <c r="S10" s="429"/>
-      <c r="T10" s="429"/>
+      <c r="R10" s="428"/>
+      <c r="S10" s="428"/>
+      <c r="T10" s="428"/>
       <c r="U10" s="309" t="s">
         <v>718</v>
       </c>
@@ -23220,17 +23186,14 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6399F038-EC48-4048-B5DA-2BA7ACE5CEC5}">
-  <sheetPr codeName="Sheet20">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23689,7 +23652,7 @@
         <v>||</v>
       </c>
       <c r="F15" s="98" t="str" cm="1">
-        <f t="array" ref="F15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$F:$F,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$F:$F,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="F15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$H:$H,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$H:$H,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="G15" s="75" t="str">
@@ -23757,10 +23720,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="469" t="s">
+      <c r="A1" s="467" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="469"/>
+      <c r="B1" s="467"/>
       <c r="C1" s="22"/>
       <c r="D1" s="23" t="str">
         <f>"Hello, "&amp;Home!$B$20&amp;" Team"</f>
@@ -23781,15 +23744,15 @@
       <c r="Q1" s="22"/>
       <c r="R1" s="24" t="str">
         <f ca="1">TEXT(TODAY(),"ddd, mmm dd")</f>
-        <v>Wed, Dec 29</v>
+        <v>Thu, Dec 30</v>
       </c>
       <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="470" t="s">
+      <c r="A2" s="468" t="s">
         <v>1094</v>
       </c>
-      <c r="B2" s="470"/>
+      <c r="B2" s="468"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -23887,33 +23850,33 @@
       <c r="A6" s="13"/>
       <c r="B6" s="14"/>
       <c r="C6" s="22"/>
-      <c r="D6" s="466" t="str">
+      <c r="D6" s="464" t="str">
         <f>IFERROR(SUM(Cascade!$T:$T)/SUM(Cascade!$H:$H),"")</f>
         <v/>
       </c>
-      <c r="E6" s="467"/>
-      <c r="F6" s="468"/>
+      <c r="E6" s="465"/>
+      <c r="F6" s="466"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="471">
+      <c r="H6" s="469">
         <f>SUM(Cascade!$T:$T)-Cascade!$T$4</f>
         <v>0</v>
       </c>
-      <c r="I6" s="472"/>
-      <c r="J6" s="473"/>
+      <c r="I6" s="470"/>
+      <c r="J6" s="471"/>
       <c r="K6" s="22"/>
-      <c r="L6" s="471">
+      <c r="L6" s="469">
         <f>SUM(Cascade!$BQ:$BQ)-Cascade!$BQ$4</f>
         <v>0</v>
       </c>
-      <c r="M6" s="472"/>
-      <c r="N6" s="473"/>
+      <c r="M6" s="470"/>
+      <c r="N6" s="471"/>
       <c r="O6" s="22"/>
-      <c r="P6" s="466" t="str">
+      <c r="P6" s="464" t="str">
         <f>IFERROR(SUM(Cascade!$H:$H)/SUM(Cascade!$F:$F),"")</f>
         <v/>
       </c>
-      <c r="Q6" s="467"/>
-      <c r="R6" s="468"/>
+      <c r="Q6" s="465"/>
+      <c r="R6" s="466"/>
       <c r="S6" s="22"/>
     </row>
     <row r="7" spans="1:19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -23924,42 +23887,42 @@
         <v>764</v>
       </c>
       <c r="C7" s="22"/>
-      <c r="D7" s="466"/>
-      <c r="E7" s="467"/>
-      <c r="F7" s="468"/>
+      <c r="D7" s="464"/>
+      <c r="E7" s="465"/>
+      <c r="F7" s="466"/>
       <c r="G7" s="22"/>
-      <c r="H7" s="471"/>
-      <c r="I7" s="472"/>
-      <c r="J7" s="473"/>
+      <c r="H7" s="469"/>
+      <c r="I7" s="470"/>
+      <c r="J7" s="471"/>
       <c r="K7" s="22"/>
-      <c r="L7" s="471"/>
-      <c r="M7" s="472"/>
-      <c r="N7" s="473"/>
+      <c r="L7" s="469"/>
+      <c r="M7" s="470"/>
+      <c r="N7" s="471"/>
       <c r="O7" s="22"/>
-      <c r="P7" s="466"/>
-      <c r="Q7" s="467"/>
-      <c r="R7" s="468"/>
+      <c r="P7" s="464"/>
+      <c r="Q7" s="465"/>
+      <c r="R7" s="466"/>
       <c r="S7" s="22"/>
     </row>
     <row r="8" spans="1:19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="22"/>
-      <c r="D8" s="466"/>
-      <c r="E8" s="467"/>
-      <c r="F8" s="468"/>
+      <c r="D8" s="464"/>
+      <c r="E8" s="465"/>
+      <c r="F8" s="466"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="471"/>
-      <c r="I8" s="472"/>
-      <c r="J8" s="473"/>
+      <c r="H8" s="469"/>
+      <c r="I8" s="470"/>
+      <c r="J8" s="471"/>
       <c r="K8" s="22"/>
-      <c r="L8" s="471"/>
-      <c r="M8" s="472"/>
-      <c r="N8" s="473"/>
+      <c r="L8" s="469"/>
+      <c r="M8" s="470"/>
+      <c r="N8" s="471"/>
       <c r="O8" s="22"/>
-      <c r="P8" s="466"/>
-      <c r="Q8" s="467"/>
-      <c r="R8" s="468"/>
+      <c r="P8" s="464"/>
+      <c r="Q8" s="465"/>
+      <c r="R8" s="466"/>
       <c r="S8" s="22"/>
     </row>
     <row r="9" spans="1:19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -24240,17 +24203,17 @@
       <c r="B22" s="7"/>
       <c r="C22" s="275"/>
       <c r="D22" s="279"/>
-      <c r="E22" s="462" t="s">
+      <c r="E22" s="460" t="s">
         <v>765</v>
       </c>
-      <c r="F22" s="463"/>
-      <c r="G22" s="463"/>
-      <c r="H22" s="463"/>
-      <c r="I22" s="463" t="s">
+      <c r="F22" s="461"/>
+      <c r="G22" s="461"/>
+      <c r="H22" s="461"/>
+      <c r="I22" s="461" t="s">
         <v>1101</v>
       </c>
-      <c r="J22" s="463"/>
-      <c r="K22" s="464"/>
+      <c r="J22" s="461"/>
+      <c r="K22" s="462"/>
       <c r="L22" s="275"/>
       <c r="M22" s="275"/>
       <c r="N22" s="275"/>
@@ -24701,14 +24664,14 @@
       <c r="B40" s="7"/>
       <c r="C40" s="275"/>
       <c r="D40" s="279"/>
-      <c r="E40" s="465" t="s">
+      <c r="E40" s="463" t="s">
         <v>1101</v>
       </c>
-      <c r="F40" s="465"/>
-      <c r="G40" s="465"/>
-      <c r="H40" s="465"/>
-      <c r="I40" s="465"/>
-      <c r="J40" s="465"/>
+      <c r="F40" s="463"/>
+      <c r="G40" s="463"/>
+      <c r="H40" s="463"/>
+      <c r="I40" s="463"/>
+      <c r="J40" s="463"/>
       <c r="Q40" s="275"/>
       <c r="R40" s="280"/>
       <c r="S40" s="275"/>
@@ -24948,16 +24911,12 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F911F448-5EAB-1F4B-8570-DBE686D65A04}">
-  <sheetPr>
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="14" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -24967,7 +24926,7 @@
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="417" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="416" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" style="295" customWidth="1"/>
     <col min="7" max="9" width="11.83203125" style="294" customWidth="1"/>
     <col min="10" max="11" width="11.83203125" style="72" customWidth="1"/>
@@ -25011,7 +24970,7 @@
     </row>
     <row r="3" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="63"/>
-      <c r="E3" s="431" t="s">
+      <c r="E3" s="430" t="s">
         <v>892</v>
       </c>
       <c r="F3" s="147" t="s">
@@ -25367,16 +25326,12 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D6209B-A31F-0140-BC0B-6F9EBD3DCD27}">
-  <sheetPr>
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
   <dimension ref="A1:BV63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="14" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="topRight" activeCell="X15" sqref="A15:XFD15"/>
-      <selection pane="bottomLeft" activeCell="X15" sqref="A15:XFD15"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -25538,10 +25493,10 @@
       <c r="BV1" s="67"/>
     </row>
     <row r="2" spans="1:74" s="56" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="479" t="s">
+      <c r="A2" s="477" t="s">
         <v>1179</v>
       </c>
-      <c r="B2" s="476"/>
+      <c r="B2" s="474"/>
       <c r="C2" s="111" t="s">
         <v>720</v>
       </c>
@@ -25656,8 +25611,8 @@
       <c r="BV2" s="68"/>
     </row>
     <row r="3" spans="1:74" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477"/>
-      <c r="B3" s="478"/>
+      <c r="A3" s="475"/>
+      <c r="B3" s="476"/>
       <c r="C3" s="255" t="s">
         <v>861</v>
       </c>
@@ -25667,7 +25622,7 @@
       <c r="E3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="F3" s="437" t="s">
+      <c r="F3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="G3" s="409" t="s">
@@ -25691,7 +25646,7 @@
       <c r="M3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="N3" s="437" t="s">
+      <c r="N3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="O3" s="409" t="s">
@@ -25712,7 +25667,7 @@
       <c r="T3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="U3" s="437" t="s">
+      <c r="U3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="V3" s="409" t="s">
@@ -25733,7 +25688,7 @@
       <c r="AA3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="AB3" s="437" t="s">
+      <c r="AB3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="AC3" s="409" t="s">
@@ -25754,7 +25709,7 @@
       <c r="AH3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="AI3" s="437" t="s">
+      <c r="AI3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="AJ3" s="409" t="s">
@@ -25775,7 +25730,7 @@
       <c r="AO3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="AP3" s="437" t="s">
+      <c r="AP3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="AQ3" s="409" t="s">
@@ -25796,7 +25751,7 @@
       <c r="AV3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="AW3" s="437" t="s">
+      <c r="AW3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="AX3" s="409" t="s">
@@ -25817,7 +25772,7 @@
       <c r="BC3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="BD3" s="437" t="s">
+      <c r="BD3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="BE3" s="409" t="s">
@@ -25838,7 +25793,7 @@
       <c r="BJ3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="BK3" s="437" t="s">
+      <c r="BK3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="BL3" s="409" t="s">
@@ -25859,7 +25814,7 @@
       <c r="BQ3" s="265" t="s">
         <v>862</v>
       </c>
-      <c r="BR3" s="437" t="s">
+      <c r="BR3" s="436" t="s">
         <v>592</v>
       </c>
       <c r="BS3" s="409" t="s">
@@ -27822,10 +27777,16 @@
     <hyperlink ref="BK3:BO3" location="KP!AL:AL" display="FSW" xr:uid="{4AA32165-9DD7-7B4D-B7ED-C3CDBAA6E700}"/>
     <hyperlink ref="D3" location="PrEP!O:O" display="AGYW, 15+ (FY22)" xr:uid="{D30B5AD7-D583-BD4C-B576-5E7D99AFD2B2}"/>
     <hyperlink ref="L3" location="PrEP!L:L" display="AGYW, 15+ (FY22)" xr:uid="{BF8F5AB6-9824-ED4D-B099-A1CC6AEFCC17}"/>
-    <hyperlink ref="S3" location="Cascade!BF:BF" display="Female, 15+ (FY23)" xr:uid="{37FA98D1-33BD-A444-97A0-A68B9AD4B59C}"/>
-    <hyperlink ref="Z3" location="Cascade!BB:BB" display="Female, 15+ (FY23)" xr:uid="{C166170E-FAD7-8C4B-9B92-D03B73B0F353}"/>
+    <hyperlink ref="S3" location="Cascade!BQ:BQ" display="Female, 15+ (FY23)" xr:uid="{37FA98D1-33BD-A444-97A0-A68B9AD4B59C}"/>
+    <hyperlink ref="Z3" location="Cascade!BN:BN" display="Female, 15+ (FY23)" xr:uid="{C166170E-FAD7-8C4B-9B92-D03B73B0F353}"/>
     <hyperlink ref="AB3" location="KP!V:V" display="FSW" xr:uid="{AE125712-464A-CE49-8AE4-D446A32C3C4E}"/>
     <hyperlink ref="BR3:BV3" location="KP!AN:AN" display="FSW" xr:uid="{1B8C1FEC-5D47-C34B-95DE-D53DDC509080}"/>
+    <hyperlink ref="T3" location="Cascade!BQ:BQ" display="Male, 15+ (FY23)" xr:uid="{F06DCFDA-0A19-634D-97ED-8F6C547DE634}"/>
+    <hyperlink ref="AA3" location="Cascade!BN:BN" display="Male, 15+ (FY23)" xr:uid="{7BD444EF-467E-E94B-9D2F-3DA8EC805AEF}"/>
+    <hyperlink ref="AG3" location="Cascade!AU:AU" display="Female, 15+ (FY23)" xr:uid="{6BC9F814-6722-5248-9E75-12AE0093D6EA}"/>
+    <hyperlink ref="AH3" location="Cascade!AU:AU" display="Male, 15+ (FY23)" xr:uid="{194C7A63-C228-0941-B91F-DE816D723BEE}"/>
+    <hyperlink ref="AN3" location="Cascade!AP:AP" display="Female, 15+ (FY23)" xr:uid="{453F390E-49DF-3343-B441-35D881A719FE}"/>
+    <hyperlink ref="AO3" location="Cascade!AP:AP" display="Male, 15+ (FY23)" xr:uid="{478BF3D1-075E-0145-8D8D-5CFAEE85DAB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -27960,7 +27921,7 @@
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="474" t="s">
+      <c r="B6" s="472" t="s">
         <v>278</v>
       </c>
       <c r="D6" s="8"/>
@@ -27973,7 +27934,7 @@
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="474"/>
+      <c r="B7" s="472"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -28019,7 +27980,7 @@
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B11" s="474" t="s">
+      <c r="B11" s="472" t="s">
         <v>280</v>
       </c>
       <c r="D11" s="8"/>
@@ -28032,7 +27993,7 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B12" s="474"/>
+      <c r="B12" s="472"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -28078,7 +28039,7 @@
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B16" s="474" t="s">
+      <c r="B16" s="472" t="s">
         <v>282</v>
       </c>
       <c r="D16" s="8"/>
@@ -28091,7 +28052,7 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="474"/>
+      <c r="B17" s="472"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -28113,7 +28074,7 @@
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="474" t="s">
+      <c r="B19" s="472" t="s">
         <v>283</v>
       </c>
       <c r="D19" s="8"/>
@@ -28126,7 +28087,7 @@
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="474"/>
+      <c r="B20" s="472"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -28194,7 +28155,7 @@
       <c r="L25" s="8"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="474" t="s">
+      <c r="B26" s="472" t="s">
         <v>761</v>
       </c>
       <c r="D26" s="8"/>
@@ -28207,7 +28168,7 @@
       <c r="L26" s="8"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="474"/>
+      <c r="B27" s="472"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
@@ -41744,9 +41705,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AC8B68-6747-844D-847F-C4519A511429}">
-  <sheetPr>
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -41760,7 +41718,7 @@
   <cols>
     <col min="1" max="1" width="16.1640625" style="8" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="436" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="435" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" style="189" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
@@ -41770,7 +41728,7 @@
         <v>71</v>
       </c>
       <c r="B1" s="184"/>
-      <c r="C1" s="432" t="s">
+      <c r="C1" s="431" t="s">
         <v>71</v>
       </c>
       <c r="D1" s="185"/>
@@ -41779,7 +41737,7 @@
     <row r="2" spans="1:5" s="186" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
-      <c r="C2" s="433" t="s">
+      <c r="C2" s="432" t="s">
         <v>74</v>
       </c>
       <c r="D2" s="153" t="s">
@@ -41805,7 +41763,7 @@
       <c r="B4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="434"/>
+      <c r="C4" s="433"/>
       <c r="D4" s="191"/>
       <c r="E4" s="188" t="str">
         <f>IF(COUNTIF(D$15:INDEX($D:$D,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)),"")&gt;0,"BLANK PRIORITIZATIONS","")</f>
@@ -41819,7 +41777,7 @@
       <c r="B5" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="434" t="s">
+      <c r="C5" s="433" t="s">
         <v>107</v>
       </c>
       <c r="D5" s="191" t="s">
@@ -41836,7 +41794,7 @@
       <c r="B6" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="434" t="s">
+      <c r="C6" s="433" t="s">
         <v>111</v>
       </c>
       <c r="D6" s="191" t="s">
@@ -41853,7 +41811,7 @@
       <c r="B7" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="434" t="s">
+      <c r="C7" s="433" t="s">
         <v>95</v>
       </c>
       <c r="D7" s="191" t="s">
@@ -41864,7 +41822,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C8" s="435" t="s">
+      <c r="C8" s="434" t="s">
         <v>106</v>
       </c>
       <c r="D8" s="323" t="s">
@@ -41872,23 +41830,23 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="435"/>
+      <c r="C9" s="434"/>
       <c r="D9" s="323"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" s="435"/>
+      <c r="C10" s="434"/>
       <c r="D10" s="323"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" s="434"/>
+      <c r="C11" s="433"/>
       <c r="D11" s="191"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C12" s="434"/>
+      <c r="C12" s="433"/>
       <c r="D12" s="191"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C13" s="434"/>
+      <c r="C13" s="433"/>
       <c r="D13" s="191"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -41954,12 +41912,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DDBC09-F535-654B-A49D-7D22E3100EEA}">
-  <sheetPr codeName="Sheet13">
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:DC15"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -41973,15 +41929,15 @@
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" customWidth="1"/>
     <col min="5" max="5" width="39" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="416" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="415" customWidth="1"/>
     <col min="7" max="7" width="12" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" customWidth="1"/>
     <col min="9" max="9" width="11.83203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" customWidth="1"/>
     <col min="11" max="11" width="11.83203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" style="456" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" style="454" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" style="456" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="454" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="11.83203125" customWidth="1"/>
     <col min="17" max="17" width="11.83203125" hidden="1" customWidth="1"/>
@@ -41993,38 +41949,38 @@
     <col min="23" max="23" width="11.83203125" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="11.83203125" customWidth="1"/>
     <col min="25" max="25" width="11.83203125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="11.83203125" style="416" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" style="415" customWidth="1"/>
     <col min="27" max="30" width="11.83203125" customWidth="1"/>
-    <col min="31" max="31" width="11.83203125" style="416" customWidth="1"/>
+    <col min="31" max="31" width="11.83203125" style="415" customWidth="1"/>
     <col min="32" max="35" width="11.83203125" customWidth="1"/>
-    <col min="36" max="36" width="11.83203125" style="416" customWidth="1"/>
-    <col min="37" max="38" width="11.83203125" style="438" customWidth="1"/>
-    <col min="39" max="39" width="11.83203125" style="439" customWidth="1"/>
-    <col min="40" max="40" width="11.83203125" style="438" customWidth="1"/>
-    <col min="41" max="41" width="11.83203125" style="447" customWidth="1"/>
-    <col min="42" max="42" width="11.83203125" style="438" customWidth="1"/>
-    <col min="43" max="43" width="11.83203125" style="416" customWidth="1"/>
-    <col min="44" max="47" width="11.83203125" style="438" customWidth="1"/>
-    <col min="48" max="48" width="11.83203125" style="416" customWidth="1"/>
+    <col min="36" max="36" width="11.83203125" style="415" customWidth="1"/>
+    <col min="37" max="38" width="11.83203125" style="437" customWidth="1"/>
+    <col min="39" max="39" width="11.83203125" style="438" customWidth="1"/>
+    <col min="40" max="40" width="11.83203125" style="437" customWidth="1"/>
+    <col min="41" max="41" width="11.83203125" style="445" customWidth="1"/>
+    <col min="42" max="42" width="11.83203125" style="437" customWidth="1"/>
+    <col min="43" max="43" width="11.83203125" style="415" customWidth="1"/>
+    <col min="44" max="47" width="11.83203125" style="437" customWidth="1"/>
+    <col min="48" max="48" width="11.83203125" style="415" customWidth="1"/>
     <col min="49" max="49" width="11.83203125" customWidth="1"/>
-    <col min="50" max="51" width="11.83203125" style="438" customWidth="1"/>
+    <col min="50" max="51" width="11.83203125" style="437" customWidth="1"/>
     <col min="52" max="52" width="11.83203125" customWidth="1"/>
-    <col min="53" max="59" width="11.83203125" style="438" customWidth="1"/>
+    <col min="53" max="59" width="11.83203125" style="437" customWidth="1"/>
     <col min="60" max="61" width="11.83203125" customWidth="1"/>
-    <col min="62" max="64" width="11.83203125" style="438" customWidth="1"/>
-    <col min="65" max="65" width="11.83203125" style="416" customWidth="1"/>
-    <col min="66" max="66" width="11.83203125" style="438" customWidth="1"/>
-    <col min="67" max="67" width="11.83203125" style="416" customWidth="1"/>
-    <col min="68" max="69" width="11.83203125" style="438" customWidth="1"/>
-    <col min="70" max="70" width="11.83203125" style="416" customWidth="1"/>
-    <col min="71" max="72" width="11.83203125" style="438" customWidth="1"/>
-    <col min="73" max="73" width="11.83203125" style="416" customWidth="1"/>
+    <col min="62" max="64" width="11.83203125" style="437" customWidth="1"/>
+    <col min="65" max="65" width="11.83203125" style="415" customWidth="1"/>
+    <col min="66" max="66" width="11.83203125" style="437" customWidth="1"/>
+    <col min="67" max="67" width="11.83203125" style="415" customWidth="1"/>
+    <col min="68" max="69" width="11.83203125" style="437" customWidth="1"/>
+    <col min="70" max="70" width="11.83203125" style="415" customWidth="1"/>
+    <col min="71" max="72" width="11.83203125" style="437" customWidth="1"/>
+    <col min="73" max="73" width="11.83203125" style="415" customWidth="1"/>
     <col min="74" max="85" width="11.83203125" customWidth="1"/>
-    <col min="86" max="86" width="11.83203125" style="416" customWidth="1"/>
+    <col min="86" max="86" width="11.83203125" style="415" customWidth="1"/>
     <col min="87" max="92" width="11.83203125" customWidth="1"/>
-    <col min="93" max="93" width="11.83203125" style="416" customWidth="1"/>
+    <col min="93" max="93" width="11.83203125" style="415" customWidth="1"/>
     <col min="94" max="100" width="11.83203125" customWidth="1"/>
-    <col min="101" max="101" width="11.83203125" style="416" customWidth="1"/>
+    <col min="101" max="101" width="11.83203125" style="415" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:107" s="57" customFormat="1" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -42043,7 +41999,7 @@
       <c r="I1" s="35"/>
       <c r="J1" s="85"/>
       <c r="K1" s="35"/>
-      <c r="L1" s="421"/>
+      <c r="L1" s="420"/>
       <c r="M1" s="35"/>
       <c r="N1" s="80"/>
       <c r="O1" s="35"/>
@@ -42078,7 +42034,7 @@
       <c r="AL1" s="360"/>
       <c r="AM1" s="357"/>
       <c r="AN1" s="96"/>
-      <c r="AO1" s="440" t="s">
+      <c r="AO1" s="439" t="s">
         <v>51</v>
       </c>
       <c r="AP1" s="96"/>
@@ -42117,7 +42073,7 @@
       </c>
       <c r="BP1" s="360"/>
       <c r="BQ1" s="96"/>
-      <c r="BR1" s="440" t="s">
+      <c r="BR1" s="439" t="s">
         <v>767</v>
       </c>
       <c r="BS1" s="244"/>
@@ -42161,14 +42117,14 @@
       </c>
     </row>
     <row r="2" spans="1:107" s="56" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="475" t="s">
+      <c r="A2" s="473" t="s">
         <v>1145</v>
       </c>
-      <c r="B2" s="476"/>
+      <c r="B2" s="474"/>
       <c r="C2" s="2"/>
       <c r="D2" s="298"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="459" t="s">
+      <c r="F2" s="457" t="s">
         <v>74</v>
       </c>
       <c r="G2" s="34"/>
@@ -42213,7 +42169,7 @@
       <c r="AN2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="AO2" s="444" t="s">
+      <c r="AO2" s="443" t="s">
         <v>3</v>
       </c>
       <c r="AP2" s="102"/>
@@ -42262,7 +42218,7 @@
       <c r="BQ2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="444" t="s">
+      <c r="BR2" s="443" t="s">
         <v>3</v>
       </c>
       <c r="BS2" s="245"/>
@@ -42307,17 +42263,17 @@
       <c r="CV2" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="CW2" s="449" t="s">
+      <c r="CW2" s="447" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:107" s="40" customFormat="1" ht="134" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477"/>
-      <c r="B3" s="478"/>
+      <c r="A3" s="475"/>
+      <c r="B3" s="476"/>
       <c r="C3" s="47"/>
       <c r="D3" s="299"/>
       <c r="E3" s="47"/>
-      <c r="F3" s="460" t="s">
+      <c r="F3" s="458" t="s">
         <v>1126</v>
       </c>
       <c r="G3" s="348" t="s">
@@ -42335,13 +42291,13 @@
       <c r="K3" s="348" t="s">
         <v>970</v>
       </c>
-      <c r="L3" s="457" t="s">
+      <c r="L3" s="455" t="s">
         <v>1142</v>
       </c>
       <c r="M3" s="348" t="s">
         <v>1141</v>
       </c>
-      <c r="N3" s="454" t="s">
+      <c r="N3" s="452" t="s">
         <v>1129</v>
       </c>
       <c r="O3" s="348" t="s">
@@ -42422,7 +42378,7 @@
       <c r="AN3" s="296" t="s">
         <v>1187</v>
       </c>
-      <c r="AO3" s="445" t="s">
+      <c r="AO3" s="255" t="s">
         <v>977</v>
       </c>
       <c r="AP3" s="296" t="s">
@@ -42509,7 +42465,7 @@
       <c r="BQ3" s="296" t="s">
         <v>789</v>
       </c>
-      <c r="BR3" s="448" t="s">
+      <c r="BR3" s="446" t="s">
         <v>962</v>
       </c>
       <c r="BS3" s="358" t="s">
@@ -42602,7 +42558,7 @@
       <c r="CV3" s="373" t="s">
         <v>945</v>
       </c>
-      <c r="CW3" s="450" t="s">
+      <c r="CW3" s="448" t="s">
         <v>1135</v>
       </c>
       <c r="CX3"/>
@@ -42730,7 +42686,7 @@
         <f>SUBTOTAL(109,AN$15:INDEX(AN:AN,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="AO4" s="441">
+      <c r="AO4" s="440">
         <f>SUBTOTAL(109,AO$15:INDEX(AO:AO,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
@@ -42840,7 +42796,7 @@
         <f>SUBTOTAL(109,BQ$15:INDEX(BQ:BQ,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="BR4" s="441">
+      <c r="BR4" s="440">
         <f>SUBTOTAL(109,BR$15:INDEX(BR:BR,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
@@ -42961,7 +42917,7 @@
         <f>IF(SUM($BZ4)=0,"",SUM($CR4,$CT4)/$BZ4)</f>
         <v/>
       </c>
-      <c r="CW4" s="451">
+      <c r="CW4" s="449">
         <f>SUBTOTAL(109,CW$15:INDEX(CW:CW,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
@@ -43273,7 +43229,7 @@
       <c r="CV5" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="CW5" s="452" t="s">
+      <c r="CW5" s="450" t="s">
         <v>108</v>
       </c>
       <c r="CX5"/>
@@ -43584,7 +43540,7 @@
       <c r="CV6" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="CW6" s="452" t="s">
+      <c r="CW6" s="450" t="s">
         <v>93</v>
       </c>
       <c r="CX6"/>
@@ -43895,7 +43851,7 @@
       <c r="CV7" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="CW7" s="452" t="s">
+      <c r="CW7" s="450" t="s">
         <v>95</v>
       </c>
       <c r="CX7"/>
@@ -43911,7 +43867,7 @@
       <c r="C8" s="329"/>
       <c r="D8" s="386"/>
       <c r="E8" s="329"/>
-      <c r="F8" s="442" t="s">
+      <c r="F8" s="441" t="s">
         <v>97</v>
       </c>
       <c r="G8" s="332"/>
@@ -43923,7 +43879,7 @@
         <v>98</v>
       </c>
       <c r="K8" s="332"/>
-      <c r="L8" s="423"/>
+      <c r="L8" s="422"/>
       <c r="M8" s="332"/>
       <c r="N8" s="214"/>
       <c r="O8" s="332"/>
@@ -43978,7 +43934,7 @@
       <c r="AN8" s="395" t="s">
         <v>101</v>
       </c>
-      <c r="AO8" s="442"/>
+      <c r="AO8" s="441"/>
       <c r="AP8" s="395" t="s">
         <v>793</v>
       </c>
@@ -44015,7 +43971,7 @@
       <c r="BQ8" s="395" t="s">
         <v>136</v>
       </c>
-      <c r="BR8" s="442" t="s">
+      <c r="BR8" s="441" t="s">
         <v>295</v>
       </c>
       <c r="BS8" s="392"/>
@@ -44056,7 +44012,7 @@
         <v>147</v>
       </c>
       <c r="CV8" s="332"/>
-      <c r="CW8" s="453"/>
+      <c r="CW8" s="451"/>
       <c r="CX8" s="22"/>
       <c r="CY8" s="22"/>
       <c r="CZ8" s="22"/>
@@ -44070,13 +44026,13 @@
       <c r="C9" s="329"/>
       <c r="D9" s="386"/>
       <c r="E9" s="329"/>
-      <c r="F9" s="442"/>
+      <c r="F9" s="441"/>
       <c r="G9" s="332"/>
       <c r="H9" s="119"/>
       <c r="I9" s="332"/>
       <c r="J9" s="387"/>
       <c r="K9" s="332"/>
-      <c r="L9" s="423"/>
+      <c r="L9" s="422"/>
       <c r="M9" s="332"/>
       <c r="N9" s="214"/>
       <c r="O9" s="332"/>
@@ -44121,7 +44077,7 @@
       <c r="AL9" s="389"/>
       <c r="AM9" s="393"/>
       <c r="AN9" s="395"/>
-      <c r="AO9" s="442"/>
+      <c r="AO9" s="441"/>
       <c r="AP9" s="395" t="s">
         <v>794</v>
       </c>
@@ -44158,7 +44114,7 @@
       <c r="BQ9" s="395" t="s">
         <v>137</v>
       </c>
-      <c r="BR9" s="442"/>
+      <c r="BR9" s="441"/>
       <c r="BS9" s="392"/>
       <c r="BT9" s="394"/>
       <c r="BU9" s="331"/>
@@ -44197,7 +44153,7 @@
         <v>148</v>
       </c>
       <c r="CV9" s="396"/>
-      <c r="CW9" s="453"/>
+      <c r="CW9" s="451"/>
       <c r="CX9" s="22"/>
       <c r="CY9" s="22"/>
       <c r="CZ9" s="22"/>
@@ -44211,7 +44167,7 @@
       <c r="C10" s="329"/>
       <c r="D10" s="386"/>
       <c r="E10" s="329"/>
-      <c r="F10" s="442"/>
+      <c r="F10" s="441"/>
       <c r="G10" s="332"/>
       <c r="H10" s="119" t="s">
         <v>105</v>
@@ -44219,7 +44175,7 @@
       <c r="I10" s="332"/>
       <c r="J10" s="387"/>
       <c r="K10" s="332"/>
-      <c r="L10" s="423"/>
+      <c r="L10" s="422"/>
       <c r="M10" s="332"/>
       <c r="N10" s="214"/>
       <c r="O10" s="332"/>
@@ -44274,7 +44230,7 @@
       <c r="AN10" s="395" t="s">
         <v>105</v>
       </c>
-      <c r="AO10" s="442"/>
+      <c r="AO10" s="441"/>
       <c r="AP10" s="395" t="s">
         <v>142</v>
       </c>
@@ -44311,7 +44267,7 @@
       <c r="BQ10" s="395" t="s">
         <v>105</v>
       </c>
-      <c r="BR10" s="442" t="s">
+      <c r="BR10" s="441" t="s">
         <v>105</v>
       </c>
       <c r="BS10" s="392"/>
@@ -44352,7 +44308,7 @@
         <v>104</v>
       </c>
       <c r="CV10" s="332"/>
-      <c r="CW10" s="453"/>
+      <c r="CW10" s="451"/>
       <c r="CX10" s="22"/>
       <c r="CY10" s="22"/>
       <c r="CZ10" s="22"/>
@@ -44651,7 +44607,7 @@
       <c r="CV11" s="36" t="s">
         <v>688</v>
       </c>
-      <c r="CW11" s="452" t="s">
+      <c r="CW11" s="450" t="s">
         <v>203</v>
       </c>
       <c r="CX11"/>
@@ -44952,7 +44908,7 @@
       <c r="CV12" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="CW12" s="452" t="s">
+      <c r="CW12" s="450" t="s">
         <v>202</v>
       </c>
       <c r="CX12"/>
@@ -45063,7 +45019,7 @@
       <c r="CT13" s="72"/>
       <c r="CU13" s="72"/>
       <c r="CV13" s="36"/>
-      <c r="CW13" s="452"/>
+      <c r="CW13" s="450"/>
       <c r="CX13"/>
       <c r="CY13"/>
       <c r="CZ13"/>
@@ -45192,7 +45148,7 @@
       <c r="AN14" s="99" t="s">
         <v>951</v>
       </c>
-      <c r="AO14" s="443" t="s">
+      <c r="AO14" s="442" t="s">
         <v>979</v>
       </c>
       <c r="AP14" s="99" t="s">
@@ -45279,7 +45235,7 @@
       <c r="BQ14" s="99" t="s">
         <v>317</v>
       </c>
-      <c r="BR14" s="443" t="s">
+      <c r="BR14" s="442" t="s">
         <v>963</v>
       </c>
       <c r="BS14" s="249" t="s">
@@ -45385,7 +45341,7 @@
         <f>B15&amp;"|"&amp;C15&amp;"|"&amp;D15</f>
         <v>||</v>
       </c>
-      <c r="F15" s="461" t="str">
+      <c r="F15" s="459" t="str">
         <f>IF(LEFT($B15,4)="_Mil","",_xlfn.IFNA(ROUND(INDEX(Spectrum!$N:$N,MATCH(RIGHT($B15,13)&amp;"|"&amp;$C15&amp;"|"&amp;$D15&amp;"|"&amp;F$14&amp;"|"&amp;"CY2022Q3",Spectrum!$Q:$Q,0)),0),""))</f>
         <v/>
       </c>
@@ -45409,7 +45365,7 @@
         <f>IF(OR($J15="",LEFT($B15,4)="_Mil"),"",_xlfn.IFNA(INDEX(Spectrum!$P:$P,MATCH(RIGHT($B15,13)&amp;"|"&amp;$C15&amp;"|"&amp;$D15&amp;"|"&amp;J$14&amp;"|"&amp;"CY2022Q3",Spectrum!$Q:$Q,0)),""))</f>
         <v/>
       </c>
-      <c r="L15" s="458" t="str">
+      <c r="L15" s="456" t="str">
         <f>IF(LEFT($B15,4)="_Mil","",_xlfn.IFNA(INDEX(Spectrum!$N:$N,MATCH(RIGHT($B15,13)&amp;"|"&amp;$C15&amp;"|"&amp;$D15&amp;"|"&amp;L$14&amp;"|"&amp;"CY2022Q3",Spectrum!$Q:$Q,0)),""))</f>
         <v/>
       </c>
@@ -45417,7 +45373,7 @@
         <f>IF(OR($J15="",LEFT($B15,4)="_Mil"),"",_xlfn.IFNA(INDEX(Spectrum!$P:$P,MATCH(RIGHT($B15,13)&amp;"|"&amp;$C15&amp;"|"&amp;$D15&amp;"|"&amp;L$14&amp;"|"&amp;"CY2022Q3",Spectrum!$Q:$Q,0)),""))</f>
         <v/>
       </c>
-      <c r="N15" s="455" t="str">
+      <c r="N15" s="453" t="str">
         <f>IF(LEFT($B15,4)="_Mil","",_xlfn.IFNA(ROUND(INDEX(Spectrum!$N:$N,MATCH(RIGHT($B15,13)&amp;"|"&amp;$C15&amp;"|"&amp;$D15&amp;"|"&amp;N$14&amp;"|"&amp;"CY2022Q3",Spectrum!$Q:$Q,0)),0),""))</f>
         <v/>
       </c>
@@ -45495,12 +45451,12 @@
         <f>IF(LEFT($B15,4)="_Mil","",ROUND($AM15*SUM($H15,$N15),0))</f>
         <v>0</v>
       </c>
-      <c r="AO15" s="446" t="str">
-        <f>IF($C15="&lt;01",IFERROR(ROUND(INDEX(EID!$V:$V,MATCH($B15,EID!$B:$B,0))/2,0),""),"")</f>
+      <c r="AO15" s="444" t="str">
+        <f>IF($C15="&lt;01",ROUND(INDEX(EID!$V:$V,MATCH($B15,EID!$B:$B,0))/2,0),"")</f>
         <v/>
       </c>
       <c r="AP15" s="219" t="str">
-        <f>IF(LEFT($B15,4)="_Mil",HYPERLINK("","Paste _Mil Targets Here"),IF($C15="&lt;01",HYPERLINK("",$AO15),IFERROR(HYPERLINK("",ROUND(SUM($AN15)*AK15,0)),HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add PEPFAR Contribution %"))))</f>
+        <f>IF($C15="&lt;01",HYPERLINK("",$AO15),IF(LEFT($B15,4)="_Mil",HYPERLINK("","Paste _Mil Targets Here"),IFERROR(HYPERLINK("",ROUND($AN15*AK15,0)),HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add PEPFAR Contribution %"))))</f>
         <v>&lt;- Add PEPFAR Contribution %</v>
       </c>
       <c r="AQ15" s="161" t="str">
@@ -45560,7 +45516,7 @@
         <v>0.7</v>
       </c>
       <c r="BE15" s="248" t="str">
-        <f>IF(OR(LEFT($B15,4)="_Mil",$C15="&lt;01"),"",IFERROR(SUM($V15)/IF(SUM($T15)=0,SUM($R15),$T15),""))</f>
+        <f>IF(OR(LEFT($B15,4)="_Mil",$C15="&lt;01"),"",IFERROR($V15/IF(SUM($T15)=0,$R15,$T15),""))</f>
         <v/>
       </c>
       <c r="BF15" s="356" t="str">
@@ -45572,7 +45528,7 @@
         <v>1</v>
       </c>
       <c r="BH15" s="217" t="str">
-        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$N:$N,MATCH($B15,EID!$B:$B,0)),0),0)),IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW(AK15),"&lt;- Add PEPFAR Contribution %"),IF($AZ15="",HYPERLINK("#Cascade!AZ"&amp;ROW(AZ15),"&lt;- Add % New Infections Diagnosed &amp; Linked"),IF($BC15="",HYPERLINK("#Cascade!BC"&amp;ROW(BC15),"&lt;- Add Linkage"),HYPERLINK("",ROUND(SUM($N15)*$AK15*$AZ15*$BC15,0))))))</f>
+        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$N:$N,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(AND($AK15="",LEFT($B15,4)&lt;&gt;"_Mil"),HYPERLINK("#Cascade!AK"&amp;ROW(AK15),"&lt;- Add PEPFAR Contribution %"),IF($AZ15="",HYPERLINK("#Cascade!AZ"&amp;ROW(AZ15),"&lt;- Add % New Infections Diagnosed &amp; Linked"),IF($BC15="",HYPERLINK("#Cascade!BC"&amp;ROW(BC15),"&lt;- Add Linkage"),HYPERLINK("",ROUND(SUM($N15)*IF(LEFT($B15,4)="_Mil",1,$AK15)*$AZ15*$BC15,0))))))</f>
         <v>&lt;- Add PEPFAR Contribution %</v>
       </c>
       <c r="BI15" s="217">
@@ -45580,7 +45536,7 @@
         <v>0</v>
       </c>
       <c r="BJ15" s="219">
-        <f>IF(AND(LEFT($B15,4)="_Mil",SUM($AP15)=0),"",SUM($BH15,$BI15))</f>
+        <f>SUM($BH15,$BI15)</f>
         <v>0</v>
       </c>
       <c r="BK15" s="219">
@@ -45611,7 +45567,7 @@
         <f>IF(AND(LEFT($B15,4)="_Mil",SUM($AP15)=0),"",ROUND(IF($C15="&lt;01",IFERROR(INDEX(EID!P:$P,MATCH($B15,EID!$B:$B,0))/2,0),SUM($AG15)*SUM($BP15)+SUM($BJ15)*SUM($BO15)),0))</f>
         <v>0</v>
       </c>
-      <c r="BR15" s="446" t="str">
+      <c r="BR15" s="444" t="str">
         <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add PEPFAR Contribution %"),HYPERLINK("",ROUND($BQ15/$AK15,0))))</f>
         <v>&lt;- Add PEPFAR Contribution %</v>
       </c>
@@ -45669,7 +45625,7 @@
         <v/>
       </c>
       <c r="CG15" s="105" t="str">
-        <f>IF(SUM($BZ15)=0,"",$BZ15-SUM($CA15:$CF15))</f>
+        <f>IF(SUM($BZ15)=0,"",IFERROR(1/(1/($BZ15-SUM($CA15:$CF15))),""))</f>
         <v/>
       </c>
       <c r="CH15" s="163" t="str">
@@ -45723,8 +45679,8 @@
         <f>IF(OR(SUM($BZ15)=0,$C15="&lt;01"),"",SUM($CR15,$CT15)/$BZ15)</f>
         <v/>
       </c>
-      <c r="CW15" s="452" t="str" cm="1">
-        <f t="array" ref="CW15">IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add % PEPFAR Contribution"),HYPERLINK("",UM($P15,$BZ15/$AK15))))</f>
+      <c r="CW15" s="450" t="str">
+        <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add % PEPFAR Contribution"),HYPERLINK("",IF($C15="&lt;01",0,SUM($P15))+SUM($BZ15)/$AK15)))</f>
         <v>&lt;- Add % PEPFAR Contribution</v>
       </c>
       <c r="CX15"/>
@@ -45859,14 +45815,14 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="CA3" location="Cascade!CI:CK" display="Cascade!CI:CK" xr:uid="{CFC22E83-CD81-744A-BD97-81BDFE5732F2}"/>
+    <hyperlink ref="CA3" location="Cascade!CR:CU" display="Cascade!CR:CU" xr:uid="{CFC22E83-CD81-744A-BD97-81BDFE5732F2}"/>
     <hyperlink ref="CB3" location="PMTCT!AF:AF" display="PMTCT_STAT New Positives (FY23)" xr:uid="{072C5291-7010-704F-BBB9-7097DE99B670}"/>
     <hyperlink ref="CC3" location="PMTCT!AV:AV" display="HTS_TST Post ANC1 New Positives (FY23)" xr:uid="{BD5510F0-19E5-3C41-B8F3-9039D1D2730F}"/>
     <hyperlink ref="CD3" location="TB!Q:Q" display="TB_STAT New Positives (FY22)" xr:uid="{4946A338-D073-E84B-90AE-459B22CC722F}"/>
     <hyperlink ref="CE3" location="VMMC!AC:AC" display="VMMC Tested Positives (FY22)" xr:uid="{9324AD3D-0667-6B41-8A55-485E12745DBA}"/>
-    <hyperlink ref="CF3" location="EID!Q:Q" display="EID!Q:Q" xr:uid="{DD5860B7-2BBA-D54C-AC3A-9FA1A8C82695}"/>
+    <hyperlink ref="CF3" location="EID!L:L" display="EID!L:L" xr:uid="{DD5860B7-2BBA-D54C-AC3A-9FA1A8C82695}"/>
     <hyperlink ref="CG3" location="HTS!O:O" display="HTS_TST_POS from All Other Modalities (FY23)" xr:uid="{94117302-B331-2E49-A0BD-18496ED310FB}"/>
-    <hyperlink ref="AO3" location="EID!U:U" display="PMTCT_HEI_POS Virally Suppressed (FY23)" xr:uid="{72DBFF04-97B7-3548-95A9-48E392DE0703}"/>
+    <hyperlink ref="AO3" location="EID!V:V" display="PMTCT_HEI_POS Virally Suppressed (FY23)" xr:uid="{72DBFF04-97B7-3548-95A9-48E392DE0703}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -46007,10 +45963,10 @@
       <c r="BE1" s="244"/>
     </row>
     <row r="2" spans="1:57" s="56" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="479" t="s">
+      <c r="A2" s="477" t="s">
         <v>797</v>
       </c>
-      <c r="B2" s="476"/>
+      <c r="B2" s="474"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="94" t="s">
@@ -46099,8 +46055,8 @@
       <c r="BE2" s="245"/>
     </row>
     <row r="3" spans="1:57" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477"/>
-      <c r="B3" s="478"/>
+      <c r="A3" s="475"/>
+      <c r="B3" s="476"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
       <c r="F3" s="256" t="s">
@@ -47960,21 +47916,21 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="AV3" location="Cascade!CK:CK" display="Positive (FY23)" xr:uid="{9AC7778E-2E88-7242-BE1A-0032FDF1AA0A}"/>
+    <hyperlink ref="AV3" location="Cascade!CC:CC" display="Positive (FY23)" xr:uid="{9AC7778E-2E88-7242-BE1A-0032FDF1AA0A}"/>
     <hyperlink ref="AY3" location="EID!C:C" display="Total PMTCT: Positives (From ANC1 &amp; Post ANC1) (FY23)" xr:uid="{06033567-B162-B642-952B-86F608E51389}"/>
     <hyperlink ref="F3" location="Cascade!F:F" display="Host Country Est. Female Population (FY21)" xr:uid="{9DCC4747-78E8-574F-8A0A-74D7310ECF73}"/>
     <hyperlink ref="G3" location="Cascade!H:H" display="Host Country Est. PLHIV (FY21)" xr:uid="{38AE695F-2465-C345-B2DE-60A49EB9D43A}"/>
     <hyperlink ref="H3" location="Cascade!J:J" display="Host Country Est. HIV Prevalence (FY21) (%)" xr:uid="{5FF09F6B-1BA6-A247-A7AB-EF4027EBC38D}"/>
     <hyperlink ref="I3" location="Cascade!T:T" display="Host Country Est. TX_CURR_SUBNAT (FY22)" xr:uid="{AE293FF8-6531-8E47-9771-94756A48F05D}"/>
-    <hyperlink ref="J3" location="Cascade!AS:AS" display="Host Country Est. ART Coverage (FY22) (%)" xr:uid="{62172621-78AD-F245-A486-21A9FED7A825}"/>
-    <hyperlink ref="AZ3" location="Cascade!CH:CH" display="Total HTS_TST_POS (FY23)" xr:uid="{EF1CACDE-E83E-BC49-803E-79E8D75E671B}"/>
+    <hyperlink ref="J3" location="Cascade!BS:BS" display="Host Country Est. ART Coverage (FY22) (%)" xr:uid="{62172621-78AD-F245-A486-21A9FED7A825}"/>
+    <hyperlink ref="AZ3" location="Cascade!BZ:BZ" display="Total HTS_TST_POS (FY23)" xr:uid="{EF1CACDE-E83E-BC49-803E-79E8D75E671B}"/>
     <hyperlink ref="BA3" location="PMTCT!AF:AF" display="Total Positives from PMTCT_STAT ANC1 (FY23) (%)" xr:uid="{237D0CFB-FBAB-3A42-9524-0309C16E980E}"/>
     <hyperlink ref="BB3" location="PMTCT!AV:AV" display="Total Positives from PMTCT Post ANC1 (FY23) (%)" xr:uid="{D680F786-FE9E-564F-8330-479022D7C4BA}"/>
-    <hyperlink ref="BC3" location="Cascade!CI:CI" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{A440D5C0-3246-D64E-9D9A-125BFE1073A1}"/>
-    <hyperlink ref="BD3" location="Cascade!CL:CL" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{37B73FCD-3AA1-4546-B221-83E509C72600}"/>
-    <hyperlink ref="BE3" location="Cascade!CO:CO" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{EA06E773-2DB3-0B4D-BA39-4517BD65D120}"/>
-    <hyperlink ref="K3" location="Cascade!BO:BO" display="Host Country Est. PopVLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{117CCFAC-2256-F346-BBFA-6D9C183041C6}"/>
-    <hyperlink ref="AF3" location="Cascade!CJ:CJ" display="Newly Tested, Positive (FY23)" xr:uid="{ABC0F45D-6FF3-E94C-B20E-66540AE6F2E1}"/>
+    <hyperlink ref="BC3" location="Cascade!CH:CH" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{A440D5C0-3246-D64E-9D9A-125BFE1073A1}"/>
+    <hyperlink ref="BD3" location="Cascade!CK:CK" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{37B73FCD-3AA1-4546-B221-83E509C72600}"/>
+    <hyperlink ref="BE3" location="Cascade!CN:CN" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{EA06E773-2DB3-0B4D-BA39-4517BD65D120}"/>
+    <hyperlink ref="K3" location="Cascade!AL:AL" display="Host Country Est. PopVLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{117CCFAC-2256-F346-BBFA-6D9C183041C6}"/>
+    <hyperlink ref="AF3" location="Cascade!CB:CB" display="Newly Tested, Positive (FY23)" xr:uid="{ABC0F45D-6FF3-E94C-B20E-66540AE6F2E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -47984,16 +47940,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA74C1D-81B4-2043-80AE-5A5C831472EB}">
-  <sheetPr codeName="Sheet10">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="14" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48104,19 +48058,19 @@
       <c r="J3" s="403" t="s">
         <v>931</v>
       </c>
-      <c r="K3" s="414" t="s">
+      <c r="K3" s="413" t="s">
         <v>932</v>
       </c>
-      <c r="L3" s="413" t="s">
+      <c r="L3" s="70" t="s">
         <v>994</v>
       </c>
-      <c r="M3" s="414" t="s">
+      <c r="M3" s="413" t="s">
         <v>842</v>
       </c>
       <c r="N3" s="70" t="s">
         <v>997</v>
       </c>
-      <c r="O3" s="414" t="s">
+      <c r="O3" s="413" t="s">
         <v>993</v>
       </c>
       <c r="P3" s="70" t="s">
@@ -48646,9 +48600,9 @@
     <row r="15" spans="1:22" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="53"/>
       <c r="B15" s="53"/>
-      <c r="C15" s="79" t="str">
-        <f>IFERROR(1/(1/SUMIF(PMTCT!$B:$B,$B15,PMTCT!$AY:$AY)),"")</f>
-        <v/>
+      <c r="C15" s="79">
+        <f>SUMIF(PMTCT!$B:$B,$B15,PMTCT!$AY:$AY)</f>
+        <v>0</v>
       </c>
       <c r="D15" s="36">
         <v>0.95</v>
@@ -48767,11 +48721,12 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N3" location="Cascade!BL:BL" display="HIV+ infants linked to ART (FY23)" xr:uid="{DAA7530A-3E04-1740-9290-973637420098}"/>
+    <hyperlink ref="N3" location="Cascade!BH:BH" display="HIV+ infants linked to ART (FY23)" xr:uid="{DAA7530A-3E04-1740-9290-973637420098}"/>
     <hyperlink ref="C3" location="PMTCT!AY:AY" display="Est. # infants born to HIV-positive women (FY23)" xr:uid="{1452E224-9F1C-1442-AC84-D0C0D1BADDB9}"/>
-    <hyperlink ref="V3" location="Cascade!AU:AU" display="HIV+ infants  Virally Suppressed (FY23)" xr:uid="{B588F469-4EE5-124C-9655-BE4B92E2099B}"/>
-    <hyperlink ref="T3" location="Cascade!AZ:BA" display="HIV+ infants tested for VLS (FY23)" xr:uid="{204B8930-346A-BF40-BF29-A050F7DAD2C2}"/>
-    <hyperlink ref="P3" location="Cascade!BE:BE" display="HIV+ infants retained on ART at end of FY23" xr:uid="{89871460-7732-6748-8258-655A5F0C2B89}"/>
+    <hyperlink ref="V3" location="Cascade!AP:AP" display="HIV+ infants  Virally Suppressed (FY23)" xr:uid="{B588F469-4EE5-124C-9655-BE4B92E2099B}"/>
+    <hyperlink ref="T3" location="Cascade!AU:AU" display="HIV+ infants tested for VLS (FY23)" xr:uid="{204B8930-346A-BF40-BF29-A050F7DAD2C2}"/>
+    <hyperlink ref="P3" location="Cascade!BQ:BQ" display="HIV+ infants retained on ART at end of FY23" xr:uid="{89871460-7732-6748-8258-655A5F0C2B89}"/>
+    <hyperlink ref="L3" location="Cascade!CF:CF" display="Total HIV+ infants identified (FY23)" xr:uid="{29465258-72C7-F34F-B99E-5CC67BF8776B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -48781,16 +48736,14 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085771F4-2CA4-C146-8002-F8A9EABADF75}">
-  <sheetPr codeName="Sheet11">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48855,10 +48808,10 @@
       <c r="AB1" s="35"/>
     </row>
     <row r="2" spans="1:28" s="56" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="479" t="s">
+      <c r="A2" s="477" t="s">
         <v>812</v>
       </c>
-      <c r="B2" s="476"/>
+      <c r="B2" s="474"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -48905,8 +48858,8 @@
       <c r="AB2" s="34"/>
     </row>
     <row r="3" spans="1:28" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477"/>
-      <c r="B3" s="478"/>
+      <c r="A3" s="475"/>
+      <c r="B3" s="476"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
@@ -49788,14 +49741,14 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="Q3" location="Cascade!BS:BS" display="Newly Tested, Positive" xr:uid="{F41C5CBD-C2B6-7349-92F3-4B3EE0741D63}"/>
-    <hyperlink ref="V3" location="Cascade!BO:BO" display="Total HTS_TST_POS (FY23)" xr:uid="{0C12D99A-2693-9E4D-945B-D14B7A252AA9}"/>
-    <hyperlink ref="W3" location="TB!P:P" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{B168364E-0686-8544-BA70-DF499D18A47C}"/>
-    <hyperlink ref="X3" location="Cascade!BW:BW" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{05C499CF-75CA-2A49-859D-540B72651529}"/>
-    <hyperlink ref="Y3" location="Cascade!BX:BX" display="Total Positives from PMTCT_STAT (FY23) (%)" xr:uid="{54774E98-3A3D-4D48-90D1-801481ED11B7}"/>
-    <hyperlink ref="Z3" location="Cascade!BY:BY" display="Total Positives from Post ANC1 (FY23) (%)" xr:uid="{6E885B80-FB4C-E04D-B2FB-104D9CEB3861}"/>
-    <hyperlink ref="AA3" location="Cascade!CA:CA" display="Total Positives from VMMC (FY23) (%)" xr:uid="{C15FB732-6CF1-6C44-B544-07BF476A6F31}"/>
-    <hyperlink ref="AB3" location="Cascade!CC:CC" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{9AC9FE86-7701-D446-947B-8E63FD134235}"/>
+    <hyperlink ref="Q3" location="Cascade!CD:CD" display="Newly Tested, Positive" xr:uid="{F41C5CBD-C2B6-7349-92F3-4B3EE0741D63}"/>
+    <hyperlink ref="V3" location="Cascade!BZ:BZ" display="Total HTS_TST_POS (FY23)" xr:uid="{0C12D99A-2693-9E4D-945B-D14B7A252AA9}"/>
+    <hyperlink ref="W3" location="TB!Q:Q" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{B168364E-0686-8544-BA70-DF499D18A47C}"/>
+    <hyperlink ref="X3" location="Cascade!CH:CH" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{05C499CF-75CA-2A49-859D-540B72651529}"/>
+    <hyperlink ref="Y3" location="Cascade!CI:CI" display="Total Positives from PMTCT_STAT (FY23) (%)" xr:uid="{54774E98-3A3D-4D48-90D1-801481ED11B7}"/>
+    <hyperlink ref="Z3" location="Cascade!CJ:CJ" display="Total Positives from Post ANC1 (FY23) (%)" xr:uid="{6E885B80-FB4C-E04D-B2FB-104D9CEB3861}"/>
+    <hyperlink ref="AA3" location="Cascade!CL:CL" display="Total Positives from VMMC (FY23) (%)" xr:uid="{C15FB732-6CF1-6C44-B544-07BF476A6F31}"/>
+    <hyperlink ref="AB3" location="Cascade!CN:CN" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{9AC9FE86-7701-D446-947B-8E63FD134235}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -49805,16 +49758,14 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40254BD6-96BC-8E43-A17A-C96765FDD558}">
-  <sheetPr codeName="Sheet12">
-    <tabColor rgb="FF63BE7B"/>
-  </sheetPr>
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="14" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:V1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49836,7 +49787,7 @@
     <col min="19" max="19" width="11.83203125" style="75" customWidth="1"/>
     <col min="20" max="26" width="11.83203125" style="208" customWidth="1"/>
     <col min="27" max="30" width="11.83203125" style="72" customWidth="1"/>
-    <col min="31" max="31" width="11.83203125" style="415" customWidth="1"/>
+    <col min="31" max="31" width="11.83203125" style="414" customWidth="1"/>
     <col min="32" max="32" width="11.83203125" style="72" customWidth="1"/>
     <col min="33" max="33" width="11.83203125" style="98" customWidth="1"/>
     <col min="34" max="34" width="11.83203125" style="248" customWidth="1"/>
@@ -49894,10 +49845,10 @@
       <c r="AK1" s="357"/>
     </row>
     <row r="2" spans="1:37" s="56" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="479" t="s">
+      <c r="A2" s="477" t="s">
         <v>760</v>
       </c>
-      <c r="B2" s="476"/>
+      <c r="B2" s="474"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -49953,8 +49904,8 @@
       <c r="AK2" s="245"/>
     </row>
     <row r="3" spans="1:37" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="477"/>
-      <c r="B3" s="478"/>
+      <c r="A3" s="475"/>
+      <c r="B3" s="476"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
@@ -51102,17 +51053,17 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F3" location="Cascade!F:F" display="Host Country Est. Male Population (FY21)" xr:uid="{C6A99DFC-4F48-404C-9B66-D9590F47A2D3}"/>
-    <hyperlink ref="AC3" location="Cascade!BT:BT" display="HIV Positive" xr:uid="{2DCD329B-B29F-704E-8461-36B4301F077A}"/>
+    <hyperlink ref="AC3" location="Cascade!CE:CE" display="HIV Positive" xr:uid="{2DCD329B-B29F-704E-8461-36B4301F077A}"/>
     <hyperlink ref="G3" location="Cascade!H:H" display="Host Country Est. PLHIV (FY21)" xr:uid="{2930CCBC-8F45-954A-9C4B-E82145674BB9}"/>
     <hyperlink ref="H3" location="Cascade!J:J" display="Host Country Est. HIV Prevalence (FY21) (%)" xr:uid="{5289F01F-A702-2040-B8A4-F3E42F6D1A29}"/>
-    <hyperlink ref="I3" location="Cascade!P:P" display="Host Country Est. TX_CURR_SUBNAT (FY21)" xr:uid="{0B9E2838-E36E-914B-ABB2-4D62A487F4F9}"/>
-    <hyperlink ref="J3" location="Cascade!Z:Z" display="Host Country Est. Art Coverage (FY22) (%)" xr:uid="{A7D90546-FC05-1942-88B3-F73371278897}"/>
-    <hyperlink ref="AG3" location="Cascade!BO:BO" display="Total HTS_TST_POS (FY23)" xr:uid="{54DA9148-5100-4B4B-9121-6C351B2AE8A1}"/>
-    <hyperlink ref="AH3" location="VMMC!Z:Z" display="Total Positives from VMMC_CIRC (FY23) (%)" xr:uid="{823FE536-9720-0B41-B603-761E70AF5F5E}"/>
-    <hyperlink ref="AI3" location="Cascade!BW:BW" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{51CE2F45-E9AC-8943-8F4A-61132094AC48}"/>
-    <hyperlink ref="AJ3" location="Cascade!BZ:BZ" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{89FDD463-524F-4745-993F-7C848E2A4A01}"/>
-    <hyperlink ref="AK3" location="Cascade!CC:CC" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{DF85F481-72CF-A242-8614-1D2F503366BF}"/>
-    <hyperlink ref="K3" location="Cascade!AA:AA" display="Host Country Est. Population VLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{B9826B15-EC60-524A-9E47-7913491A2C2F}"/>
+    <hyperlink ref="I3" location="Cascade!T:T" display="Host Country Est. TX_CURR_SUBNAT (FY22)" xr:uid="{0B9E2838-E36E-914B-ABB2-4D62A487F4F9}"/>
+    <hyperlink ref="J3" location="Cascade!BS:BS" display="Host Country Est. ART Coverage (FY22) (%)" xr:uid="{A7D90546-FC05-1942-88B3-F73371278897}"/>
+    <hyperlink ref="AG3" location="Cascade!BZ:BZ" display="Total HTS_TST_POS (FY23)" xr:uid="{54DA9148-5100-4B4B-9121-6C351B2AE8A1}"/>
+    <hyperlink ref="AH3" location="VMMC!AC:AC" display="Total Positives from VMMC_CIRC (FY23) (%)" xr:uid="{823FE536-9720-0B41-B603-761E70AF5F5E}"/>
+    <hyperlink ref="AI3" location="Cascade!CH:CH" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{51CE2F45-E9AC-8943-8F4A-61132094AC48}"/>
+    <hyperlink ref="AJ3" location="Cascade!CK:CK" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{89FDD463-524F-4745-993F-7C848E2A4A01}"/>
+    <hyperlink ref="AK3" location="Cascade!CN:CN" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{DF85F481-72CF-A242-8614-1D2F503366BF}"/>
+    <hyperlink ref="K3" location="Cascade!AL:AL" display="Host Country Est. PopVLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{B9826B15-EC60-524A-9E47-7913491A2C2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Getting final COP22 Data Pack Template & Schema
Add TX_NET_NEW comparison
Update hyperlinks
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_Data_Pack_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D279E282-0D04-BF45-AFD0-D1FD86EADBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE7C2E6-D0EE-7A4C-9977-BC8D792893CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10480" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
+    <workbookView xWindow="-10480" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AGYW!$B$14:$M$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Cascade!$B$14:$CN$3876</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Cascade!$B$14:$CP$3876</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">CXCA!$C$1:$C$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">EID!$B$14:$G$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">HTS!$B$14:$CC$3551</definedName>
@@ -286,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ3" authorId="0" shapeId="0" xr:uid="{178F0F06-2EAF-1C4A-A595-51E401BF1B9C}">
+    <comment ref="AX3" authorId="0" shapeId="0" xr:uid="{178F0F06-2EAF-1C4A-A595-51E401BF1B9C}">
       <text>
         <r>
           <rPr>
@@ -295,7 +295,30 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Defaults to the higher of 90%, or the Estimated Host Country Diagnosis Rate.</t>
+          <t xml:space="preserve">Based on the combination of the </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AZ3" authorId="0" shapeId="0" xr:uid="{E43E5662-6968-0144-B73A-1BC6A5F35D49}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Negative values</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> in this column may potentially be related to differences between residential- vs. treatment-centric models.</t>
         </r>
       </text>
     </comment>
@@ -321,7 +344,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Per MER Guidance, must have been initiated on ART for at least 3 months to be eligible for VL Testing.</t>
+          <t>Per MER Guidance, individuals must have been initiated on ART for at least 3 months to be eligible for VL Testing.</t>
         </r>
       </text>
     </comment>
@@ -388,6 +411,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="BI3" authorId="0" shapeId="0" xr:uid="{944DCC40-618A-CC44-8550-DFCA544FB07E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Based on the combination of Planned PopVLS rate, the number of newly infected initiated on TX_CURR, &amp; the planned Eligibility rate of those recently initiated on ART.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="BM3" authorId="0" shapeId="0" xr:uid="{3FE1B096-924E-414E-8CD0-4533F2F27374}">
       <text>
         <r>
@@ -427,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BT3" authorId="0" shapeId="0" xr:uid="{159659A3-B5D7-0B4C-B5D3-73D03A4E82D0}">
+    <comment ref="BV3" authorId="0" shapeId="0" xr:uid="{159659A3-B5D7-0B4C-B5D3-73D03A4E82D0}">
       <text>
         <r>
           <rPr>
@@ -440,7 +476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BU3" authorId="0" shapeId="0" xr:uid="{023C1A10-F0BC-8D4C-BB93-A1477BF969E7}">
+    <comment ref="BW3" authorId="0" shapeId="0" xr:uid="{023C1A10-F0BC-8D4C-BB93-A1477BF969E7}">
       <text>
         <r>
           <rPr>
@@ -453,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CB3" authorId="0" shapeId="0" xr:uid="{B370B5FC-F9EB-DD42-AC95-33EC4A095AA6}">
+    <comment ref="CD3" authorId="0" shapeId="0" xr:uid="{B370B5FC-F9EB-DD42-AC95-33EC4A095AA6}">
       <text>
         <r>
           <rPr>
@@ -476,7 +512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CC3" authorId="0" shapeId="0" xr:uid="{F87C6E9F-BB82-7843-9D11-41D4D4919EE5}">
+    <comment ref="CE3" authorId="0" shapeId="0" xr:uid="{F87C6E9F-BB82-7843-9D11-41D4D4919EE5}">
       <text>
         <r>
           <rPr>
@@ -499,7 +535,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CD3" authorId="0" shapeId="0" xr:uid="{5781455F-CF5D-4642-A660-A7D892977F10}">
+    <comment ref="CF3" authorId="0" shapeId="0" xr:uid="{5781455F-CF5D-4642-A660-A7D892977F10}">
       <text>
         <r>
           <rPr>
@@ -522,7 +558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CE3" authorId="0" shapeId="0" xr:uid="{0DAA8CD2-C824-2B4A-86FD-97EB7498DC1C}">
+    <comment ref="CG3" authorId="0" shapeId="0" xr:uid="{0DAA8CD2-C824-2B4A-86FD-97EB7498DC1C}">
       <text>
         <r>
           <rPr>
@@ -545,7 +581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CO3" authorId="0" shapeId="0" xr:uid="{554A2474-AA4F-0E45-AE83-49ED7F3B5318}">
+    <comment ref="CQ3" authorId="0" shapeId="0" xr:uid="{554A2474-AA4F-0E45-AE83-49ED7F3B5318}">
       <text>
         <r>
           <rPr>
@@ -568,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CP3" authorId="1" shapeId="0" xr:uid="{846982D7-B956-9C43-80AF-9987410C0060}">
+    <comment ref="CR3" authorId="1" shapeId="0" xr:uid="{846982D7-B956-9C43-80AF-9987410C0060}">
       <text>
         <r>
           <rPr>
@@ -621,7 +657,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CQ3" authorId="1" shapeId="0" xr:uid="{8C5EA5CF-B22C-2841-8751-BF3E2FC571B4}">
+    <comment ref="CS3" authorId="1" shapeId="0" xr:uid="{8C5EA5CF-B22C-2841-8751-BF3E2FC571B4}">
       <text>
         <r>
           <rPr>
@@ -673,7 +709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CS3" authorId="1" shapeId="0" xr:uid="{E5E68074-A876-F143-8AD6-A88BBEF2EC75}">
+    <comment ref="CU3" authorId="1" shapeId="0" xr:uid="{E5E68074-A876-F143-8AD6-A88BBEF2EC75}">
       <text>
         <r>
           <rPr>
@@ -697,7 +733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CU3" authorId="1" shapeId="0" xr:uid="{6A88A0D6-7A4C-9C4F-A2EF-91A4A73C6EC0}">
+    <comment ref="CW3" authorId="1" shapeId="0" xr:uid="{6A88A0D6-7A4C-9C4F-A2EF-91A4A73C6EC0}">
       <text>
         <r>
           <rPr>
@@ -2608,7 +2644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4618" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4633" uniqueCount="1220">
   <si>
     <t>TX_CURR</t>
   </si>
@@ -6209,9 +6245,6 @@
     <t>H.C. Est. VLT Coverage (FY22) (%)</t>
   </si>
   <si>
-    <t>Planned % Newly or Re-Initiated on ART Eligible for VLT (FY23) (%)</t>
-  </si>
-  <si>
     <t>PEPFAR  Total EVLT (FY23)</t>
   </si>
   <si>
@@ -6344,9 +6377,6 @@
     <t>PEPFAR VLT Coverage (FY22 Targets) (%)</t>
   </si>
   <si>
-    <t>Planned % New Infections Diagnosed &amp; Linked to ART (FY23) (%)</t>
-  </si>
-  <si>
     <t>Prev. PLHIV Initiated on TX_CURR (FY23)</t>
   </si>
   <si>
@@ -6356,9 +6386,6 @@
     <t>% Prev. Infected TX_NEW from Prev. Diagnosed (FY23) (%)</t>
   </si>
   <si>
-    <t>TX_NEW from New Diagnosis (FY23)</t>
-  </si>
-  <si>
     <t>PLHIV.Undiagnosed.T_1</t>
   </si>
   <si>
@@ -6414,6 +6441,27 @@
   </si>
   <si>
     <t>TX_CURR.NoTPT.T_1</t>
+  </si>
+  <si>
+    <t>Planned % New Infections Diagnosed (FY23) (%)</t>
+  </si>
+  <si>
+    <t>Planned % Recently Initiated on ART Eligible for VLT (FY23) (%)</t>
+  </si>
+  <si>
+    <t>TX_NET_NEW (FY23)</t>
+  </si>
+  <si>
+    <t>TX_NET_NEW.T_1</t>
+  </si>
+  <si>
+    <t>TX_NET_NEW.T</t>
+  </si>
+  <si>
+    <t>TX_NEW from New Diagnoses (FY23)</t>
+  </si>
+  <si>
+    <t>TX_NET_NEW (FY22 Targets)</t>
   </si>
 </sst>
 </file>
@@ -7135,7 +7183,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="478">
+  <cellXfs count="479">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -8122,6 +8170,9 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="33" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
@@ -8132,7 +8183,7 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="3" xr:uid="{EBDE175B-1152-3C44-B18E-2B948C595077}"/>
   </cellStyles>
-  <dxfs count="177">
+  <dxfs count="176">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -9619,16 +9670,6 @@
       </font>
       <fill>
         <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -13413,9 +13454,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17780,7 +17819,7 @@
         <v>||</v>
       </c>
       <c r="F15" s="161" t="str" cm="1">
-        <f t="array" ref="F15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$BS:$BS,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$BS:$BS,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="F15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$BU:$BU,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$BU:$BU,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="G15" s="248" t="str" cm="1">
@@ -17788,15 +17827,15 @@
         <v/>
       </c>
       <c r="H15" s="118" t="str" cm="1">
-        <f t="array" ref="H15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$BZ:$BZ,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$BZ:$BZ,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="H15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CB:$CB,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CB:$CB,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="I15" s="118" t="str" cm="1">
-        <f t="array" ref="I15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CR:$CR,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CR:$CR,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="I15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CT:$CT,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CT:$CT,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="J15" s="118" t="str" cm="1">
-        <f t="array" ref="J15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CT:$CT,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CT:$CT,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="J15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CV:$CV,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CV:$CV,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="K15" s="118" t="str" cm="1">
@@ -17816,7 +17855,7 @@
         <v/>
       </c>
       <c r="O15" s="118" t="str" cm="1">
-        <f t="array" ref="O15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CG:$CG,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CG:$CG,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="O15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CI:$CI,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CI:$CI,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="P15" s="161" t="str">
@@ -17976,11 +18015,11 @@
         <v/>
       </c>
       <c r="BR15" s="118" t="str" cm="1">
-        <f t="array" ref="BR15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CS:$CS,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CS:$CS,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="BR15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CU:$CU,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CU:$CU,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="BS15" s="118" t="str" cm="1">
-        <f t="array" ref="BS15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CU:$CU,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CU:$CU,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
+        <f t="array" ref="BS15">IFERROR(1/(1/IF($C15="50+",SUM(SUMIFS(Cascade!$CW:$CW,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CW:$CW,MATCH($E15,Cascade!$E:$E,0)))),"")</f>
         <v/>
       </c>
       <c r="BT15" s="118" t="str" cm="1">
@@ -18116,20 +18155,20 @@
     <hyperlink ref="S3" location="HTS!L:L" display="HTS_TST PMTCT Post ANC1: Positive (%)" xr:uid="{F1FC89C1-DC5F-B840-AAF9-44A1F4477F09}"/>
     <hyperlink ref="U3" location="HTS!N:N" display="VMMC_CIRC: HIV Positive (%)" xr:uid="{B1FE978A-966A-8843-8592-43CD0B9E86E3}"/>
     <hyperlink ref="F3" location="Cascade!BS:BS" display="Host Country Est. ART Coverage (FY22) (%)" xr:uid="{62E0A0AF-20D9-6845-8B29-307EB64A2270}"/>
-    <hyperlink ref="H3" location="Cascade!BZ:BZ" display="Total HTS_TST_POS (FY23)" xr:uid="{4F5D648D-D7C2-5348-BC20-3F43FA74D673}"/>
-    <hyperlink ref="I3" location="Cascade!CR:CR" display="HTS_INDEX Community Positives (FY23)" xr:uid="{F10D394A-A559-CD44-A6BB-3657FE272021}"/>
+    <hyperlink ref="H3" location="Cascade!CB:CB" display="Total HTS_TST_POS (FY23)" xr:uid="{4F5D648D-D7C2-5348-BC20-3F43FA74D673}"/>
+    <hyperlink ref="I3" location="Cascade!CT:CT" display="HTS_INDEX Community Positives (FY23)" xr:uid="{F10D394A-A559-CD44-A6BB-3657FE272021}"/>
     <hyperlink ref="K3" location="PMTCT!AF:AF" display="PMTCT_STAT New Positives (FY23)" xr:uid="{812A1C32-C461-DA45-A52E-F20D4356FFAA}"/>
     <hyperlink ref="L3" location="PMTCT!AV:AV" display="HTS_TST Post ANC1 New Positives (FY23)" xr:uid="{D8D811EC-2ACC-F544-8B0B-9B3CA11DE028}"/>
     <hyperlink ref="M3" location="TB!Q:Q" display="TB_STAT New Positives (FY23)" xr:uid="{E57FF0A3-0CCA-514F-A80D-BBE50EC0318F}"/>
     <hyperlink ref="N3" location="VMMC!AC:AC" display="VMMC_CIRC New Positives (FY23)" xr:uid="{844A055A-478B-6640-9164-F1EA9117BE57}"/>
-    <hyperlink ref="O3" location="Cascade!CG:CG" display="HTS_TST_POS from All Other Modalities (FY23)" xr:uid="{C5277E53-10C0-2243-A9D4-1D88FF90A312}"/>
+    <hyperlink ref="O3" location="Cascade!CI:CI" display="HTS_TST_POS from All Other Modalities (FY23)" xr:uid="{C5277E53-10C0-2243-A9D4-1D88FF90A312}"/>
     <hyperlink ref="BT3" location="PMTCT!AG:AG" display="PMTCT_STAT New Negatives (FY23)" xr:uid="{59410773-B3DC-854C-945D-B45072CA61F7}"/>
     <hyperlink ref="BU3" location="PMTCT!AW:AW" display="HTS_TST Post ANC1 Negatives (FY23)" xr:uid="{C61C3228-0418-F04A-A70D-6531131C0C12}"/>
     <hyperlink ref="BV3" location="TB!R:R" display="TB_STAT New Negatives (FY22)" xr:uid="{86527BC9-57C0-1640-BE6B-CB6BEA15D2D3}"/>
     <hyperlink ref="BW3" location="VMMC!AD:AD" display="VMMC_CIRC Negatives (FY22)" xr:uid="{3AD47724-6BB1-D148-BE45-144B25A52781}"/>
-    <hyperlink ref="J3" location="Cascade!CT:CT" display="HTS_INDEX Facility Positives (FY23)" xr:uid="{F530B28A-AF9A-CF45-8C43-7C26547A0809}"/>
-    <hyperlink ref="BR3" location="Cascade!CS:CS" display="HTS_INDEX Community New Negatives (FY23)" xr:uid="{7614C962-EB54-114D-8144-33CC1CCC8A19}"/>
-    <hyperlink ref="BS3" location="Cascade!CU:CU" display="HTS_INDEX Facility New Negatives (FY23)" xr:uid="{9F773D86-C36C-D14F-AD2D-78557CF866D2}"/>
+    <hyperlink ref="J3" location="Cascade!CV:CV" display="HTS_INDEX Facility Positives (FY23)" xr:uid="{F530B28A-AF9A-CF45-8C43-7C26547A0809}"/>
+    <hyperlink ref="BR3" location="Cascade!CU:CU" display="HTS_INDEX Community New Negatives (FY23)" xr:uid="{7614C962-EB54-114D-8144-33CC1CCC8A19}"/>
+    <hyperlink ref="BS3" location="Cascade!CW:CW" display="HTS_INDEX Facility New Negatives (FY23)" xr:uid="{9F773D86-C36C-D14F-AD2D-78557CF866D2}"/>
     <hyperlink ref="G3" location="Cascade!AL:AL" display="Host Country Est. PopVLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{F30F0EE7-FFA9-BF42-AF25-EB64195A4AA3}"/>
     <hyperlink ref="R3" location="HTS!K:K" display="PMTCT_STAT: New Positive (%)" xr:uid="{92A92D18-3020-A74B-ACBE-46783EF61EC0}"/>
     <hyperlink ref="BD3" location="HTS!AC:AC" display="Positive" xr:uid="{0268EFB4-1FE0-9648-AF9F-08E2D9DE337E}"/>
@@ -19867,14 +19906,14 @@
         <v>1</v>
       </c>
       <c r="O15" s="72" t="str" cm="1">
-        <f t="array" ref="O15">IFERROR(ROUND($N15*IF($C15="50+",SUM(SUMIFS(Cascade!$CR:$CR,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CR:$CR,MATCH($E15,Cascade!$E:$E,0))),0),"")</f>
+        <f t="array" ref="O15">IFERROR(ROUND($N15*IF($C15="50+",SUM(SUMIFS(Cascade!$CT:$CT,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CT:$CT,MATCH($E15,Cascade!$E:$E,0))),0),"")</f>
         <v/>
       </c>
       <c r="P15" s="161">
         <v>1</v>
       </c>
       <c r="Q15" s="72" t="str" cm="1">
-        <f t="array" ref="Q15">IFERROR(ROUND($P15*IF($C15="50+",SUM(SUMIFS(Cascade!$CT:$CT,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CT:$CT,MATCH($E15,Cascade!$E:$E,0))),0),"")</f>
+        <f t="array" ref="Q15">IFERROR(ROUND($P15*IF($C15="50+",SUM(SUMIFS(Cascade!$CV:$CV,Cascade!$B:$B,$B15,Cascade!$C:$C,{"50-54","55-59","60-64","65+"},Cascade!$D:$D,$D15)),INDEX(Cascade!$CV:$CV,MATCH($E15,Cascade!$E:$E,0))),0),"")</f>
         <v/>
       </c>
       <c r="R15" s="161">
@@ -19983,8 +20022,8 @@
   <hyperlinks>
     <hyperlink ref="J3" location="TB!Q:Q" display="% of Positives" xr:uid="{C240581F-0312-414F-99B5-7DC0EEDCE2D4}"/>
     <hyperlink ref="R3" location="HTS!AI:AI" display="% of Positives" xr:uid="{BCB03ADB-EB0F-9449-B4AD-8CCCC65196F5}"/>
-    <hyperlink ref="P3" location="Cascade!CT:CT" display="% of Positives" xr:uid="{F5E990DE-DF37-E84A-B2EC-94F34D61814F}"/>
-    <hyperlink ref="N3" location="Cascade!CR:CR" display="% of Positives" xr:uid="{8E652247-ECD7-3148-9B98-BE20BACDD9E8}"/>
+    <hyperlink ref="P3" location="Cascade!CV:CV" display="% of Positives" xr:uid="{F5E990DE-DF37-E84A-B2EC-94F34D61814F}"/>
+    <hyperlink ref="N3" location="Cascade!CT:CT" display="% of Positives" xr:uid="{8E652247-ECD7-3148-9B98-BE20BACDD9E8}"/>
     <hyperlink ref="F3" location="PMTCT!AF:AF" display="% of Positives" xr:uid="{F2B49097-C594-1242-BE6B-4FE63474113E}"/>
     <hyperlink ref="H3" location="PMTCT!AV:AV" display="% of Positives" xr:uid="{564F8A9F-7394-CC4D-8071-B2C639592C77}"/>
     <hyperlink ref="L3" location="VMMC!AC:AC" display="% of Positives" xr:uid="{475FB800-421E-EC40-BC04-9B9751E0C7DD}"/>
@@ -20165,25 +20204,25 @@
         <v>40</v>
       </c>
       <c r="P3" s="144" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="Q3" s="116" t="s">
+        <v>1174</v>
+      </c>
+      <c r="R3" s="145" t="s">
         <v>1175</v>
       </c>
-      <c r="R3" s="145" t="s">
-        <v>1176</v>
-      </c>
       <c r="S3" s="116" t="s">
+        <v>1208</v>
+      </c>
+      <c r="T3" s="116" t="s">
         <v>1211</v>
       </c>
-      <c r="T3" s="116" t="s">
-        <v>1214</v>
-      </c>
       <c r="U3" s="354" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="V3" s="48" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="W3" s="69" t="s">
         <v>32</v>
@@ -20873,7 +20912,7 @@
         <v>434</v>
       </c>
       <c r="P14" s="174" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="Q14" s="176" t="s">
         <v>439</v>
@@ -20882,10 +20921,10 @@
         <v>440</v>
       </c>
       <c r="S14" s="176" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="T14" s="176" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="U14" s="249" t="s">
         <v>435</v>
@@ -21444,7 +21483,7 @@
         <v>585</v>
       </c>
       <c r="T3" s="376" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="U3" s="69" t="s">
         <v>1085</v>
@@ -25494,7 +25533,7 @@
     </row>
     <row r="2" spans="1:74" s="56" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="477" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B2" s="474"/>
       <c r="C2" s="111" t="s">
@@ -25617,7 +25656,7 @@
         <v>861</v>
       </c>
       <c r="D3" s="259" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="E3" s="265" t="s">
         <v>862</v>
@@ -25641,7 +25680,7 @@
         <v>861</v>
       </c>
       <c r="L3" s="259" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="M3" s="265" t="s">
         <v>862</v>
@@ -41889,21 +41928,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4">
-    <cfRule type="containsText" dxfId="176" priority="3" operator="containsText" text="BLANK PRIORITIZATIONS">
+    <cfRule type="containsText" dxfId="175" priority="3" operator="containsText" text="BLANK PRIORITIZATIONS">
       <formula>NOT(ISERROR(SEARCH("BLANK PRIORITIZATIONS",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="expression" dxfId="175" priority="2">
+    <cfRule type="expression" dxfId="174" priority="2">
       <formula>AND(ROW(C1)&gt;14,$B1&lt;&gt;"",C1&lt;&gt;1,C1&lt;&gt;2,C1&lt;&gt;4,C1&lt;&gt;5,C1&lt;&gt;6,C1&lt;&gt;7,C1&lt;&gt;8,C1&lt;&gt;"M",C1&lt;&gt;"NA")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="174" priority="728">
+    <cfRule type="expression" dxfId="173" priority="728">
       <formula>AND(ROW($D1)&gt;14,$D1="",$B1&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="729">
-      <formula>AND(ROW($D1)&gt;14,$D1&lt;&gt;$C1,$B1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="172" priority="729">
+      <formula>AND(LEFT($B1,4)&lt;&gt;"_Mil",ROW($D1)&gt;14,$D1&lt;&gt;$C1,$B1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41913,9 +41952,9 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DDBC09-F535-654B-A49D-7D22E3100EEA}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:DC15"/>
+  <dimension ref="A1:DE15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -41962,28 +42001,27 @@
     <col min="43" max="43" width="11.83203125" style="415" customWidth="1"/>
     <col min="44" max="47" width="11.83203125" style="437" customWidth="1"/>
     <col min="48" max="48" width="11.83203125" style="415" customWidth="1"/>
-    <col min="49" max="49" width="11.83203125" customWidth="1"/>
-    <col min="50" max="51" width="11.83203125" style="437" customWidth="1"/>
-    <col min="52" max="52" width="11.83203125" customWidth="1"/>
-    <col min="53" max="59" width="11.83203125" style="437" customWidth="1"/>
+    <col min="49" max="50" width="11.83203125" customWidth="1"/>
+    <col min="51" max="59" width="11.83203125" style="437" customWidth="1"/>
     <col min="60" max="61" width="11.83203125" customWidth="1"/>
     <col min="62" max="64" width="11.83203125" style="437" customWidth="1"/>
     <col min="65" max="65" width="11.83203125" style="415" customWidth="1"/>
     <col min="66" max="66" width="11.83203125" style="437" customWidth="1"/>
     <col min="67" max="67" width="11.83203125" style="415" customWidth="1"/>
     <col min="68" max="69" width="11.83203125" style="437" customWidth="1"/>
-    <col min="70" max="70" width="11.83203125" style="415" customWidth="1"/>
-    <col min="71" max="72" width="11.83203125" style="437" customWidth="1"/>
-    <col min="73" max="73" width="11.83203125" style="415" customWidth="1"/>
-    <col min="74" max="85" width="11.83203125" customWidth="1"/>
-    <col min="86" max="86" width="11.83203125" style="415" customWidth="1"/>
-    <col min="87" max="92" width="11.83203125" customWidth="1"/>
-    <col min="93" max="93" width="11.83203125" style="415" customWidth="1"/>
-    <col min="94" max="100" width="11.83203125" customWidth="1"/>
-    <col min="101" max="101" width="11.83203125" style="415" customWidth="1"/>
+    <col min="70" max="71" width="11.83203125" style="438" customWidth="1"/>
+    <col min="72" max="72" width="11.83203125" style="415" customWidth="1"/>
+    <col min="73" max="74" width="11.83203125" style="437" customWidth="1"/>
+    <col min="75" max="75" width="11.83203125" style="415" customWidth="1"/>
+    <col min="76" max="87" width="11.83203125" customWidth="1"/>
+    <col min="88" max="88" width="11.83203125" style="415" customWidth="1"/>
+    <col min="89" max="94" width="11.83203125" customWidth="1"/>
+    <col min="95" max="95" width="11.83203125" style="415" customWidth="1"/>
+    <col min="96" max="102" width="11.83203125" customWidth="1"/>
+    <col min="103" max="103" width="11.83203125" style="415" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" s="57" customFormat="1" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:109" s="57" customFormat="1" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>301</v>
       </c>
@@ -42046,12 +42084,12 @@
       <c r="AT1" s="360"/>
       <c r="AU1" s="96"/>
       <c r="AV1" s="242" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="AW1" s="114"/>
-      <c r="AX1" s="357"/>
-      <c r="AY1" s="340"/>
-      <c r="AZ1" s="244"/>
+      <c r="AX1" s="244"/>
+      <c r="AY1" s="357"/>
+      <c r="AZ1" s="340"/>
       <c r="BA1" s="410"/>
       <c r="BB1" s="165"/>
       <c r="BC1" s="360"/>
@@ -42073,50 +42111,52 @@
       </c>
       <c r="BP1" s="360"/>
       <c r="BQ1" s="96"/>
-      <c r="BR1" s="439" t="s">
+      <c r="BR1" s="380"/>
+      <c r="BS1" s="380"/>
+      <c r="BT1" s="439" t="s">
         <v>767</v>
       </c>
-      <c r="BS1" s="244"/>
-      <c r="BT1" s="360"/>
-      <c r="BU1" s="164" t="s">
+      <c r="BU1" s="244"/>
+      <c r="BV1" s="360"/>
+      <c r="BW1" s="164" t="s">
         <v>1138</v>
       </c>
-      <c r="BV1" s="77"/>
-      <c r="BW1" s="77"/>
-      <c r="BX1" s="165"/>
-      <c r="BY1" s="165"/>
-      <c r="BZ1" s="130"/>
-      <c r="CA1" s="130"/>
+      <c r="BX1" s="77"/>
+      <c r="BY1" s="77"/>
+      <c r="BZ1" s="165"/>
+      <c r="CA1" s="165"/>
       <c r="CB1" s="130"/>
       <c r="CC1" s="130"/>
       <c r="CD1" s="130"/>
       <c r="CE1" s="130"/>
       <c r="CF1" s="130"/>
       <c r="CG1" s="130"/>
-      <c r="CH1" s="242" t="s">
+      <c r="CH1" s="130"/>
+      <c r="CI1" s="130"/>
+      <c r="CJ1" s="242" t="s">
         <v>966</v>
       </c>
-      <c r="CI1" s="357"/>
-      <c r="CJ1" s="357"/>
       <c r="CK1" s="357"/>
       <c r="CL1" s="357"/>
       <c r="CM1" s="357"/>
       <c r="CN1" s="357"/>
-      <c r="CO1" s="242" t="s">
+      <c r="CO1" s="357"/>
+      <c r="CP1" s="357"/>
+      <c r="CQ1" s="242" t="s">
         <v>9</v>
       </c>
-      <c r="CP1" s="45"/>
-      <c r="CQ1" s="45"/>
-      <c r="CR1" s="80"/>
-      <c r="CS1" s="80"/>
+      <c r="CR1" s="45"/>
+      <c r="CS1" s="45"/>
       <c r="CT1" s="80"/>
       <c r="CU1" s="80"/>
-      <c r="CV1" s="35"/>
-      <c r="CW1" s="110" t="s">
+      <c r="CV1" s="80"/>
+      <c r="CW1" s="80"/>
+      <c r="CX1" s="35"/>
+      <c r="CY1" s="110" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:107" s="56" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:109" s="56" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="473" t="s">
         <v>1145</v>
       </c>
@@ -42188,11 +42228,11 @@
         <v>74</v>
       </c>
       <c r="AW2" s="115"/>
-      <c r="AX2" s="245"/>
-      <c r="AY2" s="115"/>
-      <c r="AZ2" s="245" t="s">
+      <c r="AX2" s="245" t="s">
         <v>2</v>
       </c>
+      <c r="AY2" s="245"/>
+      <c r="AZ2" s="115"/>
       <c r="BA2" s="166"/>
       <c r="BB2" s="166"/>
       <c r="BC2" s="361"/>
@@ -42218,56 +42258,60 @@
       <c r="BQ2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="443" t="s">
+      <c r="BR2" s="333" t="s">
+        <v>74</v>
+      </c>
+      <c r="BS2" s="333"/>
+      <c r="BT2" s="443" t="s">
         <v>3</v>
       </c>
-      <c r="BS2" s="245"/>
-      <c r="BT2" s="363"/>
-      <c r="BU2" s="159" t="s">
+      <c r="BU2" s="245"/>
+      <c r="BV2" s="363"/>
+      <c r="BW2" s="159" t="s">
         <v>2</v>
       </c>
-      <c r="BV2" s="91"/>
-      <c r="BW2" s="88"/>
-      <c r="BX2" s="166"/>
-      <c r="BY2" s="166"/>
-      <c r="BZ2" s="102" t="s">
+      <c r="BX2" s="91"/>
+      <c r="BY2" s="88"/>
+      <c r="BZ2" s="166"/>
+      <c r="CA2" s="166"/>
+      <c r="CB2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="CA2" s="102"/>
-      <c r="CB2" s="102"/>
       <c r="CC2" s="102"/>
       <c r="CD2" s="102"/>
       <c r="CE2" s="102"/>
       <c r="CF2" s="102"/>
       <c r="CG2" s="102"/>
-      <c r="CH2" s="159" t="s">
+      <c r="CH2" s="102"/>
+      <c r="CI2" s="102"/>
+      <c r="CJ2" s="159" t="s">
         <v>59</v>
       </c>
-      <c r="CI2" s="361"/>
-      <c r="CJ2" s="361"/>
       <c r="CK2" s="361"/>
       <c r="CL2" s="361"/>
       <c r="CM2" s="361"/>
       <c r="CN2" s="361"/>
-      <c r="CO2" s="243" t="s">
+      <c r="CO2" s="361"/>
+      <c r="CP2" s="361"/>
+      <c r="CQ2" s="243" t="s">
         <v>2</v>
       </c>
-      <c r="CP2" s="34"/>
-      <c r="CQ2" s="34"/>
-      <c r="CR2" s="81" t="s">
+      <c r="CR2" s="34"/>
+      <c r="CS2" s="34"/>
+      <c r="CT2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="CS2" s="81"/>
-      <c r="CT2" s="81"/>
       <c r="CU2" s="81"/>
-      <c r="CV2" s="34" t="s">
+      <c r="CV2" s="81"/>
+      <c r="CW2" s="81"/>
+      <c r="CX2" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="CW2" s="447" t="s">
+      <c r="CY2" s="447" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:107" s="40" customFormat="1" ht="134" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:109" s="40" customFormat="1" ht="134" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="475"/>
       <c r="B3" s="476"/>
       <c r="C3" s="47"/>
@@ -42364,10 +42408,10 @@
         <v>51</v>
       </c>
       <c r="AJ3" s="372" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="AK3" s="274" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="AL3" s="358" t="s">
         <v>1111</v>
@@ -42376,7 +42420,7 @@
         <v>1120</v>
       </c>
       <c r="AN3" s="296" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="AO3" s="255" t="s">
         <v>977</v>
@@ -42400,19 +42444,19 @@
         <v>1119</v>
       </c>
       <c r="AV3" s="353" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="AW3" s="116" t="s">
+        <v>1188</v>
+      </c>
+      <c r="AX3" s="354" t="s">
+        <v>1213</v>
+      </c>
+      <c r="AY3" s="358" t="s">
+        <v>1125</v>
+      </c>
+      <c r="AZ3" s="272" t="s">
         <v>1189</v>
-      </c>
-      <c r="AX3" s="358" t="s">
-        <v>1125</v>
-      </c>
-      <c r="AY3" s="272" t="s">
-        <v>1190</v>
-      </c>
-      <c r="AZ3" s="354" t="s">
-        <v>1192</v>
       </c>
       <c r="BA3" s="200" t="s">
         <v>1115</v>
@@ -42421,37 +42465,37 @@
         <v>1116</v>
       </c>
       <c r="BC3" s="274" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="BD3" s="274" t="s">
-        <v>1148</v>
+        <v>1214</v>
       </c>
       <c r="BE3" s="246" t="s">
         <v>1147</v>
       </c>
       <c r="BF3" s="371" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="BG3" s="274" t="s">
         <v>1146</v>
       </c>
       <c r="BH3" s="253" t="s">
+        <v>1182</v>
+      </c>
+      <c r="BI3" s="253" t="s">
+        <v>1191</v>
+      </c>
+      <c r="BJ3" s="296" t="s">
         <v>1183</v>
       </c>
-      <c r="BI3" s="253" t="s">
-        <v>1193</v>
-      </c>
-      <c r="BJ3" s="296" t="s">
+      <c r="BK3" s="296" t="s">
+        <v>1148</v>
+      </c>
+      <c r="BL3" s="253" t="s">
         <v>1184</v>
       </c>
-      <c r="BK3" s="296" t="s">
-        <v>1149</v>
-      </c>
-      <c r="BL3" s="253" t="s">
-        <v>1185</v>
-      </c>
       <c r="BM3" s="368" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="BN3" s="296" t="s">
         <v>788</v>
@@ -42465,110 +42509,116 @@
       <c r="BQ3" s="296" t="s">
         <v>789</v>
       </c>
-      <c r="BR3" s="446" t="s">
+      <c r="BR3" s="334" t="s">
+        <v>1219</v>
+      </c>
+      <c r="BS3" s="334" t="s">
+        <v>1215</v>
+      </c>
+      <c r="BT3" s="446" t="s">
         <v>962</v>
       </c>
-      <c r="BS3" s="358" t="s">
+      <c r="BU3" s="358" t="s">
         <v>1136</v>
       </c>
-      <c r="BT3" s="364" t="s">
-        <v>1170</v>
-      </c>
-      <c r="BU3" s="58" t="s">
-        <v>1195</v>
-      </c>
-      <c r="BV3" s="93" t="s">
+      <c r="BV3" s="364" t="s">
+        <v>1169</v>
+      </c>
+      <c r="BW3" s="58" t="s">
+        <v>1193</v>
+      </c>
+      <c r="BX3" s="93" t="s">
         <v>840</v>
       </c>
-      <c r="BW3" s="93" t="s">
-        <v>1196</v>
-      </c>
-      <c r="BX3" s="200" t="s">
+      <c r="BY3" s="93" t="s">
+        <v>1218</v>
+      </c>
+      <c r="BZ3" s="200" t="s">
         <v>1102</v>
       </c>
-      <c r="BY3" s="167" t="s">
+      <c r="CA3" s="167" t="s">
         <v>1103</v>
       </c>
-      <c r="BZ3" s="100" t="s">
+      <c r="CB3" s="100" t="s">
         <v>936</v>
       </c>
-      <c r="CA3" s="70" t="s">
+      <c r="CC3" s="70" t="s">
         <v>937</v>
       </c>
-      <c r="CB3" s="70" t="s">
+      <c r="CD3" s="70" t="s">
         <v>851</v>
       </c>
-      <c r="CC3" s="70" t="s">
+      <c r="CE3" s="70" t="s">
         <v>852</v>
       </c>
-      <c r="CD3" s="70" t="s">
+      <c r="CF3" s="70" t="s">
         <v>853</v>
       </c>
-      <c r="CE3" s="70" t="s">
+      <c r="CG3" s="70" t="s">
         <v>938</v>
       </c>
-      <c r="CF3" s="70" t="s">
+      <c r="CH3" s="70" t="s">
         <v>939</v>
       </c>
-      <c r="CG3" s="70" t="s">
+      <c r="CI3" s="70" t="s">
         <v>855</v>
       </c>
-      <c r="CH3" s="374" t="s">
+      <c r="CJ3" s="374" t="s">
         <v>806</v>
       </c>
-      <c r="CI3" s="375" t="s">
+      <c r="CK3" s="375" t="s">
         <v>940</v>
       </c>
-      <c r="CJ3" s="375" t="s">
+      <c r="CL3" s="375" t="s">
         <v>805</v>
       </c>
-      <c r="CK3" s="375" t="s">
+      <c r="CM3" s="375" t="s">
         <v>807</v>
       </c>
-      <c r="CL3" s="375" t="s">
+      <c r="CN3" s="375" t="s">
         <v>817</v>
       </c>
-      <c r="CM3" s="375" t="s">
+      <c r="CO3" s="375" t="s">
         <v>941</v>
       </c>
-      <c r="CN3" s="375" t="s">
+      <c r="CP3" s="375" t="s">
         <v>808</v>
       </c>
-      <c r="CO3" s="376" t="s">
+      <c r="CQ3" s="376" t="s">
         <v>942</v>
       </c>
-      <c r="CP3" s="48" t="s">
+      <c r="CR3" s="48" t="s">
         <v>964</v>
       </c>
-      <c r="CQ3" s="48" t="s">
+      <c r="CS3" s="48" t="s">
         <v>965</v>
       </c>
-      <c r="CR3" s="69" t="s">
+      <c r="CT3" s="69" t="s">
         <v>1017</v>
       </c>
-      <c r="CS3" s="69" t="s">
+      <c r="CU3" s="69" t="s">
         <v>943</v>
       </c>
-      <c r="CT3" s="69" t="s">
+      <c r="CV3" s="69" t="s">
         <v>1018</v>
       </c>
-      <c r="CU3" s="69" t="s">
+      <c r="CW3" s="69" t="s">
         <v>944</v>
       </c>
-      <c r="CV3" s="373" t="s">
+      <c r="CX3" s="373" t="s">
         <v>945</v>
       </c>
-      <c r="CW3" s="448" t="s">
+      <c r="CY3" s="448" t="s">
         <v>1135</v>
       </c>
-      <c r="CX3"/>
-      <c r="CY3"/>
       <c r="CZ3"/>
       <c r="DA3"/>
       <c r="DB3"/>
       <c r="DC3"/>
-    </row>
-    <row r="4" spans="1:107" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD3"/>
+      <c r="DE3"/>
+    </row>
+    <row r="4" spans="1:109" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
@@ -42722,17 +42772,17 @@
         <f>SUBTOTAL(109,AW$15:INDEX(AW:AW,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="AX4" s="359" t="str">
+      <c r="AX4" s="247" t="str">
+        <f>IF($N$4=0,"",($BH$4/$AK$4)/$N$4)</f>
+        <v/>
+      </c>
+      <c r="AY4" s="359" t="str">
         <f>IF(SUM($P4)=0,"",SUM($T4)/$P4)</f>
         <v/>
       </c>
-      <c r="AY4" s="337">
-        <f>SUBTOTAL(109,AY$15:INDEX(AY:AY,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+      <c r="AZ4" s="337">
+        <f>SUBTOTAL(109,AZ$15:INDEX(AZ:AZ,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
-      </c>
-      <c r="AZ4" s="247" t="str">
-        <f>IF($N$4=0,"",($BH$4/$AK$4)/$N$4)</f>
-        <v/>
       </c>
       <c r="BA4" s="168" t="str">
         <f>IF(SUM($Z4)=0,"",SUM($AA4)/$Z4)</f>
@@ -42743,7 +42793,7 @@
         <v/>
       </c>
       <c r="BC4" s="247" t="str">
-        <f>IF($BZ$4=0,"",$BN$4/$BZ$4)</f>
+        <f>IF($CB$4=0,"",$BN$4/$CB$4)</f>
         <v/>
       </c>
       <c r="BD4" s="247" t="str">
@@ -42796,56 +42846,56 @@
         <f>SUBTOTAL(109,BQ$15:INDEX(BQ:BQ,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="BR4" s="440">
+      <c r="BR4" s="381">
         <f>SUBTOTAL(109,BR$15:INDEX(BR:BR,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="BS4" s="247" t="str">
+      <c r="BS4" s="381">
+        <f>SUBTOTAL(109,BS$15:INDEX(BS:BS,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+        <v>0</v>
+      </c>
+      <c r="BT4" s="440">
+        <f>SUBTOTAL(109,BT$15:INDEX(BT:BT,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+        <v>0</v>
+      </c>
+      <c r="BU4" s="247" t="str">
         <f>IF(SUM($H4)=0,"",SUM($T4)/$H4)</f>
         <v/>
       </c>
-      <c r="BT4" s="365" t="str">
-        <f>IF(SUM($H4,$N4)=0,"",SUM($BR4)/SUM($H4,$N4))</f>
+      <c r="BV4" s="365" t="str">
+        <f>IF(SUM($H4,$N4)=0,"",SUM($BT4)/SUM($H4,$N4))</f>
         <v/>
       </c>
-      <c r="BU4" s="160" t="str">
-        <f>IF(SUM($BN4)=0,"",SUM($BV4)/$BN4)</f>
+      <c r="BW4" s="160" t="str">
+        <f>IF(SUM($BN4)=0,"",SUM($BX4)/$BN4)</f>
         <v/>
       </c>
-      <c r="BV4" s="101">
-        <f>SUBTOTAL(109,BV$15:INDEX(BV:BV,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+      <c r="BX4" s="101">
+        <f>SUBTOTAL(109,BX$15:INDEX(BX:BX,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="BW4" s="101">
-        <f>SUBTOTAL(109,BW$15:INDEX(BW:BW,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+      <c r="BY4" s="101">
+        <f>SUBTOTAL(109,BY$15:INDEX(BY:BY,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="BX4" s="168"/>
-      <c r="BY4" s="168" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CA4)/$BZ4)</f>
+      <c r="BZ4" s="168"/>
+      <c r="CA4" s="168" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CC4)/$CB4)</f>
         <v/>
       </c>
-      <c r="BZ4" s="103">
-        <f>SUBTOTAL(109,BZ$15:INDEX(BZ:BZ,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
-        <v>0</v>
-      </c>
-      <c r="CA4" s="103">
-        <f>SUBTOTAL(109,CA$15:INDEX(CA:CA,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
-        <v>0</v>
-      </c>
-      <c r="CB4" s="86">
+      <c r="CB4" s="103">
         <f>SUBTOTAL(109,CB$15:INDEX(CB:CB,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="CC4" s="134">
+      <c r="CC4" s="103">
         <f>SUBTOTAL(109,CC$15:INDEX(CC:CC,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="CD4" s="71">
+      <c r="CD4" s="86">
         <f>SUBTOTAL(109,CD$15:INDEX(CD:CD,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="CE4" s="71">
+      <c r="CE4" s="134">
         <f>SUBTOTAL(109,CE$15:INDEX(CE:CE,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
@@ -42853,57 +42903,57 @@
         <f>SUBTOTAL(109,CF$15:INDEX(CF:CF,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="CG4" s="103">
+      <c r="CG4" s="71">
         <f>SUBTOTAL(109,CG$15:INDEX(CG:CG,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="CH4" s="377" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CA4)/$BZ4)</f>
+      <c r="CH4" s="71">
+        <f>SUBTOTAL(109,CH$15:INDEX(CH:CH,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+        <v>0</v>
+      </c>
+      <c r="CI4" s="103">
+        <f>SUBTOTAL(109,CI$15:INDEX(CI:CI,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+        <v>0</v>
+      </c>
+      <c r="CJ4" s="377" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CC4)/$CB4)</f>
         <v/>
       </c>
-      <c r="CI4" s="378" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CB4)/$BZ4)</f>
+      <c r="CK4" s="378" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CD4)/$CB4)</f>
         <v/>
       </c>
-      <c r="CJ4" s="378" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CC4)/$BZ4)</f>
+      <c r="CL4" s="378" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CE4)/$CB4)</f>
         <v/>
       </c>
-      <c r="CK4" s="378" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CD4)/$BZ4)</f>
+      <c r="CM4" s="378" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CF4)/$CB4)</f>
         <v/>
       </c>
-      <c r="CL4" s="378" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CE4)/$BZ4)</f>
+      <c r="CN4" s="378" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CG4)/$CB4)</f>
         <v/>
       </c>
-      <c r="CM4" s="378" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CF4)/$BZ4)</f>
+      <c r="CO4" s="378" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CH4)/$CB4)</f>
         <v/>
       </c>
-      <c r="CN4" s="378" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CG4)/$BZ4)</f>
+      <c r="CP4" s="378" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CI4)/$CB4)</f>
         <v/>
       </c>
-      <c r="CO4" s="160" t="str">
-        <f>IF(SUM($CA4)=0,"",SUM($CR4)/$CA4)</f>
+      <c r="CQ4" s="160" t="str">
+        <f>IF(SUM($CC4)=0,"",SUM($CT4)/$CC4)</f>
         <v/>
       </c>
-      <c r="CP4" s="50" t="str">
-        <f>IF(SUM($CS4,$CR4)=0,"",SUM($CR4)/SUM($CS4,$CR4))</f>
+      <c r="CR4" s="50" t="str">
+        <f>IF(SUM($CU4,$CT4)=0,"",SUM($CT4)/SUM($CU4,$CT4))</f>
         <v/>
       </c>
-      <c r="CQ4" s="50" t="str">
-        <f>IF(SUM($CT4,$CU4)=0,"",SUM($CT4)/SUM($CT4,$CU4))</f>
+      <c r="CS4" s="50" t="str">
+        <f>IF(SUM($CV4,$CW4)=0,"",SUM($CV4)/SUM($CV4,$CW4))</f>
         <v/>
-      </c>
-      <c r="CR4" s="71">
-        <f>SUBTOTAL(109,CR$15:INDEX(CR:CR,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
-        <v>0</v>
-      </c>
-      <c r="CS4" s="71">
-        <f>SUBTOTAL(109,CS$15:INDEX(CS:CS,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
-        <v>0</v>
       </c>
       <c r="CT4" s="71">
         <f>SUBTOTAL(109,CT$15:INDEX(CT:CT,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
@@ -42913,22 +42963,30 @@
         <f>SUBTOTAL(109,CU$15:INDEX(CU:CU,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="CV4" s="50" t="str">
-        <f>IF(SUM($BZ4)=0,"",SUM($CR4,$CT4)/$BZ4)</f>
-        <v/>
-      </c>
-      <c r="CW4" s="449">
+      <c r="CV4" s="71">
+        <f>SUBTOTAL(109,CV$15:INDEX(CV:CV,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+        <v>0</v>
+      </c>
+      <c r="CW4" s="71">
         <f>SUBTOTAL(109,CW$15:INDEX(CW:CW,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
         <v>0</v>
       </c>
-      <c r="CX4"/>
-      <c r="CY4"/>
+      <c r="CX4" s="50" t="str">
+        <f>IF(SUM($CB4)=0,"",SUM($CT4,$CV4)/$CB4)</f>
+        <v/>
+      </c>
+      <c r="CY4" s="449">
+        <f>SUBTOTAL(109,CY$15:INDEX(CY:CY,COUNTA($B:$B)+14-COUNTA($B$1:$B$14)))</f>
+        <v>0</v>
+      </c>
       <c r="CZ4"/>
       <c r="DA4"/>
       <c r="DB4"/>
       <c r="DC4"/>
-    </row>
-    <row r="5" spans="1:107" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD4"/>
+      <c r="DE4"/>
+    </row>
+    <row r="5" spans="1:109" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
         <v>99</v>
       </c>
@@ -43076,13 +43134,13 @@
       <c r="AW5" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="AX5" s="273" t="s">
+      <c r="AX5" s="248" t="s">
         <v>99</v>
       </c>
-      <c r="AY5" s="97" t="s">
+      <c r="AY5" s="273" t="s">
         <v>99</v>
       </c>
-      <c r="AZ5" s="248" t="s">
+      <c r="AZ5" s="97" t="s">
         <v>99</v>
       </c>
       <c r="BA5" s="169" t="s">
@@ -43136,37 +43194,37 @@
       <c r="BQ5" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="BR5" s="122" t="s">
+      <c r="BR5" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="BS5" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="BT5" s="122" t="s">
         <v>108</v>
       </c>
-      <c r="BS5" s="169" t="s">
+      <c r="BU5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="BT5" s="366" t="s">
+      <c r="BV5" s="366" t="s">
         <v>99</v>
       </c>
-      <c r="BU5" s="161" t="s">
+      <c r="BW5" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="BV5" s="75" t="s">
+      <c r="BX5" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="BW5" s="75" t="s">
+      <c r="BY5" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="BX5" s="169" t="s">
+      <c r="BZ5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="BY5" s="169" t="s">
+      <c r="CA5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="BZ5" s="104" t="s">
-        <v>99</v>
-      </c>
-      <c r="CA5" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="CB5" s="72" t="s">
+      <c r="CB5" s="104" t="s">
         <v>99</v>
       </c>
       <c r="CC5" s="72" t="s">
@@ -43184,13 +43242,13 @@
       <c r="CG5" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="CH5" s="161" t="s">
+      <c r="CH5" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="CI5" s="248" t="s">
+      <c r="CI5" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="CJ5" s="248" t="s">
+      <c r="CJ5" s="161" t="s">
         <v>99</v>
       </c>
       <c r="CK5" s="248" t="s">
@@ -43205,20 +43263,20 @@
       <c r="CN5" s="248" t="s">
         <v>99</v>
       </c>
-      <c r="CO5" s="161" t="s">
+      <c r="CO5" s="248" t="s">
         <v>99</v>
       </c>
-      <c r="CP5" s="36" t="s">
+      <c r="CP5" s="248" t="s">
         <v>99</v>
       </c>
-      <c r="CQ5" s="36" t="s">
+      <c r="CQ5" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="CR5" s="72" t="s">
-        <v>110</v>
-      </c>
-      <c r="CS5" s="72" t="s">
-        <v>110</v>
+      <c r="CR5" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="CS5" s="36" t="s">
+        <v>99</v>
       </c>
       <c r="CT5" s="72" t="s">
         <v>110</v>
@@ -43226,20 +43284,26 @@
       <c r="CU5" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="CV5" s="36" t="s">
+      <c r="CV5" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="CW5" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="CX5" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="CW5" s="450" t="s">
+      <c r="CY5" s="450" t="s">
         <v>108</v>
       </c>
-      <c r="CX5"/>
-      <c r="CY5"/>
       <c r="CZ5"/>
       <c r="DA5"/>
       <c r="DB5"/>
       <c r="DC5"/>
-    </row>
-    <row r="6" spans="1:107" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD5"/>
+      <c r="DE5"/>
+    </row>
+    <row r="6" spans="1:109" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>201</v>
       </c>
@@ -43387,14 +43451,14 @@
       <c r="AW6" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="AX6" s="273" t="s">
+      <c r="AX6" s="248" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY6" s="273" t="s">
         <v>94</v>
       </c>
-      <c r="AY6" s="97" t="s">
+      <c r="AZ6" s="97" t="s">
         <v>94</v>
-      </c>
-      <c r="AZ6" s="248" t="s">
-        <v>113</v>
       </c>
       <c r="BA6" s="169" t="s">
         <v>94</v>
@@ -43447,37 +43511,37 @@
       <c r="BQ6" s="104" t="s">
         <v>93</v>
       </c>
-      <c r="BR6" s="122" t="s">
+      <c r="BR6" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="BS6" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="BT6" s="122" t="s">
         <v>93</v>
       </c>
-      <c r="BS6" s="169" t="s">
+      <c r="BU6" s="169" t="s">
         <v>94</v>
       </c>
-      <c r="BT6" s="366" t="s">
+      <c r="BV6" s="366" t="s">
         <v>94</v>
       </c>
-      <c r="BU6" s="161" t="s">
+      <c r="BW6" s="161" t="s">
         <v>113</v>
       </c>
-      <c r="BV6" s="75" t="s">
+      <c r="BX6" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="BW6" s="75" t="s">
+      <c r="BY6" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="BX6" s="169" t="s">
+      <c r="BZ6" s="169" t="s">
         <v>112</v>
       </c>
-      <c r="BY6" s="169" t="s">
+      <c r="CA6" s="169" t="s">
         <v>113</v>
       </c>
-      <c r="BZ6" s="104" t="s">
-        <v>94</v>
-      </c>
-      <c r="CA6" s="72" t="s">
-        <v>94</v>
-      </c>
-      <c r="CB6" s="72" t="s">
+      <c r="CB6" s="104" t="s">
         <v>94</v>
       </c>
       <c r="CC6" s="72" t="s">
@@ -43495,13 +43559,13 @@
       <c r="CG6" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="CH6" s="161" t="s">
+      <c r="CH6" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="CI6" s="248" t="s">
+      <c r="CI6" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="CJ6" s="248" t="s">
+      <c r="CJ6" s="161" t="s">
         <v>94</v>
       </c>
       <c r="CK6" s="248" t="s">
@@ -43516,20 +43580,20 @@
       <c r="CN6" s="248" t="s">
         <v>94</v>
       </c>
-      <c r="CO6" s="161" t="s">
+      <c r="CO6" s="248" t="s">
+        <v>94</v>
+      </c>
+      <c r="CP6" s="248" t="s">
+        <v>94</v>
+      </c>
+      <c r="CQ6" s="161" t="s">
         <v>112</v>
       </c>
-      <c r="CP6" s="36" t="s">
+      <c r="CR6" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="CQ6" s="36" t="s">
+      <c r="CS6" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="CR6" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="CS6" s="72" t="s">
-        <v>93</v>
       </c>
       <c r="CT6" s="72" t="s">
         <v>93</v>
@@ -43537,20 +43601,26 @@
       <c r="CU6" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="CV6" s="36" t="s">
+      <c r="CV6" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="CW6" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="CX6" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="CW6" s="450" t="s">
+      <c r="CY6" s="450" t="s">
         <v>93</v>
       </c>
-      <c r="CX6"/>
-      <c r="CY6"/>
       <c r="CZ6"/>
       <c r="DA6"/>
       <c r="DB6"/>
       <c r="DC6"/>
-    </row>
-    <row r="7" spans="1:107" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD6"/>
+      <c r="DE6"/>
+    </row>
+    <row r="7" spans="1:109" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>109</v>
       </c>
@@ -43698,14 +43768,14 @@
       <c r="AW7" s="118" t="s">
         <v>95</v>
       </c>
-      <c r="AX7" s="273" t="s">
+      <c r="AX7" s="248" t="s">
         <v>96</v>
       </c>
-      <c r="AY7" s="97" t="s">
+      <c r="AY7" s="273" t="s">
+        <v>96</v>
+      </c>
+      <c r="AZ7" s="97" t="s">
         <v>95</v>
-      </c>
-      <c r="AZ7" s="248" t="s">
-        <v>96</v>
       </c>
       <c r="BA7" s="169" t="s">
         <v>96</v>
@@ -43758,37 +43828,37 @@
       <c r="BQ7" s="104" t="s">
         <v>95</v>
       </c>
-      <c r="BR7" s="122" t="s">
+      <c r="BR7" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="BS7" s="169" t="s">
+      <c r="BS7" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="BT7" s="122" t="s">
+        <v>95</v>
+      </c>
+      <c r="BU7" s="169" t="s">
         <v>96</v>
       </c>
-      <c r="BT7" s="366" t="s">
+      <c r="BV7" s="366" t="s">
         <v>96</v>
       </c>
-      <c r="BU7" s="161" t="s">
+      <c r="BW7" s="161" t="s">
         <v>96</v>
       </c>
-      <c r="BV7" s="75" t="s">
+      <c r="BX7" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="BW7" s="75" t="s">
+      <c r="BY7" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="BX7" s="169" t="s">
+      <c r="BZ7" s="169" t="s">
         <v>96</v>
       </c>
-      <c r="BY7" s="169" t="s">
+      <c r="CA7" s="169" t="s">
         <v>96</v>
       </c>
-      <c r="BZ7" s="104" t="s">
-        <v>95</v>
-      </c>
-      <c r="CA7" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="CB7" s="72" t="s">
+      <c r="CB7" s="104" t="s">
         <v>95</v>
       </c>
       <c r="CC7" s="72" t="s">
@@ -43806,13 +43876,13 @@
       <c r="CG7" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="CH7" s="161" t="s">
-        <v>96</v>
-      </c>
-      <c r="CI7" s="248" t="s">
-        <v>96</v>
-      </c>
-      <c r="CJ7" s="248" t="s">
+      <c r="CH7" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="CI7" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="CJ7" s="161" t="s">
         <v>96</v>
       </c>
       <c r="CK7" s="248" t="s">
@@ -43827,20 +43897,20 @@
       <c r="CN7" s="248" t="s">
         <v>96</v>
       </c>
-      <c r="CO7" s="161" t="s">
+      <c r="CO7" s="248" t="s">
         <v>96</v>
       </c>
-      <c r="CP7" s="36" t="s">
+      <c r="CP7" s="248" t="s">
         <v>96</v>
       </c>
-      <c r="CQ7" s="36" t="s">
+      <c r="CQ7" s="161" t="s">
         <v>96</v>
       </c>
-      <c r="CR7" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="CS7" s="72" t="s">
-        <v>95</v>
+      <c r="CR7" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="CS7" s="36" t="s">
+        <v>96</v>
       </c>
       <c r="CT7" s="72" t="s">
         <v>95</v>
@@ -43848,20 +43918,26 @@
       <c r="CU7" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="CV7" s="36" t="s">
+      <c r="CV7" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="CW7" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="CX7" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="CW7" s="450" t="s">
+      <c r="CY7" s="450" t="s">
         <v>95</v>
       </c>
-      <c r="CX7"/>
-      <c r="CY7"/>
       <c r="CZ7"/>
       <c r="DA7"/>
       <c r="DB7"/>
       <c r="DC7"/>
-    </row>
-    <row r="8" spans="1:107" s="328" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD7"/>
+      <c r="DE7"/>
+    </row>
+    <row r="8" spans="1:109" s="328" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="329"/>
       <c r="B8" s="329"/>
       <c r="C8" s="329"/>
@@ -43947,9 +44023,9 @@
       </c>
       <c r="AV8" s="331"/>
       <c r="AW8" s="390"/>
-      <c r="AX8" s="393"/>
-      <c r="AY8" s="386"/>
-      <c r="AZ8" s="389"/>
+      <c r="AX8" s="389"/>
+      <c r="AY8" s="393"/>
+      <c r="AZ8" s="386"/>
       <c r="BA8" s="392"/>
       <c r="BB8" s="392"/>
       <c r="BC8" s="389"/>
@@ -43971,56 +44047,58 @@
       <c r="BQ8" s="395" t="s">
         <v>136</v>
       </c>
-      <c r="BR8" s="441" t="s">
+      <c r="BR8" s="386"/>
+      <c r="BS8" s="386"/>
+      <c r="BT8" s="441" t="s">
         <v>295</v>
       </c>
-      <c r="BS8" s="392"/>
-      <c r="BT8" s="394"/>
-      <c r="BU8" s="331"/>
-      <c r="BV8" s="173"/>
-      <c r="BW8" s="173"/>
-      <c r="BX8" s="392"/>
-      <c r="BY8" s="392"/>
-      <c r="BZ8" s="395"/>
-      <c r="CA8" s="395"/>
-      <c r="CB8" s="119"/>
+      <c r="BU8" s="392"/>
+      <c r="BV8" s="394"/>
+      <c r="BW8" s="331"/>
+      <c r="BX8" s="173"/>
+      <c r="BY8" s="173"/>
+      <c r="BZ8" s="392"/>
+      <c r="CA8" s="392"/>
+      <c r="CB8" s="395"/>
       <c r="CC8" s="395"/>
       <c r="CD8" s="119"/>
-      <c r="CE8" s="119"/>
+      <c r="CE8" s="395"/>
       <c r="CF8" s="119"/>
-      <c r="CG8" s="395"/>
-      <c r="CH8" s="331"/>
-      <c r="CI8" s="389"/>
-      <c r="CJ8" s="389"/>
+      <c r="CG8" s="119"/>
+      <c r="CH8" s="119"/>
+      <c r="CI8" s="395"/>
+      <c r="CJ8" s="331"/>
       <c r="CK8" s="389"/>
       <c r="CL8" s="389"/>
       <c r="CM8" s="389"/>
       <c r="CN8" s="389"/>
-      <c r="CO8" s="331"/>
-      <c r="CP8" s="332"/>
-      <c r="CQ8" s="332"/>
-      <c r="CR8" s="119" t="s">
+      <c r="CO8" s="389"/>
+      <c r="CP8" s="389"/>
+      <c r="CQ8" s="331"/>
+      <c r="CR8" s="332"/>
+      <c r="CS8" s="332"/>
+      <c r="CT8" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="CS8" s="119" t="s">
+      <c r="CU8" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="CT8" s="119" t="s">
+      <c r="CV8" s="119" t="s">
         <v>147</v>
       </c>
-      <c r="CU8" s="119" t="s">
+      <c r="CW8" s="119" t="s">
         <v>147</v>
       </c>
-      <c r="CV8" s="332"/>
-      <c r="CW8" s="451"/>
-      <c r="CX8" s="22"/>
-      <c r="CY8" s="22"/>
+      <c r="CX8" s="332"/>
+      <c r="CY8" s="451"/>
       <c r="CZ8" s="22"/>
       <c r="DA8" s="22"/>
       <c r="DB8" s="22"/>
       <c r="DC8" s="22"/>
-    </row>
-    <row r="9" spans="1:107" s="328" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD8" s="22"/>
+      <c r="DE8" s="22"/>
+    </row>
+    <row r="9" spans="1:109" s="328" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="329"/>
       <c r="B9" s="329"/>
       <c r="C9" s="329"/>
@@ -44090,9 +44168,9 @@
       </c>
       <c r="AV9" s="331"/>
       <c r="AW9" s="390"/>
-      <c r="AX9" s="393"/>
-      <c r="AY9" s="386"/>
-      <c r="AZ9" s="389"/>
+      <c r="AX9" s="389"/>
+      <c r="AY9" s="393"/>
+      <c r="AZ9" s="386"/>
       <c r="BA9" s="392"/>
       <c r="BB9" s="392"/>
       <c r="BC9" s="389"/>
@@ -44114,54 +44192,56 @@
       <c r="BQ9" s="395" t="s">
         <v>137</v>
       </c>
-      <c r="BR9" s="441"/>
-      <c r="BS9" s="392"/>
-      <c r="BT9" s="394"/>
-      <c r="BU9" s="331"/>
-      <c r="BV9" s="173"/>
-      <c r="BW9" s="173"/>
-      <c r="BX9" s="392"/>
-      <c r="BY9" s="392"/>
-      <c r="BZ9" s="395"/>
-      <c r="CA9" s="395"/>
-      <c r="CB9" s="119"/>
+      <c r="BR9" s="386"/>
+      <c r="BS9" s="386"/>
+      <c r="BT9" s="441"/>
+      <c r="BU9" s="392"/>
+      <c r="BV9" s="394"/>
+      <c r="BW9" s="331"/>
+      <c r="BX9" s="173"/>
+      <c r="BY9" s="173"/>
+      <c r="BZ9" s="392"/>
+      <c r="CA9" s="392"/>
+      <c r="CB9" s="395"/>
       <c r="CC9" s="395"/>
       <c r="CD9" s="119"/>
-      <c r="CE9" s="119"/>
+      <c r="CE9" s="395"/>
       <c r="CF9" s="119"/>
-      <c r="CG9" s="395"/>
-      <c r="CH9" s="331"/>
-      <c r="CI9" s="389"/>
-      <c r="CJ9" s="389"/>
+      <c r="CG9" s="119"/>
+      <c r="CH9" s="119"/>
+      <c r="CI9" s="395"/>
+      <c r="CJ9" s="331"/>
       <c r="CK9" s="389"/>
       <c r="CL9" s="389"/>
       <c r="CM9" s="389"/>
       <c r="CN9" s="389"/>
-      <c r="CO9" s="331"/>
-      <c r="CP9" s="332"/>
-      <c r="CQ9" s="332"/>
-      <c r="CR9" s="119" t="s">
+      <c r="CO9" s="389"/>
+      <c r="CP9" s="389"/>
+      <c r="CQ9" s="331"/>
+      <c r="CR9" s="332"/>
+      <c r="CS9" s="332"/>
+      <c r="CT9" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="CS9" s="119" t="s">
+      <c r="CU9" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="CT9" s="119" t="s">
+      <c r="CV9" s="119" t="s">
         <v>148</v>
       </c>
-      <c r="CU9" s="119" t="s">
+      <c r="CW9" s="119" t="s">
         <v>148</v>
       </c>
-      <c r="CV9" s="396"/>
-      <c r="CW9" s="451"/>
-      <c r="CX9" s="22"/>
-      <c r="CY9" s="22"/>
+      <c r="CX9" s="396"/>
+      <c r="CY9" s="451"/>
       <c r="CZ9" s="22"/>
       <c r="DA9" s="22"/>
       <c r="DB9" s="22"/>
       <c r="DC9" s="22"/>
-    </row>
-    <row r="10" spans="1:107" s="328" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD9" s="22"/>
+      <c r="DE9" s="22"/>
+    </row>
+    <row r="10" spans="1:109" s="328" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="329"/>
       <c r="B10" s="329"/>
       <c r="C10" s="329"/>
@@ -44243,9 +44323,9 @@
       </c>
       <c r="AV10" s="331"/>
       <c r="AW10" s="390"/>
-      <c r="AX10" s="393"/>
-      <c r="AY10" s="386"/>
-      <c r="AZ10" s="389"/>
+      <c r="AX10" s="389"/>
+      <c r="AY10" s="393"/>
+      <c r="AZ10" s="386"/>
       <c r="BA10" s="392"/>
       <c r="BB10" s="392"/>
       <c r="BC10" s="389"/>
@@ -44267,56 +44347,58 @@
       <c r="BQ10" s="395" t="s">
         <v>105</v>
       </c>
-      <c r="BR10" s="441" t="s">
+      <c r="BR10" s="386"/>
+      <c r="BS10" s="386"/>
+      <c r="BT10" s="441" t="s">
         <v>105</v>
       </c>
-      <c r="BS10" s="392"/>
-      <c r="BT10" s="394"/>
-      <c r="BU10" s="331"/>
-      <c r="BV10" s="173"/>
-      <c r="BW10" s="173"/>
-      <c r="BX10" s="392"/>
-      <c r="BY10" s="392"/>
-      <c r="BZ10" s="395"/>
-      <c r="CA10" s="395"/>
-      <c r="CB10" s="119"/>
+      <c r="BU10" s="392"/>
+      <c r="BV10" s="394"/>
+      <c r="BW10" s="331"/>
+      <c r="BX10" s="173"/>
+      <c r="BY10" s="173"/>
+      <c r="BZ10" s="392"/>
+      <c r="CA10" s="392"/>
+      <c r="CB10" s="395"/>
       <c r="CC10" s="395"/>
       <c r="CD10" s="119"/>
-      <c r="CE10" s="119"/>
+      <c r="CE10" s="395"/>
       <c r="CF10" s="119"/>
-      <c r="CG10" s="395"/>
-      <c r="CH10" s="331"/>
-      <c r="CI10" s="389"/>
-      <c r="CJ10" s="389"/>
+      <c r="CG10" s="119"/>
+      <c r="CH10" s="119"/>
+      <c r="CI10" s="395"/>
+      <c r="CJ10" s="331"/>
       <c r="CK10" s="389"/>
       <c r="CL10" s="389"/>
       <c r="CM10" s="389"/>
       <c r="CN10" s="389"/>
-      <c r="CO10" s="331"/>
-      <c r="CP10" s="332"/>
-      <c r="CQ10" s="332"/>
-      <c r="CR10" s="119" t="s">
-        <v>103</v>
-      </c>
-      <c r="CS10" s="119" t="s">
-        <v>104</v>
-      </c>
+      <c r="CO10" s="389"/>
+      <c r="CP10" s="389"/>
+      <c r="CQ10" s="331"/>
+      <c r="CR10" s="332"/>
+      <c r="CS10" s="332"/>
       <c r="CT10" s="119" t="s">
         <v>103</v>
       </c>
       <c r="CU10" s="119" t="s">
         <v>104</v>
       </c>
-      <c r="CV10" s="332"/>
-      <c r="CW10" s="451"/>
-      <c r="CX10" s="22"/>
-      <c r="CY10" s="22"/>
+      <c r="CV10" s="119" t="s">
+        <v>103</v>
+      </c>
+      <c r="CW10" s="119" t="s">
+        <v>104</v>
+      </c>
+      <c r="CX10" s="332"/>
+      <c r="CY10" s="451"/>
       <c r="CZ10" s="22"/>
       <c r="DA10" s="22"/>
       <c r="DB10" s="22"/>
       <c r="DC10" s="22"/>
-    </row>
-    <row r="11" spans="1:107" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD10" s="22"/>
+      <c r="DE10" s="22"/>
+    </row>
+    <row r="11" spans="1:109" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42"/>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
@@ -44454,13 +44536,13 @@
       <c r="AW11" s="118" t="s">
         <v>688</v>
       </c>
-      <c r="AX11" s="273" t="s">
+      <c r="AX11" s="248" t="s">
         <v>688</v>
       </c>
-      <c r="AY11" s="97" t="s">
+      <c r="AY11" s="273" t="s">
         <v>688</v>
       </c>
-      <c r="AZ11" s="248" t="s">
+      <c r="AZ11" s="97" t="s">
         <v>688</v>
       </c>
       <c r="BA11" s="169" t="s">
@@ -44514,88 +44596,88 @@
       <c r="BQ11" s="104" t="s">
         <v>203</v>
       </c>
-      <c r="BR11" s="122" t="s">
+      <c r="BR11" s="97" t="s">
         <v>203</v>
       </c>
-      <c r="BS11" s="169" t="s">
+      <c r="BS11" s="97" t="s">
         <v>203</v>
       </c>
-      <c r="BT11" s="366" t="s">
+      <c r="BT11" s="122" t="s">
         <v>203</v>
       </c>
-      <c r="BU11" s="161" t="s">
+      <c r="BU11" s="169" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV11" s="366" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW11" s="161" t="s">
         <v>688</v>
       </c>
-      <c r="BV11" s="75" t="s">
+      <c r="BX11" s="75" t="s">
         <v>688</v>
       </c>
-      <c r="BW11" s="75" t="s">
+      <c r="BY11" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="BX11" s="169" t="s">
+      <c r="BZ11" s="169" t="s">
         <v>688</v>
       </c>
-      <c r="BY11" s="169" t="s">
+      <c r="CA11" s="169" t="s">
         <v>688</v>
       </c>
-      <c r="BZ11" s="104" t="s">
+      <c r="CB11" s="104" t="s">
         <v>203</v>
       </c>
-      <c r="CA11" s="104" t="s">
+      <c r="CC11" s="104" t="s">
         <v>688</v>
       </c>
-      <c r="CB11" s="72" t="s">
+      <c r="CD11" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="CC11" s="104" t="s">
+      <c r="CE11" s="104" t="s">
         <v>204</v>
       </c>
-      <c r="CD11" s="72" t="s">
+      <c r="CF11" s="72" t="s">
         <v>688</v>
       </c>
-      <c r="CE11" s="72" t="s">
+      <c r="CG11" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="CF11" s="72" t="s">
+      <c r="CH11" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="CG11" s="104" t="s">
+      <c r="CI11" s="104" t="s">
         <v>688</v>
       </c>
-      <c r="CH11" s="161" t="s">
+      <c r="CJ11" s="161" t="s">
         <v>688</v>
       </c>
-      <c r="CI11" s="248" t="s">
+      <c r="CK11" s="248" t="s">
         <v>204</v>
       </c>
-      <c r="CJ11" s="248" t="s">
+      <c r="CL11" s="248" t="s">
         <v>204</v>
       </c>
-      <c r="CK11" s="248" t="s">
+      <c r="CM11" s="248" t="s">
         <v>688</v>
       </c>
-      <c r="CL11" s="248" t="s">
+      <c r="CN11" s="248" t="s">
         <v>206</v>
       </c>
-      <c r="CM11" s="248" t="s">
+      <c r="CO11" s="248" t="s">
         <v>38</v>
       </c>
-      <c r="CN11" s="248" t="s">
+      <c r="CP11" s="248" t="s">
         <v>688</v>
       </c>
-      <c r="CO11" s="161" t="s">
+      <c r="CQ11" s="161" t="s">
         <v>688</v>
       </c>
-      <c r="CP11" s="36" t="s">
+      <c r="CR11" s="36" t="s">
         <v>688</v>
       </c>
-      <c r="CQ11" s="36" t="s">
-        <v>688</v>
-      </c>
-      <c r="CR11" s="72" t="s">
-        <v>688</v>
-      </c>
-      <c r="CS11" s="72" t="s">
+      <c r="CS11" s="36" t="s">
         <v>688</v>
       </c>
       <c r="CT11" s="72" t="s">
@@ -44604,20 +44686,26 @@
       <c r="CU11" s="72" t="s">
         <v>688</v>
       </c>
-      <c r="CV11" s="36" t="s">
+      <c r="CV11" s="72" t="s">
         <v>688</v>
       </c>
-      <c r="CW11" s="450" t="s">
+      <c r="CW11" s="72" t="s">
+        <v>688</v>
+      </c>
+      <c r="CX11" s="36" t="s">
+        <v>688</v>
+      </c>
+      <c r="CY11" s="450" t="s">
         <v>203</v>
       </c>
-      <c r="CX11"/>
-      <c r="CY11"/>
       <c r="CZ11"/>
       <c r="DA11"/>
       <c r="DB11"/>
       <c r="DC11"/>
-    </row>
-    <row r="12" spans="1:107" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD11"/>
+      <c r="DE11"/>
+    </row>
+    <row r="12" spans="1:109" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="42"/>
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
@@ -44755,13 +44843,13 @@
       <c r="AW12" s="118" t="s">
         <v>202</v>
       </c>
-      <c r="AX12" s="273" t="s">
+      <c r="AX12" s="248" t="s">
         <v>202</v>
       </c>
-      <c r="AY12" s="97" t="s">
+      <c r="AY12" s="273" t="s">
         <v>202</v>
       </c>
-      <c r="AZ12" s="248" t="s">
+      <c r="AZ12" s="97" t="s">
         <v>202</v>
       </c>
       <c r="BA12" s="169" t="s">
@@ -44815,88 +44903,88 @@
       <c r="BQ12" s="104" t="s">
         <v>202</v>
       </c>
-      <c r="BR12" s="122" t="s">
+      <c r="BR12" s="97" t="s">
         <v>202</v>
       </c>
-      <c r="BS12" s="169" t="s">
+      <c r="BS12" s="97" t="s">
         <v>202</v>
       </c>
-      <c r="BT12" s="366" t="s">
+      <c r="BT12" s="122" t="s">
         <v>202</v>
       </c>
-      <c r="BU12" s="161" t="s">
+      <c r="BU12" s="169" t="s">
         <v>202</v>
       </c>
-      <c r="BV12" s="75" t="s">
+      <c r="BV12" s="366" t="s">
         <v>202</v>
       </c>
-      <c r="BW12" s="75" t="s">
+      <c r="BW12" s="161" t="s">
         <v>202</v>
       </c>
-      <c r="BX12" s="169" t="s">
+      <c r="BX12" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="BY12" s="169" t="s">
+      <c r="BY12" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="BZ12" s="104" t="s">
+      <c r="BZ12" s="169" t="s">
         <v>202</v>
       </c>
-      <c r="CA12" s="104" t="s">
+      <c r="CA12" s="169" t="s">
         <v>202</v>
       </c>
-      <c r="CB12" s="72" t="s">
+      <c r="CB12" s="104" t="s">
+        <v>202</v>
+      </c>
+      <c r="CC12" s="104" t="s">
+        <v>202</v>
+      </c>
+      <c r="CD12" s="72" t="s">
         <v>689</v>
       </c>
-      <c r="CC12" s="104" t="s">
+      <c r="CE12" s="104" t="s">
         <v>689</v>
-      </c>
-      <c r="CD12" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="CE12" s="72" t="s">
-        <v>690</v>
       </c>
       <c r="CF12" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="CG12" s="104" t="s">
+      <c r="CG12" s="72" t="s">
+        <v>690</v>
+      </c>
+      <c r="CH12" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="CH12" s="161" t="s">
+      <c r="CI12" s="104" t="s">
         <v>202</v>
       </c>
-      <c r="CI12" s="248" t="s">
+      <c r="CJ12" s="161" t="s">
+        <v>202</v>
+      </c>
+      <c r="CK12" s="248" t="s">
         <v>689</v>
       </c>
-      <c r="CJ12" s="248" t="s">
+      <c r="CL12" s="248" t="s">
         <v>689</v>
-      </c>
-      <c r="CK12" s="248" t="s">
-        <v>202</v>
-      </c>
-      <c r="CL12" s="248" t="s">
-        <v>690</v>
       </c>
       <c r="CM12" s="248" t="s">
         <v>202</v>
       </c>
       <c r="CN12" s="248" t="s">
+        <v>690</v>
+      </c>
+      <c r="CO12" s="248" t="s">
         <v>202</v>
       </c>
-      <c r="CO12" s="161" t="s">
+      <c r="CP12" s="248" t="s">
         <v>202</v>
       </c>
-      <c r="CP12" s="36" t="s">
+      <c r="CQ12" s="161" t="s">
         <v>202</v>
       </c>
-      <c r="CQ12" s="36" t="s">
+      <c r="CR12" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="CR12" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="CS12" s="72" t="s">
+      <c r="CS12" s="36" t="s">
         <v>202</v>
       </c>
       <c r="CT12" s="72" t="s">
@@ -44905,20 +44993,26 @@
       <c r="CU12" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="CV12" s="36" t="s">
+      <c r="CV12" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="CW12" s="450" t="s">
+      <c r="CW12" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="CX12"/>
-      <c r="CY12"/>
+      <c r="CX12" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="CY12" s="450" t="s">
+        <v>202</v>
+      </c>
       <c r="CZ12"/>
       <c r="DA12"/>
       <c r="DB12"/>
       <c r="DC12"/>
-    </row>
-    <row r="13" spans="1:107" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD12"/>
+      <c r="DE12"/>
+    </row>
+    <row r="13" spans="1:109" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="42"/>
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
@@ -44968,9 +45062,9 @@
       <c r="AU13" s="104"/>
       <c r="AV13" s="161"/>
       <c r="AW13" s="118"/>
-      <c r="AX13" s="273"/>
-      <c r="AY13" s="97"/>
-      <c r="AZ13" s="248"/>
+      <c r="AX13" s="248"/>
+      <c r="AY13" s="273"/>
+      <c r="AZ13" s="97"/>
       <c r="BA13" s="169"/>
       <c r="BB13" s="169"/>
       <c r="BC13" s="248"/>
@@ -44988,46 +45082,48 @@
       <c r="BO13" s="161"/>
       <c r="BP13" s="248"/>
       <c r="BQ13" s="104"/>
-      <c r="BR13" s="122"/>
-      <c r="BS13" s="169"/>
-      <c r="BT13" s="366"/>
-      <c r="BU13" s="161"/>
-      <c r="BV13" s="75"/>
-      <c r="BW13" s="75"/>
-      <c r="BX13" s="169"/>
-      <c r="BY13" s="169"/>
-      <c r="BZ13" s="104"/>
-      <c r="CA13" s="104"/>
-      <c r="CB13" s="72"/>
+      <c r="BR13" s="97"/>
+      <c r="BS13" s="97"/>
+      <c r="BT13" s="122"/>
+      <c r="BU13" s="169"/>
+      <c r="BV13" s="366"/>
+      <c r="BW13" s="161"/>
+      <c r="BX13" s="75"/>
+      <c r="BY13" s="75"/>
+      <c r="BZ13" s="169"/>
+      <c r="CA13" s="169"/>
+      <c r="CB13" s="104"/>
       <c r="CC13" s="104"/>
       <c r="CD13" s="72"/>
-      <c r="CE13" s="72"/>
+      <c r="CE13" s="104"/>
       <c r="CF13" s="72"/>
-      <c r="CG13" s="104"/>
-      <c r="CH13" s="161"/>
-      <c r="CI13" s="248"/>
-      <c r="CJ13" s="248"/>
+      <c r="CG13" s="72"/>
+      <c r="CH13" s="72"/>
+      <c r="CI13" s="104"/>
+      <c r="CJ13" s="161"/>
       <c r="CK13" s="248"/>
       <c r="CL13" s="248"/>
       <c r="CM13" s="248"/>
       <c r="CN13" s="248"/>
-      <c r="CO13" s="161"/>
-      <c r="CP13" s="36"/>
-      <c r="CQ13" s="36"/>
-      <c r="CR13" s="72"/>
-      <c r="CS13" s="72"/>
+      <c r="CO13" s="248"/>
+      <c r="CP13" s="248"/>
+      <c r="CQ13" s="161"/>
+      <c r="CR13" s="36"/>
+      <c r="CS13" s="36"/>
       <c r="CT13" s="72"/>
       <c r="CU13" s="72"/>
-      <c r="CV13" s="36"/>
-      <c r="CW13" s="450"/>
-      <c r="CX13"/>
-      <c r="CY13"/>
+      <c r="CV13" s="72"/>
+      <c r="CW13" s="72"/>
+      <c r="CX13" s="36"/>
+      <c r="CY13" s="450"/>
       <c r="CZ13"/>
       <c r="DA13"/>
       <c r="DB13"/>
       <c r="DC13"/>
-    </row>
-    <row r="14" spans="1:107" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DD13"/>
+      <c r="DE13"/>
+    </row>
+    <row r="14" spans="1:109" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="s">
         <v>587</v>
       </c>
@@ -45173,16 +45269,16 @@
         <v>507</v>
       </c>
       <c r="AW14" s="176" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="AX14" s="249" t="s">
+        <v>1196</v>
+      </c>
+      <c r="AY14" s="249" t="s">
         <v>501</v>
       </c>
-      <c r="AY14" s="176" t="s">
-        <v>1198</v>
-      </c>
-      <c r="AZ14" s="249" t="s">
-        <v>1199</v>
+      <c r="AZ14" s="176" t="s">
+        <v>1195</v>
       </c>
       <c r="BA14" s="170" t="s">
         <v>504</v>
@@ -45203,25 +45299,25 @@
         <v>1109</v>
       </c>
       <c r="BG14" s="362" t="s">
+        <v>1197</v>
+      </c>
+      <c r="BH14" s="212" t="s">
         <v>1200</v>
       </c>
-      <c r="BH14" s="212" t="s">
-        <v>1203</v>
-      </c>
       <c r="BI14" s="212" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="BJ14" s="218" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="BK14" s="99" t="s">
         <v>1140</v>
       </c>
       <c r="BL14" s="218" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="BM14" s="369" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="BN14" s="218" t="s">
         <v>318</v>
@@ -45235,104 +45331,110 @@
       <c r="BQ14" s="99" t="s">
         <v>317</v>
       </c>
-      <c r="BR14" s="442" t="s">
+      <c r="BR14" s="478" t="s">
+        <v>1216</v>
+      </c>
+      <c r="BS14" s="478" t="s">
+        <v>1217</v>
+      </c>
+      <c r="BT14" s="442" t="s">
         <v>963</v>
       </c>
-      <c r="BS14" s="249" t="s">
+      <c r="BU14" s="249" t="s">
+        <v>1203</v>
+      </c>
+      <c r="BV14" s="362" t="s">
+        <v>1204</v>
+      </c>
+      <c r="BW14" s="162" t="s">
+        <v>1205</v>
+      </c>
+      <c r="BX14" s="106" t="s">
+        <v>480</v>
+      </c>
+      <c r="BY14" s="106" t="s">
         <v>1206</v>
       </c>
-      <c r="BT14" s="362" t="s">
-        <v>1207</v>
-      </c>
-      <c r="BU14" s="162" t="s">
-        <v>1208</v>
-      </c>
-      <c r="BV14" s="106" t="s">
-        <v>480</v>
-      </c>
-      <c r="BW14" s="106" t="s">
-        <v>1209</v>
-      </c>
-      <c r="BX14" s="170" t="s">
+      <c r="BZ14" s="170" t="s">
         <v>967</v>
       </c>
-      <c r="BY14" s="170" t="s">
+      <c r="CA14" s="170" t="s">
         <v>976</v>
       </c>
-      <c r="BZ14" s="99" t="s">
+      <c r="CB14" s="99" t="s">
         <v>567</v>
       </c>
-      <c r="CA14" s="99" t="s">
+      <c r="CC14" s="99" t="s">
         <v>575</v>
       </c>
-      <c r="CB14" s="385" t="s">
+      <c r="CD14" s="385" t="s">
         <v>371</v>
       </c>
-      <c r="CC14" s="385" t="s">
+      <c r="CE14" s="385" t="s">
         <v>373</v>
       </c>
-      <c r="CD14" s="172" t="s">
+      <c r="CF14" s="172" t="s">
         <v>369</v>
       </c>
-      <c r="CE14" s="172" t="s">
+      <c r="CG14" s="172" t="s">
         <v>375</v>
       </c>
-      <c r="CF14" s="172" t="s">
+      <c r="CH14" s="172" t="s">
         <v>526</v>
       </c>
-      <c r="CG14" s="99" t="s">
+      <c r="CI14" s="99" t="s">
         <v>573</v>
       </c>
-      <c r="CH14" s="162" t="s">
+      <c r="CJ14" s="162" t="s">
         <v>574</v>
       </c>
-      <c r="CI14" s="379" t="s">
+      <c r="CK14" s="379" t="s">
         <v>519</v>
       </c>
-      <c r="CJ14" s="379" t="s">
+      <c r="CL14" s="379" t="s">
         <v>518</v>
       </c>
-      <c r="CK14" s="379" t="s">
+      <c r="CM14" s="379" t="s">
         <v>576</v>
       </c>
-      <c r="CL14" s="379" t="s">
+      <c r="CN14" s="379" t="s">
         <v>577</v>
       </c>
-      <c r="CM14" s="379" t="s">
+      <c r="CO14" s="379" t="s">
         <v>578</v>
       </c>
-      <c r="CN14" s="379" t="s">
+      <c r="CP14" s="379" t="s">
         <v>579</v>
       </c>
-      <c r="CO14" s="355" t="s">
+      <c r="CQ14" s="355" t="s">
         <v>337</v>
       </c>
-      <c r="CP14" s="209" t="s">
+      <c r="CR14" s="209" t="s">
         <v>338</v>
       </c>
-      <c r="CQ14" s="209" t="s">
+      <c r="CS14" s="209" t="s">
         <v>339</v>
       </c>
-      <c r="CR14" s="92" t="s">
+      <c r="CT14" s="92" t="s">
         <v>340</v>
       </c>
-      <c r="CS14" s="92" t="s">
+      <c r="CU14" s="92" t="s">
         <v>341</v>
       </c>
-      <c r="CT14" s="92" t="s">
+      <c r="CV14" s="92" t="s">
         <v>342</v>
       </c>
-      <c r="CU14" s="92" t="s">
+      <c r="CW14" s="92" t="s">
         <v>343</v>
       </c>
-      <c r="CV14" s="209" t="s">
+      <c r="CX14" s="209" t="s">
         <v>975</v>
       </c>
-      <c r="CW14" s="250" t="s">
+      <c r="CY14" s="250" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="15" spans="1:107" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:109" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="42"/>
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
@@ -45487,17 +45589,17 @@
         <f>IF(OR(LEFT($B15,4)="_Mil",$C15="&lt;01"),"",SUM($H15)-SUM($P15))</f>
         <v>0</v>
       </c>
-      <c r="AX15" s="273" t="str">
+      <c r="AX15" s="248">
+        <f>IF($C15="&lt;01","",MAX(95%,SUM($AV15)))</f>
+        <v>0.95</v>
+      </c>
+      <c r="AY15" s="273" t="str">
         <f>IF(OR(LEFT($B15,4)="_Mil",$C15="&lt;01",SUM($P15)=0),"",IF(SUM($T15)=0,SUM($R15),$T15)/$P15)</f>
         <v/>
       </c>
-      <c r="AY15" s="118">
+      <c r="AZ15" s="118">
         <f>IF(OR(LEFT($B15,4)="_Mil",$C15="&lt;01"),"",SUM($P15)-IF(SUM($T15)=0,SUM($R15),$T15))</f>
         <v>0</v>
-      </c>
-      <c r="AZ15" s="248">
-        <f>IF($C15="&lt;01","",MAX(95%*95%,SUM($AV15)))</f>
-        <v>0.90249999999999997</v>
       </c>
       <c r="BA15" s="171" t="str">
         <f>IF(OR(SUM($Z15)=0,$C15="&lt;01"),"",SUM($AA15)/$Z15)</f>
@@ -45508,7 +45610,7 @@
         <v/>
       </c>
       <c r="BC15" s="356">
-        <f>IF($C15="&lt;01","",MIN(MAX(95%,$AX15,$BB15,$BA15),1))</f>
+        <f>IF($C15="&lt;01","",MIN(MAX(95%,$AY15,$BB15,$BA15),1))</f>
         <v>0.95</v>
       </c>
       <c r="BD15" s="356">
@@ -45528,7 +45630,7 @@
         <v>1</v>
       </c>
       <c r="BH15" s="217" t="str">
-        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$N:$N,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(AND($AK15="",LEFT($B15,4)&lt;&gt;"_Mil"),HYPERLINK("#Cascade!AK"&amp;ROW(AK15),"&lt;- Add PEPFAR Contribution %"),IF($AZ15="",HYPERLINK("#Cascade!AZ"&amp;ROW(AZ15),"&lt;- Add % New Infections Diagnosed &amp; Linked"),IF($BC15="",HYPERLINK("#Cascade!BC"&amp;ROW(BC15),"&lt;- Add Linkage"),HYPERLINK("",ROUND(SUM($N15)*IF(LEFT($B15,4)="_Mil",1,$AK15)*$AZ15*$BC15,0))))))</f>
+        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$N:$N,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(AND($AK15="",LEFT($B15,4)&lt;&gt;"_Mil"),HYPERLINK("#Cascade!AK"&amp;ROW(AK15),"&lt;- Add PEPFAR Contribution %"),IF($AX15="",HYPERLINK("#Cascade!AZ"&amp;ROW(AX15),"&lt;- Add % New Infections Diagnosed &amp; Linked"),IF($BC15="",HYPERLINK("#Cascade!BC"&amp;ROW(BC15),"&lt;- Add Linkage"),HYPERLINK("",ROUND(SUM($N15)*IF(LEFT($B15,4)="_Mil",1,$AK15)*$AX15*$BC15,0))))))</f>
         <v>&lt;- Add PEPFAR Contribution %</v>
       </c>
       <c r="BI15" s="217">
@@ -45567,261 +45669,264 @@
         <f>IF(AND(LEFT($B15,4)="_Mil",SUM($AP15)=0),"",ROUND(IF($C15="&lt;01",IFERROR(INDEX(EID!P:$P,MATCH($B15,EID!$B:$B,0))/2,0),SUM($AG15)*SUM($BP15)+SUM($BJ15)*SUM($BO15)),0))</f>
         <v>0</v>
       </c>
-      <c r="BR15" s="444" t="str">
+      <c r="BR15" s="335">
+        <f>$AG15-$AB15</f>
+        <v>0</v>
+      </c>
+      <c r="BS15" s="335">
+        <f>$BQ15-$AG15</f>
+        <v>0</v>
+      </c>
+      <c r="BT15" s="444" t="str">
         <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add PEPFAR Contribution %"),HYPERLINK("",ROUND($BQ15/$AK15,0))))</f>
         <v>&lt;- Add PEPFAR Contribution %</v>
       </c>
-      <c r="BS15" s="248" t="str">
-        <f>IF(LEFT($B15,4)="_Mil","",IFERROR(1/(1/INDEX(Spectrum!$N:$N,MATCH(RIGHT($B15,13)&amp;"|"&amp;$C15&amp;"|"&amp;$D15&amp;"|"&amp;BS$14&amp;"|"&amp;"CY2022Q3",Spectrum!$Q:$Q,0))),IF(SUM($H15)=0,"",IF(SUM($T15)=0,SUM($R15),$T15)/$H15)))</f>
+      <c r="BU15" s="248" t="str">
+        <f>IF(LEFT($B15,4)="_Mil","",IFERROR(1/(1/INDEX(Spectrum!$N:$N,MATCH(RIGHT($B15,13)&amp;"|"&amp;$C15&amp;"|"&amp;$D15&amp;"|"&amp;BU$14&amp;"|"&amp;"CY2022Q3",Spectrum!$Q:$Q,0))),IF(SUM($H15)=0,"",IF(SUM($T15)=0,SUM($R15),$T15)/$H15)))</f>
         <v/>
       </c>
-      <c r="BT15" s="367" t="str">
-        <f>IF(SUM($H15,$N15)=0,"",SUM($BR15)/SUM($H15,$N15))</f>
+      <c r="BV15" s="367" t="str">
+        <f>IF(SUM($H15,$N15)=0,"",SUM($BT15)/SUM($H15,$N15))</f>
         <v/>
       </c>
-      <c r="BU15" s="163">
+      <c r="BW15" s="163">
         <f>IF($C15="&lt;01","",0%)</f>
         <v>0</v>
       </c>
-      <c r="BV15" s="90">
-        <f>IF($C15="&lt;01","",ROUND(SUM($BU15)*(SUM($BN15)-SUM($BH15)),0))</f>
+      <c r="BX15" s="90">
+        <f>IF($C15="&lt;01","",ROUND((SUM($BN15)-SUM($BH15))*SUM($BW15),0))</f>
         <v>0</v>
       </c>
-      <c r="BW15" s="90">
-        <f>SUM($BN15)-SUM($BV15)</f>
+      <c r="BY15" s="90">
+        <f>SUM($BN15)-SUM($BX15)</f>
         <v>0</v>
       </c>
-      <c r="BX15" s="171"/>
-      <c r="BY15" s="171" t="str">
-        <f>IF(OR(SUM($BW15)=0,$C15="&lt;01"),"",SUM($BX15))</f>
+      <c r="BZ15" s="171"/>
+      <c r="CA15" s="171" t="str">
+        <f>IF(OR(SUM($BY15)=0,$C15="&lt;01"),"",SUM($BZ15))</f>
         <v/>
       </c>
-      <c r="BZ15" s="105" t="str">
-        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$L:$L,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(SUM($BW15)=0,"",IF($BC15="",HYPERLINK("#Cascade!BC"&amp;ROW($BC15),"&lt;- Add Linkage Rate"),HYPERLINK("",ROUND($BW15/$BC15,0)))))</f>
+      <c r="CB15" s="105" t="str">
+        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$L:$L,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(SUM($BY15)=0,"",IF($BC15="",HYPERLINK("#Cascade!BC"&amp;ROW($BC15),"&lt;- Add Linkage Rate"),HYPERLINK("",ROUND($BY15/$BC15,0)))))</f>
         <v/>
       </c>
-      <c r="CA15" s="105" t="str">
-        <f>IF($C15="&lt;01","",IF(SUM($BZ15)=0,"",ROUND($BZ15*SUM($BY15),0)))</f>
+      <c r="CC15" s="105" t="str">
+        <f>IF($C15="&lt;01","",IF(SUM($CB15)=0,"",ROUND($CB15*SUM($CA15),0)))</f>
         <v/>
       </c>
-      <c r="CB15" s="105" t="str">
+      <c r="CD15" s="105" t="str">
         <f>IF(OR($D15&lt;&gt;"Female",$C15="&lt;01",$C15="01-04",$C15="05-09"),"",_xlfn.IFNA(INDEX(PMTCT!$AF:$AF,MATCH($E15,PMTCT!$E:$E,0)),""))</f>
         <v/>
       </c>
-      <c r="CC15" s="105" t="str">
+      <c r="CE15" s="105" t="str">
         <f>IF(OR($D15&lt;&gt;"Female",$C15="&lt;01",$C15="01-04",$C15="05-09"),"",_xlfn.IFNA(INDEX(PMTCT!$AV:$AV,MATCH($E15,PMTCT!$E:$E,0)),""))</f>
         <v/>
       </c>
-      <c r="CD15" s="105">
+      <c r="CF15" s="105">
         <f>IF($C15="&lt;01","",_xlfn.IFNA(INDEX(TB!$Q:$Q,MATCH($E15,TB!$E:$E,0)),""))</f>
         <v>0</v>
       </c>
-      <c r="CE15" s="105" t="str">
+      <c r="CG15" s="105" t="str">
         <f>IF(OR($D15&lt;&gt;"Male",$C15="&lt;01",$C15="01-04",$C15="05-09",$C15="10-14"),"",_xlfn.IFNA(INDEX(VMMC!$AC:$AC,MATCH($E15,VMMC!$E:$E,0)),""))</f>
         <v/>
       </c>
-      <c r="CF15" s="105" t="str">
-        <f>IF($C15="&lt;01",$BZ15,"")</f>
+      <c r="CH15" s="105" t="str">
+        <f>IF($C15="&lt;01",$CB15,"")</f>
         <v/>
       </c>
-      <c r="CG15" s="105" t="str">
-        <f>IF(SUM($BZ15)=0,"",IFERROR(1/(1/($BZ15-SUM($CA15:$CF15))),""))</f>
+      <c r="CI15" s="105" t="str">
+        <f>IF(SUM($CB15)=0,"",IFERROR(1/(1/($CB15-SUM($CC15:$CH15))),""))</f>
         <v/>
       </c>
-      <c r="CH15" s="163" t="str">
-        <f>IF(OR(SUM($BZ15)=0,SUM($CA15)=0),"",$CA15/$BZ15)</f>
+      <c r="CJ15" s="163" t="str">
+        <f>IF(OR(SUM($CB15)=0,SUM($CC15)=0),"",$CC15/$CB15)</f>
         <v/>
       </c>
-      <c r="CI15" s="356" t="str">
-        <f>IF(OR(SUM($BZ15)=0,SUM($CB15)=0),"",$CB15/$BZ15)</f>
+      <c r="CK15" s="356" t="str">
+        <f>IF(OR(SUM($CB15)=0,SUM($CD15)=0),"",$CD15/$CB15)</f>
         <v/>
       </c>
-      <c r="CJ15" s="356" t="str">
-        <f>IF(OR(SUM($BZ15)=0,SUM($CC15)=0),"",$CC15/$BZ15)</f>
+      <c r="CL15" s="356" t="str">
+        <f>IF(OR(SUM($CB15)=0,SUM($CE15)=0),"",$CE15/$CB15)</f>
         <v/>
       </c>
-      <c r="CK15" s="356" t="str">
-        <f>IF(OR(SUM($BZ15)=0,SUM($CD15)=0),"",$CD15/$BZ15)</f>
+      <c r="CM15" s="356" t="str">
+        <f>IF(OR(SUM($CB15)=0,SUM($CF15)=0),"",$CF15/$CB15)</f>
         <v/>
       </c>
-      <c r="CL15" s="356" t="str">
-        <f>IF(OR(SUM($BZ15)=0,SUM($CE15)=0),"",$CE15/$BZ15)</f>
+      <c r="CN15" s="356" t="str">
+        <f>IF(OR(SUM($CB15)=0,SUM($CG15)=0),"",$CG15/$CB15)</f>
         <v/>
       </c>
-      <c r="CM15" s="356" t="str">
-        <f>IF(OR(SUM($BZ15)=0,SUM($CF15)=0),"",$CF15/$BZ15)</f>
+      <c r="CO15" s="356" t="str">
+        <f>IF(OR(SUM($CB15)=0,SUM($CH15)=0),"",$CH15/$CB15)</f>
         <v/>
       </c>
-      <c r="CN15" s="356" t="str">
-        <f>IF(OR(SUM($BZ15)=0,SUM($CG15)=0),"",$CG15/$BZ15)</f>
+      <c r="CP15" s="356" t="str">
+        <f>IF(OR(SUM($CB15)=0,SUM($CI15)=0),"",$CI15/$CB15)</f>
         <v/>
       </c>
-      <c r="CO15" s="161"/>
-      <c r="CP15" s="36"/>
-      <c r="CQ15" s="36"/>
-      <c r="CR15" s="84" t="str">
-        <f>IF(OR(SUM($CA15)=0,SUM($CO15)=0),"",ROUND($CA15*$CO15,0))</f>
+      <c r="CQ15" s="161"/>
+      <c r="CR15" s="36"/>
+      <c r="CS15" s="36"/>
+      <c r="CT15" s="84" t="str">
+        <f>IF(OR(SUM($CC15)=0,SUM($CQ15)=0),"",ROUND($CC15*$CQ15,0))</f>
         <v/>
       </c>
-      <c r="CS15" s="84" t="str">
-        <f>IF(SUM($CR15)=0,"",IF($CP15="",HYPERLINK("#Cascade!CP"&amp;ROW(CP$15),"&lt;- Add Community Yield"),HYPERLINK("",ROUND($CR15/$CP15,0)-$CR15)))</f>
+      <c r="CU15" s="84" t="str">
+        <f>IF(SUM($CT15)=0,"",IF($CR15="",HYPERLINK("#Cascade!CP"&amp;ROW(CR$15),"&lt;- Add Community Yield"),HYPERLINK("",ROUND($CT15/$CR15,0)-$CT15)))</f>
         <v/>
       </c>
-      <c r="CT15" s="84" t="str">
-        <f>IF(SUM($CA15)=0,"",$CA15-SUM($CR15))</f>
+      <c r="CV15" s="84" t="str">
+        <f>IF(SUM($CC15)=0,"",$CC15-SUM($CT15))</f>
         <v/>
       </c>
-      <c r="CU15" s="84" t="str">
-        <f>IF(SUM($CT15)=0,"",IF($CQ15="",HYPERLINK("#Cascade!CQ"&amp;ROW(CQ$15),"&lt;- Add Facility Yield"),HYPERLINK("",ROUND($CT15/$CQ15,0)-$CT15)))</f>
+      <c r="CW15" s="84" t="str">
+        <f>IF(SUM($CV15)=0,"",IF($CS15="",HYPERLINK("#Cascade!CQ"&amp;ROW(CS$15),"&lt;- Add Facility Yield"),HYPERLINK("",ROUND($CV15/$CS15,0)-$CV15)))</f>
         <v/>
       </c>
-      <c r="CV15" s="36" t="str">
-        <f>IF(OR(SUM($BZ15)=0,$C15="&lt;01"),"",SUM($CR15,$CT15)/$BZ15)</f>
+      <c r="CX15" s="36" t="str">
+        <f>IF(OR(SUM($CB15)=0,$C15="&lt;01"),"",SUM($CT15,$CV15)/$CB15)</f>
         <v/>
       </c>
-      <c r="CW15" s="450" t="str">
-        <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add % PEPFAR Contribution"),HYPERLINK("",IF($C15="&lt;01",0,SUM($P15))+SUM($BZ15)/$AK15)))</f>
+      <c r="CY15" s="450" t="str">
+        <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add % PEPFAR Contribution"),HYPERLINK("",IF($C15="&lt;01",0,SUM($P15))+SUM($CB15)/$AK15)))</f>
         <v>&lt;- Add % PEPFAR Contribution</v>
       </c>
-      <c r="CX15"/>
-      <c r="CY15"/>
       <c r="CZ15"/>
       <c r="DA15"/>
       <c r="DB15"/>
       <c r="DC15"/>
+      <c r="DD15"/>
+      <c r="DE15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B3"/>
   </mergeCells>
-  <conditionalFormatting sqref="BU1:BV1048576">
-    <cfRule type="expression" dxfId="172" priority="847">
-      <formula>AND(ISNUMBER(BU1),ROUND(BU1,2)&gt;0)</formula>
+  <conditionalFormatting sqref="BW1:BX1048576">
+    <cfRule type="expression" dxfId="171" priority="847">
+      <formula>AND(ISNUMBER(BW1),ROUND(BW1,2)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:Y1048576 AJ1:AN1048576 AQ1:AQ1048576 AV1:AY1048576 BE1:BE1048576 BR1:BT1048576 CW1:CW1048576">
-    <cfRule type="expression" dxfId="171" priority="102">
+  <conditionalFormatting sqref="F1:Y1048576 AJ1:AN1048576 AQ1:AQ1048576 BE1:BE1048576 BT1:BV1048576 CY1:CY1048576 AV1:AW1048576 AY1:AZ1048576">
+    <cfRule type="expression" dxfId="170" priority="102">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ1:AT1048576 AV1:BG1048576 BI1:BI1048576 BM1:BM1048576 BO1:BP1048576 BU1:BV1048576 BX1:BY1048576 CA1:CE1048576 CG1:CL1048576 CN1:CV1048576">
-    <cfRule type="expression" dxfId="170" priority="95">
+  <conditionalFormatting sqref="AQ1:AT1048576 BI1:BI1048576 BM1:BM1048576 BO1:BP1048576 BW1:BX1048576 BZ1:CA1048576 CC1:CG1048576 CI1:CN1048576 CP1:CX1048576 AV1:BG1048576">
+    <cfRule type="expression" dxfId="169" priority="95">
       <formula>$C1="&lt;01"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO1:BP1048576">
-    <cfRule type="expression" dxfId="169" priority="79">
+    <cfRule type="expression" dxfId="168" priority="79">
       <formula>AND(ISNUMBER(BO1),ROUND(BO1,2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO1:AO1048576 CF1:CF1048576 CM1:CM1048576">
-    <cfRule type="expression" dxfId="168" priority="28">
+  <conditionalFormatting sqref="AO1:AO1048576 CH1:CH1048576 CO1:CO1048576">
+    <cfRule type="expression" dxfId="167" priority="28">
       <formula>AND(ROW(AO1)&gt;14,$B1&lt;&gt;"",NOT($C1="&lt;01"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BY1:BY1048576">
-    <cfRule type="expression" dxfId="167" priority="2576">
-      <formula>AND(ISNUMBER($BY1),$BY1&lt;&gt;$BX1)</formula>
+  <conditionalFormatting sqref="CA1:CA1048576">
+    <cfRule type="expression" dxfId="166" priority="2576">
+      <formula>AND(ISNUMBER($CA1),$CA1&lt;&gt;$BZ1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576 L1:L1048576 AJ1:AM1048576 AQ1:AT1048576 AV1:AV1048576 AX1:AX1048576 AZ1:BG1048576 BL1:BM1048576 BO1:BP1048576 BS1:BU1048576 BX1:BY1048576 CH1:CQ1048576 CV1:CV1048576">
-    <cfRule type="expression" dxfId="166" priority="6">
+  <conditionalFormatting sqref="J1:J1048576 L1:L1048576 AJ1:AM1048576 AQ1:AT1048576 AV1:AV1048576 AX1:BG1048576 BL1:BM1048576 BO1:BP1048576 BU1:BW1048576 BZ1:CA1048576 CJ1:CS1048576 CX1:CX1048576">
+    <cfRule type="expression" dxfId="165" priority="6">
       <formula>AND(ISNUMBER(J1),OR(ROUND(J1,2)&lt;0,ROUND(J1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ1:AT1048576 AV1:AV1048576 AX1:AX1048576 BA1:BC1048576">
-    <cfRule type="expression" dxfId="165" priority="11">
+  <conditionalFormatting sqref="AQ1:AT1048576 AV1:AV1048576 AX1:AY1048576 BA1:BC1048576">
+    <cfRule type="expression" dxfId="164" priority="11">
       <formula>AND(ISNUMBER(AQ1),ROUND(AQ1,2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BS1:BT1048576">
-    <cfRule type="expression" dxfId="164" priority="9">
-      <formula>AND(ISNUMBER(BS1),ROUND(BS1,2)&lt;ROUND(90%*90%,2))</formula>
+  <conditionalFormatting sqref="BU1:BV1048576">
+    <cfRule type="expression" dxfId="163" priority="9">
+      <formula>AND(ISNUMBER(BU1),ROUND(BU1,2)&lt;ROUND(90%*90%,2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE1:BG1048576 BM1:BM1048576">
-    <cfRule type="expression" dxfId="163" priority="7">
+    <cfRule type="expression" dxfId="162" priority="7">
       <formula>AND(ISNUMBER(BE1),ROUND(BE1,2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CL1:CL1048576 CE1:CE1048576">
-    <cfRule type="expression" dxfId="162" priority="2428">
-      <formula>AND(ROW(CE1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Male")</formula>
+  <conditionalFormatting sqref="CN1:CN1048576 CG1:CG1048576">
+    <cfRule type="expression" dxfId="161" priority="2428">
+      <formula>AND(ROW(CG1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Male")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL1:AM1048576">
-    <cfRule type="expression" dxfId="161" priority="12">
+    <cfRule type="expression" dxfId="160" priority="12">
       <formula>AND(ISNUMBER(AL1),ROUND(AL1,2)&lt;POWER(0.95,3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD1:BD1048576">
-    <cfRule type="expression" dxfId="160" priority="2951">
+    <cfRule type="expression" dxfId="159" priority="2951">
       <formula>AND(ISNUMBER(BD1),ROUND(BD1,2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 H1:H1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:AI1048576 AN1:AP1048576 AU1:AU1048576 AW1:AW1048576 AY1:AY1048576 BH1:BK1048576 BN1:BN1048576 BQ1:BR1048576 BV1:BW1048576 BZ1:CG1048576 CR1:CU1048576 CW1:CW1048576">
-    <cfRule type="expression" dxfId="159" priority="5">
+  <conditionalFormatting sqref="F1:F1048576 H1:H1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:AI1048576 AN1:AP1048576 AU1:AU1048576 AW1:AW1048576 AZ1:AZ1048576 BH1:BK1048576 BN1:BN1048576 BQ1:BT1048576 BX1:BY1048576 CB1:CI1048576 CT1:CW1048576 CY1:CY1048576">
+    <cfRule type="expression" dxfId="158" priority="5">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CE1:CE1048576 CL1:CL1048576">
-    <cfRule type="expression" dxfId="158" priority="2963">
-      <formula>AND(ROW(CE1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09",$C1="10-14"))</formula>
+  <conditionalFormatting sqref="CG1:CG1048576 CN1:CN1048576">
+    <cfRule type="expression" dxfId="157" priority="2963">
+      <formula>AND(ROW(CG1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09",$C1="10-14"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO1:CO1048576">
-    <cfRule type="expression" dxfId="157" priority="4">
-      <formula>AND(ISNUMBER($CA1),$CA1&gt;0,CO1="")</formula>
+  <conditionalFormatting sqref="CQ1:CQ1048576">
+    <cfRule type="expression" dxfId="156" priority="4">
+      <formula>AND(ISNUMBER($CC1),$CC1&gt;0,CQ1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 J1:J1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576">
-    <cfRule type="expression" dxfId="156" priority="103">
+    <cfRule type="expression" dxfId="155" priority="103">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&gt;=40%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="104">
+    <cfRule type="expression" dxfId="154" priority="104">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&gt;=20%,G1&lt;40%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="106">
+    <cfRule type="expression" dxfId="153" priority="106">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&lt;20%)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AZ1:AZ1048576">
-    <cfRule type="expression" dxfId="153" priority="1">
-      <formula>AND(ISNUMBER($AZ1),ROUND($AZ1,2)&lt;ROUND(95%*95%,2))</formula>
+  <conditionalFormatting sqref="CD1:CE1048576 CK1:CL1048576">
+    <cfRule type="expression" dxfId="152" priority="92">
+      <formula>AND(ROW(CD1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="151" priority="94">
+      <formula>AND(ROW(CD1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CB1:CC1048576 CI1:CJ1048576">
-    <cfRule type="expression" dxfId="152" priority="92">
-      <formula>AND(ROW(CB1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
+  <conditionalFormatting sqref="CB1:CP1048576">
+    <cfRule type="expression" dxfId="150" priority="3288">
+      <formula>AND(ROW(CB1)&gt;14,$B1&lt;&gt;"",OR(SUM($CI1)&lt;0,ROUND(SUM($CP1),2)&lt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="94">
-      <formula>AND(ROW(CB1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09"))</formula>
+    <cfRule type="expression" dxfId="149" priority="3289">
+      <formula>AND(ROW($CI1)&gt;14,$B1&lt;&gt;"",$C1="&lt;01",OR(SUM($CI1)&lt;&gt;0,ROUND(SUM($CP1),2)&lt;&gt;0,SUM($CC1:$CG1)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BZ1:CN1048576">
-    <cfRule type="expression" dxfId="150" priority="3281">
-      <formula>AND(ROW(BZ1)&gt;14,$B1&lt;&gt;"",OR(SUM($CG1)&lt;0,ROUND(SUM($CN1),2)&lt;0))</formula>
+  <conditionalFormatting sqref="CR1:CS1048576">
+    <cfRule type="expression" dxfId="148" priority="3290">
+      <formula>AND(ISNUMBER($CC1),$CC1&lt;&gt;0,SUM(CR1)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="3282">
-      <formula>AND(ROW($CG1)&gt;14,$B1&lt;&gt;"",$C1="&lt;01",OR(SUM($CG1)&lt;&gt;0,ROUND(SUM($CN1),2)&lt;&gt;0,SUM($CA1:$CE1)&lt;&gt;0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CP1:CQ1048576">
-    <cfRule type="expression" dxfId="148" priority="3279">
-      <formula>AND(ISNUMBER($CA1),$CA1&lt;&gt;0,SUM(CP1)=0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="147" priority="3280">
-      <formula>AND(OR($C1="15-19",$C1="20-24",$C1="25-29",$C1="30-34",$C1="35-39",$C1="40-44",$C1="45-49",$C1="50-54",$C1="55-59",$C1="60-64",$C1="65+"),CP1&lt;20%,CP1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="147" priority="3291">
+      <formula>AND(OR($C1="15-19",$C1="20-24",$C1="25-29",$C1="30-34",$C1="35-39",$C1="40-44",$C1="45-49",$C1="50-54",$C1="55-59",$C1="60-64",$C1="65+"),CR1&lt;20%,CR1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="CA3" location="Cascade!CR:CU" display="Cascade!CR:CU" xr:uid="{CFC22E83-CD81-744A-BD97-81BDFE5732F2}"/>
-    <hyperlink ref="CB3" location="PMTCT!AF:AF" display="PMTCT_STAT New Positives (FY23)" xr:uid="{072C5291-7010-704F-BBB9-7097DE99B670}"/>
-    <hyperlink ref="CC3" location="PMTCT!AV:AV" display="HTS_TST Post ANC1 New Positives (FY23)" xr:uid="{BD5510F0-19E5-3C41-B8F3-9039D1D2730F}"/>
-    <hyperlink ref="CD3" location="TB!Q:Q" display="TB_STAT New Positives (FY22)" xr:uid="{4946A338-D073-E84B-90AE-459B22CC722F}"/>
-    <hyperlink ref="CE3" location="VMMC!AC:AC" display="VMMC Tested Positives (FY22)" xr:uid="{9324AD3D-0667-6B41-8A55-485E12745DBA}"/>
-    <hyperlink ref="CF3" location="EID!L:L" display="EID!L:L" xr:uid="{DD5860B7-2BBA-D54C-AC3A-9FA1A8C82695}"/>
-    <hyperlink ref="CG3" location="HTS!O:O" display="HTS_TST_POS from All Other Modalities (FY23)" xr:uid="{94117302-B331-2E49-A0BD-18496ED310FB}"/>
+    <hyperlink ref="CC3" location="Cascade!CT:CW" display="Cascade!CT:CW" xr:uid="{CFC22E83-CD81-744A-BD97-81BDFE5732F2}"/>
+    <hyperlink ref="CD3" location="PMTCT!AF:AF" display="PMTCT_STAT New Positives (FY23)" xr:uid="{072C5291-7010-704F-BBB9-7097DE99B670}"/>
+    <hyperlink ref="CE3" location="PMTCT!AV:AV" display="HTS_TST Post ANC1 New Positives (FY23)" xr:uid="{BD5510F0-19E5-3C41-B8F3-9039D1D2730F}"/>
+    <hyperlink ref="CF3" location="TB!Q:Q" display="TB_STAT New Positives (FY22)" xr:uid="{4946A338-D073-E84B-90AE-459B22CC722F}"/>
+    <hyperlink ref="CG3" location="VMMC!AC:AC" display="VMMC Tested Positives (FY22)" xr:uid="{9324AD3D-0667-6B41-8A55-485E12745DBA}"/>
+    <hyperlink ref="CH3" location="EID!L:L" display="EID!L:L" xr:uid="{DD5860B7-2BBA-D54C-AC3A-9FA1A8C82695}"/>
+    <hyperlink ref="CI3" location="HTS!O:O" display="HTS_TST_POS from All Other Modalities (FY23)" xr:uid="{94117302-B331-2E49-A0BD-18496ED310FB}"/>
     <hyperlink ref="AO3" location="EID!V:V" display="PMTCT_HEI_POS Virally Suppressed (FY23)" xr:uid="{72DBFF04-97B7-3548-95A9-48E392DE0703}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -46099,7 +46204,7 @@
         <v>756</v>
       </c>
       <c r="S3" s="136" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="T3" s="48" t="s">
         <v>260</v>
@@ -46126,22 +46231,22 @@
         <v>983</v>
       </c>
       <c r="AB3" s="246" t="s">
+        <v>1166</v>
+      </c>
+      <c r="AC3" s="354" t="s">
         <v>1167</v>
       </c>
-      <c r="AC3" s="354" t="s">
-        <v>1168</v>
-      </c>
       <c r="AD3" s="121" t="s">
+        <v>1154</v>
+      </c>
+      <c r="AE3" s="69" t="s">
         <v>1155</v>
       </c>
-      <c r="AE3" s="69" t="s">
+      <c r="AF3" s="70" t="s">
         <v>1156</v>
       </c>
-      <c r="AF3" s="70" t="s">
+      <c r="AG3" s="69" t="s">
         <v>1157</v>
-      </c>
-      <c r="AG3" s="69" t="s">
-        <v>1158</v>
       </c>
       <c r="AH3" s="270" t="s">
         <v>739</v>
@@ -46159,10 +46264,10 @@
         <v>842</v>
       </c>
       <c r="AM3" s="158" t="s">
+        <v>1158</v>
+      </c>
+      <c r="AN3" s="69" t="s">
         <v>1159</v>
-      </c>
-      <c r="AN3" s="69" t="s">
-        <v>1160</v>
       </c>
       <c r="AO3" s="270" t="s">
         <v>984</v>
@@ -46186,13 +46291,13 @@
         <v>842</v>
       </c>
       <c r="AV3" s="409" t="s">
+        <v>1160</v>
+      </c>
+      <c r="AW3" s="69" t="s">
         <v>1161</v>
       </c>
-      <c r="AW3" s="69" t="s">
+      <c r="AX3" s="406" t="s">
         <v>1162</v>
-      </c>
-      <c r="AX3" s="406" t="s">
-        <v>1163</v>
       </c>
       <c r="AY3" s="255" t="s">
         <v>1063</v>
@@ -47667,7 +47772,7 @@
         <v/>
       </c>
       <c r="J15" s="36" t="str">
-        <f>IF(LEFT($B15,4)="_Mil","",_xlfn.IFNA(INDEX(Cascade!$BS:$BS,MATCH($E15,Cascade!$E:$E,0)),""))</f>
+        <f>IF(LEFT($B15,4)="_Mil","",_xlfn.IFNA(INDEX(Cascade!$BU:$BU,MATCH($E15,Cascade!$E:$E,0)),""))</f>
         <v/>
       </c>
       <c r="K15" s="36" t="str">
@@ -47820,7 +47925,7 @@
         <v/>
       </c>
       <c r="AZ15" s="97" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$BZ:$BZ,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CB:$CB,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
       <c r="BA15" s="248" t="str">
@@ -47832,15 +47937,15 @@
         <v/>
       </c>
       <c r="BC15" s="248" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CH:$CH,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CJ:$CJ,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
       <c r="BD15" s="248" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CK:$CK,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CM:$CM,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
       <c r="BE15" s="248" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CN:$CN,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CP:$CP,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
     </row>
@@ -47916,21 +48021,21 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="AV3" location="Cascade!CC:CC" display="Positive (FY23)" xr:uid="{9AC7778E-2E88-7242-BE1A-0032FDF1AA0A}"/>
+    <hyperlink ref="AV3" location="Cascade!CE:CE" display="Positive (FY23)" xr:uid="{9AC7778E-2E88-7242-BE1A-0032FDF1AA0A}"/>
     <hyperlink ref="AY3" location="EID!C:C" display="Total PMTCT: Positives (From ANC1 &amp; Post ANC1) (FY23)" xr:uid="{06033567-B162-B642-952B-86F608E51389}"/>
     <hyperlink ref="F3" location="Cascade!F:F" display="Host Country Est. Female Population (FY21)" xr:uid="{9DCC4747-78E8-574F-8A0A-74D7310ECF73}"/>
     <hyperlink ref="G3" location="Cascade!H:H" display="Host Country Est. PLHIV (FY21)" xr:uid="{38AE695F-2465-C345-B2DE-60A49EB9D43A}"/>
     <hyperlink ref="H3" location="Cascade!J:J" display="Host Country Est. HIV Prevalence (FY21) (%)" xr:uid="{5FF09F6B-1BA6-A247-A7AB-EF4027EBC38D}"/>
     <hyperlink ref="I3" location="Cascade!T:T" display="Host Country Est. TX_CURR_SUBNAT (FY22)" xr:uid="{AE293FF8-6531-8E47-9771-94756A48F05D}"/>
     <hyperlink ref="J3" location="Cascade!BS:BS" display="Host Country Est. ART Coverage (FY22) (%)" xr:uid="{62172621-78AD-F245-A486-21A9FED7A825}"/>
-    <hyperlink ref="AZ3" location="Cascade!BZ:BZ" display="Total HTS_TST_POS (FY23)" xr:uid="{EF1CACDE-E83E-BC49-803E-79E8D75E671B}"/>
+    <hyperlink ref="AZ3" location="Cascade!CB:CB" display="Total HTS_TST_POS (FY23)" xr:uid="{EF1CACDE-E83E-BC49-803E-79E8D75E671B}"/>
     <hyperlink ref="BA3" location="PMTCT!AF:AF" display="Total Positives from PMTCT_STAT ANC1 (FY23) (%)" xr:uid="{237D0CFB-FBAB-3A42-9524-0309C16E980E}"/>
     <hyperlink ref="BB3" location="PMTCT!AV:AV" display="Total Positives from PMTCT Post ANC1 (FY23) (%)" xr:uid="{D680F786-FE9E-564F-8330-479022D7C4BA}"/>
-    <hyperlink ref="BC3" location="Cascade!CH:CH" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{A440D5C0-3246-D64E-9D9A-125BFE1073A1}"/>
-    <hyperlink ref="BD3" location="Cascade!CK:CK" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{37B73FCD-3AA1-4546-B221-83E509C72600}"/>
-    <hyperlink ref="BE3" location="Cascade!CN:CN" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{EA06E773-2DB3-0B4D-BA39-4517BD65D120}"/>
+    <hyperlink ref="BC3" location="Cascade!CJ:CJ" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{A440D5C0-3246-D64E-9D9A-125BFE1073A1}"/>
+    <hyperlink ref="BD3" location="Cascade!CM:CM" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{37B73FCD-3AA1-4546-B221-83E509C72600}"/>
+    <hyperlink ref="BE3" location="Cascade!CP:CP" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{EA06E773-2DB3-0B4D-BA39-4517BD65D120}"/>
     <hyperlink ref="K3" location="Cascade!AL:AL" display="Host Country Est. PopVLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{117CCFAC-2256-F346-BBFA-6D9C183041C6}"/>
-    <hyperlink ref="AF3" location="Cascade!CB:CB" display="Newly Tested, Positive (FY23)" xr:uid="{ABC0F45D-6FF3-E94C-B20E-66540AE6F2E1}"/>
+    <hyperlink ref="AF3" location="Cascade!CD:CD" display="Newly Tested, Positive (FY23)" xr:uid="{ABC0F45D-6FF3-E94C-B20E-66540AE6F2E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -48077,19 +48182,19 @@
         <v>998</v>
       </c>
       <c r="Q3" s="404" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="R3" s="344" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="S3" s="404" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="T3" s="70" t="s">
         <v>995</v>
       </c>
       <c r="U3" s="404" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="V3" s="70" t="s">
         <v>996</v>
@@ -48582,7 +48687,7 @@
         <v>1002</v>
       </c>
       <c r="R14" s="172" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="S14" s="209" t="s">
         <v>1001</v>
@@ -48726,7 +48831,7 @@
     <hyperlink ref="V3" location="Cascade!AP:AP" display="HIV+ infants  Virally Suppressed (FY23)" xr:uid="{B588F469-4EE5-124C-9655-BE4B92E2099B}"/>
     <hyperlink ref="T3" location="Cascade!AU:AU" display="HIV+ infants tested for VLS (FY23)" xr:uid="{204B8930-346A-BF40-BF29-A050F7DAD2C2}"/>
     <hyperlink ref="P3" location="Cascade!BQ:BQ" display="HIV+ infants retained on ART at end of FY23" xr:uid="{89871460-7732-6748-8258-655A5F0C2B89}"/>
-    <hyperlink ref="L3" location="Cascade!CF:CF" display="Total HIV+ infants identified (FY23)" xr:uid="{29465258-72C7-F34F-B99E-5CC67BF8776B}"/>
+    <hyperlink ref="L3" location="Cascade!CH:CH" display="Total HIV+ infants identified (FY23)" xr:uid="{29465258-72C7-F34F-B99E-5CC67BF8776B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -48885,10 +48990,10 @@
         <v>1003</v>
       </c>
       <c r="M3" s="246" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="N3" s="354" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="O3" s="121" t="s">
         <v>277</v>
@@ -49641,7 +49746,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="98" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$BZ:$BZ,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CB:$CB,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
       <c r="W15" s="36" t="str">
@@ -49649,23 +49754,23 @@
         <v/>
       </c>
       <c r="X15" s="36" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CH:$CH,MATCH($E15,Cascade!$E:$E,0)),"")</f>
-        <v/>
-      </c>
-      <c r="Y15" s="36" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CI:$CI,MATCH($E15,Cascade!$E:$E,0)),"")</f>
-        <v/>
-      </c>
-      <c r="Z15" s="36" t="str">
         <f>_xlfn.IFNA(INDEX(Cascade!$CJ:$CJ,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
-      <c r="AA15" s="36" t="str">
+      <c r="Y15" s="36" t="str">
+        <f>_xlfn.IFNA(INDEX(Cascade!$CK:$CK,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Z15" s="36" t="str">
         <f>_xlfn.IFNA(INDEX(Cascade!$CL:$CL,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
+      <c r="AA15" s="36" t="str">
+        <f>_xlfn.IFNA(INDEX(Cascade!$CN:$CN,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <v/>
+      </c>
       <c r="AB15" s="36" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CN:$CN,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CP:$CP,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
     </row>
@@ -49741,14 +49846,14 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="Q3" location="Cascade!CD:CD" display="Newly Tested, Positive" xr:uid="{F41C5CBD-C2B6-7349-92F3-4B3EE0741D63}"/>
-    <hyperlink ref="V3" location="Cascade!BZ:BZ" display="Total HTS_TST_POS (FY23)" xr:uid="{0C12D99A-2693-9E4D-945B-D14B7A252AA9}"/>
+    <hyperlink ref="Q3" location="Cascade!CF:CF" display="Newly Tested, Positive" xr:uid="{F41C5CBD-C2B6-7349-92F3-4B3EE0741D63}"/>
+    <hyperlink ref="V3" location="Cascade!CB:CB" display="Total HTS_TST_POS (FY23)" xr:uid="{0C12D99A-2693-9E4D-945B-D14B7A252AA9}"/>
     <hyperlink ref="W3" location="TB!Q:Q" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{B168364E-0686-8544-BA70-DF499D18A47C}"/>
-    <hyperlink ref="X3" location="Cascade!CH:CH" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{05C499CF-75CA-2A49-859D-540B72651529}"/>
-    <hyperlink ref="Y3" location="Cascade!CI:CI" display="Total Positives from PMTCT_STAT (FY23) (%)" xr:uid="{54774E98-3A3D-4D48-90D1-801481ED11B7}"/>
-    <hyperlink ref="Z3" location="Cascade!CJ:CJ" display="Total Positives from Post ANC1 (FY23) (%)" xr:uid="{6E885B80-FB4C-E04D-B2FB-104D9CEB3861}"/>
-    <hyperlink ref="AA3" location="Cascade!CL:CL" display="Total Positives from VMMC (FY23) (%)" xr:uid="{C15FB732-6CF1-6C44-B544-07BF476A6F31}"/>
-    <hyperlink ref="AB3" location="Cascade!CN:CN" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{9AC9FE86-7701-D446-947B-8E63FD134235}"/>
+    <hyperlink ref="X3" location="Cascade!CJ:CJ" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{05C499CF-75CA-2A49-859D-540B72651529}"/>
+    <hyperlink ref="Y3" location="Cascade!CK:CK" display="Total Positives from PMTCT_STAT (FY23) (%)" xr:uid="{54774E98-3A3D-4D48-90D1-801481ED11B7}"/>
+    <hyperlink ref="Z3" location="Cascade!CL:CL" display="Total Positives from Post ANC1 (FY23) (%)" xr:uid="{6E885B80-FB4C-E04D-B2FB-104D9CEB3861}"/>
+    <hyperlink ref="AA3" location="Cascade!CN:CN" display="Total Positives from VMMC (FY23) (%)" xr:uid="{C15FB732-6CF1-6C44-B544-07BF476A6F31}"/>
+    <hyperlink ref="AB3" location="Cascade!CP:CP" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{9AC9FE86-7701-D446-947B-8E63FD134235}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -49879,7 +49984,7 @@
         <v>2</v>
       </c>
       <c r="V2" s="34" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="W2" s="34"/>
       <c r="X2" s="34"/>
@@ -49955,7 +50060,7 @@
         <v>1004</v>
       </c>
       <c r="U3" s="204" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="V3" s="204" t="s">
         <v>1076</v>
@@ -49967,10 +50072,10 @@
         <v>1005</v>
       </c>
       <c r="Y3" s="336" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="Z3" s="204" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="AA3" s="69" t="s">
         <v>209</v>
@@ -50891,7 +50996,7 @@
         <v/>
       </c>
       <c r="J15" s="36" t="str">
-        <f>IF(LEFT($B15,4)="_Mil","",_xlfn.IFNA(INDEX(Cascade!$BS:$BS,MATCH($E15,Cascade!$E:$E,0)),""))</f>
+        <f>IF(LEFT($B15,4)="_Mil","",_xlfn.IFNA(INDEX(Cascade!$BU:$BU,MATCH($E15,Cascade!$E:$E,0)),""))</f>
         <v/>
       </c>
       <c r="K15" s="36" t="str">
@@ -50922,13 +51027,13 @@
         <f>IF(OR(LEFT($B15,4)="_Mil",SUM($P15)=0),"",ROUND(MAX($P15-SUM($M15),0),0))</f>
         <v/>
       </c>
-      <c r="T15" s="36" t="str">
-        <f>IF(OR(LEFT($B15,4)="_Mil",SUM($L15)=0),"",SUM($S15)/$L15)</f>
-        <v/>
-      </c>
-      <c r="U15" s="36" t="str">
-        <f>IF(SUM($T15)=0,"",$T15)</f>
-        <v/>
+      <c r="T15" s="36">
+        <f>IF(LEFT($B15,4)="_Mil","",IF(SUM($S15)=0,0,IF(SUM($L15)=0,1,$S15/$L15)))</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="36">
+        <f>IF(LEFT($B15,4)="_Mil","",$T15)</f>
+        <v>0</v>
       </c>
       <c r="V15" s="36" t="str">
         <f>IF(LEFT($B15,4)="_Mil",0,"")</f>
@@ -50969,7 +51074,7 @@
         <v>0</v>
       </c>
       <c r="AG15" s="98" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$BZ:$BZ,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CB:$CB,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
       <c r="AH15" s="248" t="str">
@@ -50977,15 +51082,15 @@
         <v/>
       </c>
       <c r="AI15" s="248" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CH:$CH,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CJ:$CJ,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
       <c r="AJ15" s="248" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CK:$CK,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CM:$CM,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
       <c r="AK15" s="248" t="str">
-        <f>_xlfn.IFNA(INDEX(Cascade!$CN:$CN,MATCH($E15,Cascade!$E:$E,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(Cascade!$CP:$CP,MATCH($E15,Cascade!$E:$E,0)),"")</f>
         <v/>
       </c>
     </row>
@@ -51053,16 +51158,16 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F3" location="Cascade!F:F" display="Host Country Est. Male Population (FY21)" xr:uid="{C6A99DFC-4F48-404C-9B66-D9590F47A2D3}"/>
-    <hyperlink ref="AC3" location="Cascade!CE:CE" display="HIV Positive" xr:uid="{2DCD329B-B29F-704E-8461-36B4301F077A}"/>
+    <hyperlink ref="AC3" location="Cascade!CG:CG" display="HIV Positive" xr:uid="{2DCD329B-B29F-704E-8461-36B4301F077A}"/>
     <hyperlink ref="G3" location="Cascade!H:H" display="Host Country Est. PLHIV (FY21)" xr:uid="{2930CCBC-8F45-954A-9C4B-E82145674BB9}"/>
     <hyperlink ref="H3" location="Cascade!J:J" display="Host Country Est. HIV Prevalence (FY21) (%)" xr:uid="{5289F01F-A702-2040-B8A4-F3E42F6D1A29}"/>
     <hyperlink ref="I3" location="Cascade!T:T" display="Host Country Est. TX_CURR_SUBNAT (FY22)" xr:uid="{0B9E2838-E36E-914B-ABB2-4D62A487F4F9}"/>
     <hyperlink ref="J3" location="Cascade!BS:BS" display="Host Country Est. ART Coverage (FY22) (%)" xr:uid="{A7D90546-FC05-1942-88B3-F73371278897}"/>
-    <hyperlink ref="AG3" location="Cascade!BZ:BZ" display="Total HTS_TST_POS (FY23)" xr:uid="{54DA9148-5100-4B4B-9121-6C351B2AE8A1}"/>
+    <hyperlink ref="AG3" location="Cascade!CB:CB" display="Total HTS_TST_POS (FY23)" xr:uid="{54DA9148-5100-4B4B-9121-6C351B2AE8A1}"/>
     <hyperlink ref="AH3" location="VMMC!AC:AC" display="Total Positives from VMMC_CIRC (FY23) (%)" xr:uid="{823FE536-9720-0B41-B603-761E70AF5F5E}"/>
-    <hyperlink ref="AI3" location="Cascade!CH:CH" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{51CE2F45-E9AC-8943-8F4A-61132094AC48}"/>
-    <hyperlink ref="AJ3" location="Cascade!CK:CK" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{89FDD463-524F-4745-993F-7C848E2A4A01}"/>
-    <hyperlink ref="AK3" location="Cascade!CN:CN" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{DF85F481-72CF-A242-8614-1D2F503366BF}"/>
+    <hyperlink ref="AI3" location="Cascade!CJ:CJ" display="Total Positives from HTS_INDEX (FY23) (%)" xr:uid="{51CE2F45-E9AC-8943-8F4A-61132094AC48}"/>
+    <hyperlink ref="AJ3" location="Cascade!CM:CM" display="Total Positives from TB_STAT (FY23) (%)" xr:uid="{89FDD463-524F-4745-993F-7C848E2A4A01}"/>
+    <hyperlink ref="AK3" location="Cascade!CP:CP" display="Total Positives from All Other Modalities (FY23) (%)" xr:uid="{DF85F481-72CF-A242-8614-1D2F503366BF}"/>
     <hyperlink ref="K3" location="Cascade!AL:AL" display="Host Country Est. PopVLS Rate (VLS/PLHIV) (FY22) (%)" xr:uid="{B9826B15-EC60-524A-9E47-7913491A2C2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update COP22 DP schema to remove FYs from PSNUxIM tab
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_Data_Pack_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3801C6A8-27B1-384C-9492-0906E8F83FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68F9432-D27B-A24F-9618-3E7197338A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="3" activeTab="5" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="3" activeTab="20" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -6497,15 +6497,6 @@
     <t>MAX - Crosswalk Total</t>
   </si>
   <si>
-    <t>Crosswalk Dedupe Resolution (FY22)</t>
-  </si>
-  <si>
-    <t>Custom Crosswalk Dedupe Allocation (FY22) (% of DataPackTarget)</t>
-  </si>
-  <si>
-    <t>Total Deduplicated Rollup (FY22)</t>
-  </si>
-  <si>
     <t>SUM - DSD</t>
   </si>
   <si>
@@ -6515,15 +6506,6 @@
     <t>DSD Count</t>
   </si>
   <si>
-    <t>DSD Dedupe Resolution (FY22)</t>
-  </si>
-  <si>
-    <t>Custom DSD Dedupe Allocation (FY22) (% of DataPackTarget)</t>
-  </si>
-  <si>
-    <t>Deduplicated DSD Rollup (FY22)</t>
-  </si>
-  <si>
     <t>SUM - TA</t>
   </si>
   <si>
@@ -6531,15 +6513,6 @@
   </si>
   <si>
     <t>TA Count</t>
-  </si>
-  <si>
-    <t>TA Dedupe Resolution (FY22)</t>
-  </si>
-  <si>
-    <t>Custom TA Dedupe Allocation (FY22) (% of DataPackTarget)</t>
-  </si>
-  <si>
-    <t>Deduplicated TA Rollup (FY22)</t>
   </si>
   <si>
     <t>Total PMTCT: Positives (From ANC1 &amp; Post ANC1, incl. Known Pos) (FY23)</t>
@@ -6577,6 +6550,33 @@
   </si>
   <si>
     <t>Not PEPFAR</t>
+  </si>
+  <si>
+    <t>Crosswalk Dedupe Resolution</t>
+  </si>
+  <si>
+    <t>Custom Crosswalk Dedupe Allocation  (% of DataPackTarget)</t>
+  </si>
+  <si>
+    <t>Total Deduplicated Rollup</t>
+  </si>
+  <si>
+    <t>DSD Dedupe Resolution</t>
+  </si>
+  <si>
+    <t>Custom DSD Dedupe Allocation  (% of DataPackTarget)</t>
+  </si>
+  <si>
+    <t>Deduplicated DSD Rollup</t>
+  </si>
+  <si>
+    <t>Deduplicated TA Rollup</t>
+  </si>
+  <si>
+    <t>Custom TA Dedupe Allocation (% of DataPackTarget)</t>
+  </si>
+  <si>
+    <t>TA Dedupe Resolution</t>
   </si>
 </sst>
 </file>
@@ -16286,16 +16286,16 @@
         <v>1156</v>
       </c>
       <c r="S3" s="316" t="s">
-        <v>1228</v>
+        <v>1219</v>
       </c>
       <c r="T3" s="100" t="s">
         <v>1184</v>
       </c>
       <c r="U3" s="316" t="s">
-        <v>1235</v>
+        <v>1226</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>1236</v>
+        <v>1227</v>
       </c>
       <c r="W3" s="53" t="s">
         <v>32</v>
@@ -18621,7 +18621,7 @@
         <v>799</v>
       </c>
       <c r="G3" s="60" t="s">
-        <v>1233</v>
+        <v>1224</v>
       </c>
       <c r="H3" s="304" t="s">
         <v>862</v>
@@ -36608,8 +36608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B207F3C7-F002-E540-88C1-75A9C9657E34}">
   <dimension ref="A1:FS23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42148,7 +42148,7 @@
         <v>1208</v>
       </c>
       <c r="I14" s="477" t="s">
-        <v>1238</v>
+        <v>1229</v>
       </c>
       <c r="J14" s="478" t="s">
         <v>1209</v>
@@ -42233,49 +42233,49 @@
         <v>1211</v>
       </c>
       <c r="CH14" s="481" t="s">
+        <v>1230</v>
+      </c>
+      <c r="CI14" s="482" t="s">
+        <v>1231</v>
+      </c>
+      <c r="CJ14" s="483" t="s">
+        <v>1232</v>
+      </c>
+      <c r="CK14" s="254" t="s">
         <v>1212</v>
       </c>
-      <c r="CI14" s="482" t="s">
+      <c r="CL14" s="254" t="s">
         <v>1213</v>
       </c>
-      <c r="CJ14" s="483" t="s">
+      <c r="CM14" s="254" t="s">
         <v>1214</v>
       </c>
-      <c r="CK14" s="254" t="s">
+      <c r="CN14" s="481" t="s">
+        <v>1233</v>
+      </c>
+      <c r="CO14" s="482" t="s">
+        <v>1234</v>
+      </c>
+      <c r="CP14" s="483" t="s">
+        <v>1235</v>
+      </c>
+      <c r="CQ14" s="254" t="s">
         <v>1215</v>
       </c>
-      <c r="CL14" s="254" t="s">
+      <c r="CR14" s="254" t="s">
         <v>1216</v>
       </c>
-      <c r="CM14" s="254" t="s">
+      <c r="CS14" s="254" t="s">
         <v>1217</v>
       </c>
-      <c r="CN14" s="481" t="s">
-        <v>1218</v>
-      </c>
-      <c r="CO14" s="482" t="s">
-        <v>1219</v>
-      </c>
-      <c r="CP14" s="483" t="s">
-        <v>1220</v>
-      </c>
-      <c r="CQ14" s="254" t="s">
-        <v>1221</v>
-      </c>
-      <c r="CR14" s="254" t="s">
-        <v>1222</v>
-      </c>
-      <c r="CS14" s="254" t="s">
-        <v>1223</v>
-      </c>
       <c r="CT14" s="481" t="s">
-        <v>1224</v>
+        <v>1238</v>
       </c>
       <c r="CU14" s="482" t="s">
-        <v>1225</v>
+        <v>1237</v>
       </c>
       <c r="CV14" s="483" t="s">
-        <v>1226</v>
+        <v>1236</v>
       </c>
       <c r="CW14" s="484" t="str">
         <f t="shared" ref="CW14:FH14" si="0">IF(I14="","",I$14)</f>
@@ -44034,13 +44034,13 @@
         <v>1127</v>
       </c>
       <c r="BH3" s="235" t="s">
-        <v>1229</v>
+        <v>1220</v>
       </c>
       <c r="BI3" s="235" t="s">
-        <v>1232</v>
+        <v>1223</v>
       </c>
       <c r="BJ3" s="259" t="s">
-        <v>1230</v>
+        <v>1221</v>
       </c>
       <c r="BK3" s="259" t="s">
         <v>1129</v>
@@ -44049,7 +44049,7 @@
         <v>1163</v>
       </c>
       <c r="BM3" s="330" t="s">
-        <v>1231</v>
+        <v>1222</v>
       </c>
       <c r="BN3" s="259" t="s">
         <v>779</v>
@@ -46830,7 +46830,7 @@
         <v>1171</v>
       </c>
       <c r="AX14" s="231" t="s">
-        <v>1234</v>
+        <v>1225</v>
       </c>
       <c r="AY14" s="231" t="s">
         <v>497</v>
@@ -47630,7 +47630,7 @@
     </row>
     <row r="2" spans="1:57" s="40" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="428" t="s">
-        <v>1237</v>
+        <v>1228</v>
       </c>
       <c r="B2" s="425"/>
       <c r="D2" s="2"/>
@@ -47861,7 +47861,7 @@
         <v>1143</v>
       </c>
       <c r="AY3" s="237" t="s">
-        <v>1227</v>
+        <v>1218</v>
       </c>
       <c r="AZ3" s="241" t="s">
         <v>793</v>
@@ -49616,7 +49616,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="14" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
Minor issues with hyperlink addresses & VLC rates
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_Data_Pack_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB78D0EF-AF3B-D44A-B621-7253AEDB717D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54521DAF-CB1E-CE47-B92C-68958AD80A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="3" activeTab="17" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
+    <workbookView xWindow="-10480" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="PrEP" sheetId="16" r:id="rId18"/>
     <sheet name="KP_MAT" sheetId="40" r:id="rId19"/>
     <sheet name="KP Validation" sheetId="46" r:id="rId20"/>
-    <sheet name="PSNUxIM" sheetId="47" r:id="rId21"/>
+    <sheet name="PSNUxIM" sheetId="47" state="hidden" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AGYW!$B$14:$M$39</definedName>
@@ -8147,47 +8147,15 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="3" xr:uid="{EBDE175B-1152-3C44-B18E-2B948C595077}"/>
   </cellStyles>
-  <dxfs count="197">
+  <dxfs count="204">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
       </fill>
     </dxf>
     <dxf>
@@ -8202,6 +8170,66 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFC00000"/>
       </font>
       <fill>
@@ -8210,10 +8238,140 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -8696,6 +8854,40 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -9137,124 +9329,6 @@
       <fill>
         <patternFill patternType="darkUp">
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10387,7 +10461,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10425,10 +10499,10 @@
   <dimension ref="A1:CC15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="14" topLeftCell="AZ15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="BC1" sqref="BC1:BC1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13454,67 +13528,67 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="N1:N1048576 U1:U1048576 BW1:BW1048576">
-    <cfRule type="expression" dxfId="101" priority="25">
+    <cfRule type="expression" dxfId="120" priority="25">
       <formula>OR($D1="Female",$C1="01-04",$C1="05-09",$C1="10-14")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:X1048576 AK1:AP1048576">
-    <cfRule type="expression" dxfId="100" priority="355">
+    <cfRule type="expression" dxfId="119" priority="355">
       <formula>AND(ROW(W1)&gt;14,$B1&lt;&gt;"",$C1&lt;&gt;"01-04")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA1:CC1048576">
-    <cfRule type="expression" dxfId="99" priority="197">
+    <cfRule type="expression" dxfId="118" priority="197">
       <formula>OR($C1="01-04",$C1="05-09")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1048576 R1:S1048576 BT1:BU1048576">
-    <cfRule type="expression" dxfId="98" priority="34">
+    <cfRule type="expression" dxfId="117" priority="34">
       <formula>OR($D1="Male",$C1="01-04",$C1="05-09")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ1:BQ1048576">
-    <cfRule type="expression" dxfId="97" priority="680">
+    <cfRule type="expression" dxfId="116" priority="680">
       <formula>AND(ISNUMBER($BQ1),ROUND(SUM($BQ1),0)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH1:AH1048576 AQ1:AQ1048576 AT1:AT1048576 AW1:AW1048576 AZ1:AZ1048576">
-    <cfRule type="expression" dxfId="96" priority="30">
+    <cfRule type="expression" dxfId="115" priority="30">
       <formula>AND(ISNUMBER(AH1),OR(AND($F1&gt;=0.7,ROUND(AH1,2)&lt;0.1),AND($F1&lt;0.7,ROUND(AH1,2)&lt;0.05)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ1:AJ1048576 AM1:AM1048576 AP1:AP1048576 AS1:AS1048576 AV1:AV1048576 AY1:AY1048576 BB1:BB1048576 BH1:BH1048576 BN1:BN1048576 BK1:BK1048576 BE1:BE1048576">
-    <cfRule type="containsText" dxfId="95" priority="26" operator="containsText" text="ENTER YIELD!">
+    <cfRule type="containsText" dxfId="114" priority="26" operator="containsText" text="ENTER YIELD!">
       <formula>NOT(ISERROR(SEARCH("ENTER YIELD!",AJ1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF1:AF1048576">
-    <cfRule type="expression" dxfId="94" priority="2165">
+    <cfRule type="expression" dxfId="113" priority="2165">
       <formula>AND(ISNUMBER($AF1),ROUND(SUM($F1),2)&gt;=80%,(SUM($H1)*SUM($AF1))&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:AG1048576">
-    <cfRule type="expression" dxfId="93" priority="2168">
+    <cfRule type="expression" dxfId="112" priority="2168">
       <formula>AND(ISNUMBER($AG1),ROUND($AG1,2)&lt;&gt;1,ROUND($H1,0)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM1:BN1048576">
-    <cfRule type="expression" dxfId="92" priority="2170">
+    <cfRule type="expression" dxfId="111" priority="2170">
       <formula>AND(ISNUMBER(BM1),SUM($F1)&gt;=80%,SUM(BM1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="expression" dxfId="91" priority="5">
+    <cfRule type="expression" dxfId="110" priority="5">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 P1:AH1048576 AK1:AK1048576 AN1:AN1048576 AQ1:AQ1048576 AT1:AT1048576 AW1:AW1048576 AZ1:AZ1048576 BC1:BC1048576 BF1:BF1048576 BI1:BI1048576 BL1:BL1048576 BZ1:BZ1048576">
-    <cfRule type="expression" dxfId="90" priority="2">
+    <cfRule type="expression" dxfId="109" priority="2">
       <formula>AND(ISNUMBER(F1),OR(ROUND(F1,2)&lt;0,ROUND(F1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:O1048576 AI1:AJ1048576 AL1:AM1048576 AO1:AP1048576 AR1:AS1048576 AU1:AV1048576 AX1:AY1048576 BA1:BB1048576 BD1:BE1048576 BG1:BH1048576 BJ1:BK1048576 BM1:BY1048576 CA1:CA1048576 CC1:CC1048576">
-    <cfRule type="expression" dxfId="89" priority="1">
+    <cfRule type="expression" dxfId="108" priority="1">
       <formula>AND(ISNUMBER(H1),ROUND(H1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13925,17 +13999,17 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="88" priority="6">
+    <cfRule type="expression" dxfId="107" priority="6">
       <formula>AND(ISNUMBER($J1),ROUND($J1,2)&lt;0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J1048576">
-    <cfRule type="expression" dxfId="87" priority="2">
+    <cfRule type="expression" dxfId="106" priority="2">
       <formula>AND(ISNUMBER(I1),OR(ROUND(I1,2)&gt;1,ROUND(I1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:H1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="86" priority="1">
+    <cfRule type="expression" dxfId="105" priority="1">
       <formula>AND(ISNUMBER(A1),ROUND(A1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15386,25 +15460,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:I1048576">
-    <cfRule type="expression" dxfId="85" priority="6">
+    <cfRule type="expression" dxfId="104" priority="6">
       <formula>$D1="Male"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M1048576">
-    <cfRule type="expression" dxfId="84" priority="9">
+    <cfRule type="expression" dxfId="103" priority="9">
       <formula>$D1="Female"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 J1:J1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:Z1048576 AB1:AB1048576 AD1:AD1048576 AF1:AF1048576 AH1:AH1048576 AL1:AL1048576">
-    <cfRule type="expression" dxfId="83" priority="2">
+    <cfRule type="expression" dxfId="102" priority="2">
       <formula>AND(ISNUMBER(F1),OR(ROUND(F1,2)&gt;1,ROUND(F1,2)&lt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="4">
+    <cfRule type="expression" dxfId="101" priority="4">
       <formula>AND(ISNUMBER(F1),ROUND(F1,2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576 Y1:Y1048576 AA1:AA1048576 AC1:AC1048576 AE1:AE1048576 AG1:AG1048576 AI1:AK1048576">
-    <cfRule type="expression" dxfId="81" priority="1">
+    <cfRule type="expression" dxfId="100" priority="1">
       <formula>AND(ISNUMBER(G1),ROUND(G1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16423,47 +16497,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="V1:V1048576 Y1:Y1048576">
-    <cfRule type="expression" dxfId="80" priority="7">
+    <cfRule type="expression" dxfId="99" priority="7">
       <formula>AND(ISNUMBER(V1),ROUND(SUM(V1),2)&lt;90%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:K1048576 U1:V1048576 Y1:Y1048576">
-    <cfRule type="expression" dxfId="79" priority="3">
+    <cfRule type="expression" dxfId="98" priority="3">
       <formula>AND(ISNUMBER(H1),OR(ROUND(SUM(H1),2)&gt;1,ROUND(SUM(H1),2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:J1048576">
-    <cfRule type="expression" dxfId="78" priority="2164">
+    <cfRule type="expression" dxfId="97" priority="2164">
       <formula>AND(SUM($F1)&lt;&gt;0,H1="",ROW(H1)&gt;14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="77" priority="2166">
+    <cfRule type="expression" dxfId="96" priority="2166">
       <formula>AND(SUM($G1)&gt;0,I1="",ROW(I1)&gt;14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="76" priority="4">
+    <cfRule type="expression" dxfId="95" priority="4">
       <formula>AND(ISNUMBER(H1),ROUND(SUM(H1),2)&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 L1:P1048576">
-    <cfRule type="expression" dxfId="75" priority="1">
+    <cfRule type="expression" dxfId="94" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:X1048576 Z1:AA1048576">
-    <cfRule type="expression" dxfId="74" priority="3284">
+    <cfRule type="expression" dxfId="93" priority="3284">
       <formula>AND(ISNUMBER(C1),ROUND(SUM(C1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1048576">
-    <cfRule type="expression" dxfId="73" priority="3286">
+    <cfRule type="expression" dxfId="92" priority="3286">
       <formula>AND(ISNUMBER(A1),ROUND(SUM(A1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576 T1:T1048576">
-    <cfRule type="expression" dxfId="72" priority="3287">
+    <cfRule type="expression" dxfId="91" priority="3287">
       <formula>AND(ISNUMBER(A1),ROUND(SUM(A1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16731,7 +16805,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576">
-    <cfRule type="expression" dxfId="71" priority="2">
+    <cfRule type="expression" dxfId="90" priority="2">
       <formula>AND(ISNUMBER(D1),ROUND(D1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17500,42 +17574,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="T1:U1048576">
-    <cfRule type="expression" dxfId="70" priority="26">
+    <cfRule type="expression" dxfId="89" priority="26">
       <formula>OR($C1="18-20",$C1="18+")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="expression" dxfId="69" priority="24">
+    <cfRule type="expression" dxfId="88" priority="24">
       <formula>AND(ISNUMBER($N1),ROUND(SUM($N1),2)&lt;20%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576 P1:P1048576">
-    <cfRule type="expression" dxfId="68" priority="18">
+    <cfRule type="expression" dxfId="87" priority="18">
       <formula>AND($B1&lt;&gt;"",ROW(K1)&gt;14,NOT(AND($D1="Female",$G1="Y",OR($C1="10-14",$C1="15-17"))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576 L1:L1048576">
-    <cfRule type="expression" dxfId="67" priority="17">
+    <cfRule type="expression" dxfId="86" priority="17">
       <formula>AND($E1&lt;&gt;"",ROW(L1)&gt;14,NOT(OR($C1="05-09",$C1="10-14")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="66" priority="4">
+    <cfRule type="expression" dxfId="85" priority="4">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:I1048576 O1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="65" priority="2">
+    <cfRule type="expression" dxfId="84" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:N1048576 T1:T1048576">
-    <cfRule type="expression" dxfId="64" priority="1">
+    <cfRule type="expression" dxfId="83" priority="1">
       <formula>AND(ISNUMBER(K1),OR(ROUND(SUM(K1),2)&lt;0,ROUND(SUM(K1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="63" priority="25">
+    <cfRule type="expression" dxfId="82" priority="25">
       <formula>AND(ISNUMBER($T1),SUM($R1,$S1)&gt;0,ROUND(SUM($T1),2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17834,7 +17908,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:H1048576 C1:D1048576">
-    <cfRule type="expression" dxfId="62" priority="2">
+    <cfRule type="expression" dxfId="81" priority="2">
       <formula>AND(ISNUMBER(C1),ROUND(SUM(C1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18571,32 +18645,32 @@
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="expression" dxfId="61" priority="14">
+    <cfRule type="expression" dxfId="80" priority="14">
       <formula>AND(ISNUMBER(V1),SUM($V1)&gt;SUM($U1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1048576">
-    <cfRule type="expression" dxfId="60" priority="6">
+    <cfRule type="expression" dxfId="79" priority="6">
       <formula>AND(ROW(H1)&gt;14,$C1="10-14")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="expression" dxfId="59" priority="3">
+    <cfRule type="expression" dxfId="78" priority="3">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576 F1:N1048576">
-    <cfRule type="expression" dxfId="58" priority="2">
+    <cfRule type="expression" dxfId="77" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1048576">
-    <cfRule type="expression" dxfId="57" priority="1">
+    <cfRule type="expression" dxfId="76" priority="1">
       <formula>AND(ISNUMBER(R1),OR(ROUND(SUM(R1),2)&lt;0,ROUND(SUM(R1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="56" priority="2997">
+    <cfRule type="expression" dxfId="75" priority="2997">
       <formula>AND(ROUND(SUM($S1),2)&lt;60%,SUM($U1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18618,7 +18692,7 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -19102,20 +19176,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:I1048576">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="74" priority="3">
       <formula>AND(ROW(H1)&gt;14,$E1&lt;&gt;"",NOT(OR($C1="15-19",$C1="20-24",$C1="25-29")))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="73" priority="4">
       <formula>AND(ROW(H1)&gt;14,$E1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="72" priority="2">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:O1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="71" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19137,7 +19211,7 @@
       <pane xSplit="4" ySplit="14" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19521,22 +19595,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576 G1:H1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="55" priority="7">
+    <cfRule type="expression" dxfId="70" priority="7">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="54" priority="3">
+    <cfRule type="expression" dxfId="69" priority="3">
       <formula>AND(ISNUMBER(H1),H1&lt;&gt;G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K1048576 E1:F1048576">
-    <cfRule type="expression" dxfId="53" priority="2">
+    <cfRule type="expression" dxfId="68" priority="2">
       <formula>AND(ISNUMBER(E1),ROUND(SUM(E1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="expression" dxfId="52" priority="1">
+    <cfRule type="expression" dxfId="67" priority="1">
       <formula>AND(ISNUMBER(G1),OR(ROUND(SUM(G1),2)&lt;0,ROUND(SUM(G1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35736,152 +35810,152 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="51" priority="10">
+    <cfRule type="expression" dxfId="66" priority="10">
       <formula>AND(ROW($U1)&gt;14,SUM($U1)&gt;$S1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576 V1:V1048576">
-    <cfRule type="expression" dxfId="50" priority="9">
+    <cfRule type="expression" dxfId="65" priority="9">
       <formula>AND(ROW($V1)&gt;14,SUM($V1)&gt;$T1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:T1048576 W1:Y1048576">
-    <cfRule type="expression" dxfId="49" priority="12">
+    <cfRule type="expression" dxfId="64" priority="12">
       <formula>(($S1-$U1)+($T1-$V1))&lt;SUM($W1:$Y1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576 AB1:AB1048576">
-    <cfRule type="expression" dxfId="48" priority="13">
+    <cfRule type="expression" dxfId="63" priority="13">
       <formula>AND(ROW($AB1)&gt;14,SUM($AB1)&gt;$Z1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576 AC1:AC1048576">
-    <cfRule type="expression" dxfId="47" priority="14">
+    <cfRule type="expression" dxfId="62" priority="14">
       <formula>AND(ROW($AC1)&gt;14,SUM($AC1)&gt;$AA1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:AA1048576 AD1:AF1048576">
-    <cfRule type="expression" dxfId="46" priority="16">
+    <cfRule type="expression" dxfId="61" priority="16">
       <formula>(($Z1-$AB1)+($AA1-$AC1))&lt;SUM($AD1:$AF1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AG1048576 AI1:AI1048576">
-    <cfRule type="expression" dxfId="45" priority="17">
+    <cfRule type="expression" dxfId="60" priority="17">
       <formula>AND(ROW($AI1)&gt;14,SUM($AI1)&gt;$AG1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH1:AH1048576 AJ1:AJ1048576">
-    <cfRule type="expression" dxfId="44" priority="18">
+    <cfRule type="expression" dxfId="59" priority="18">
       <formula>AND(ROW($AJ1)&gt;14,SUM($AJ1)&gt;$AH1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AH1048576 AK1:AM1048576">
-    <cfRule type="expression" dxfId="43" priority="20">
+    <cfRule type="expression" dxfId="58" priority="20">
       <formula>(($AG1-$AI1)+($AH1-$AJ1))&lt;SUM($AK1:$AM1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN1:AN1048576 AP1:AP1048576">
-    <cfRule type="expression" dxfId="42" priority="21">
+    <cfRule type="expression" dxfId="57" priority="21">
       <formula>AND(ROW($AP1)&gt;14,SUM($AP1)&gt;$AN1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO1:AO1048576 AQ1:AQ1048576">
-    <cfRule type="expression" dxfId="41" priority="22">
+    <cfRule type="expression" dxfId="56" priority="22">
       <formula>AND(ROW($AQ1)&gt;14,SUM($AQ1)&gt;$AO1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN1:AO1048576 AR1:AT1048576">
-    <cfRule type="expression" dxfId="40" priority="24">
+    <cfRule type="expression" dxfId="55" priority="24">
       <formula>(($AN1-$AP1)+($AO1-$AQ1))&lt;SUM($AR1:$AT1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU1:AU1048576 AW1:AW1048576">
-    <cfRule type="expression" dxfId="39" priority="25">
+    <cfRule type="expression" dxfId="54" priority="25">
       <formula>AND(ROW($AW1)&gt;14,SUM($AW1)&gt;$AU1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV1:AV1048576 AX1:AX1048576">
-    <cfRule type="expression" dxfId="38" priority="26">
+    <cfRule type="expression" dxfId="53" priority="26">
       <formula>AND(ROW($AX1)&gt;14,SUM($AX1)&gt;$AV1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU1:AV1048576 AY1:BA1048576">
-    <cfRule type="expression" dxfId="37" priority="28">
+    <cfRule type="expression" dxfId="52" priority="28">
       <formula>(($AU1-$AW1)+($AV1-$AX1))&lt;SUM($AY1:$BA1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB1:BB1048576 BD1:BD1048576">
-    <cfRule type="expression" dxfId="36" priority="29">
+    <cfRule type="expression" dxfId="51" priority="29">
       <formula>AND(ROW($BD1)&gt;14,SUM($BD1)&gt;$BB1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC1:BC1048576 BE1:BE1048576">
-    <cfRule type="expression" dxfId="35" priority="30">
+    <cfRule type="expression" dxfId="50" priority="30">
       <formula>AND(ROW($BE1)&gt;14,SUM($BE1)&gt;$BC1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB1:BC1048576 BF1:BH1048576">
-    <cfRule type="expression" dxfId="34" priority="32">
+    <cfRule type="expression" dxfId="49" priority="32">
       <formula>(($BB1-$BD1)+($BC1-$BE1))&lt;SUM($BF1:$BH1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI1:BI1048576 BK1:BK1048576">
-    <cfRule type="expression" dxfId="33" priority="33">
+    <cfRule type="expression" dxfId="48" priority="33">
       <formula>AND(ROW($BK1)&gt;14,SUM($BK1)&gt;$BI1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL1:BL1048576 BJ1:BJ1048576">
-    <cfRule type="expression" dxfId="32" priority="34">
+    <cfRule type="expression" dxfId="47" priority="34">
       <formula>AND(ROW($BL1)&gt;14,SUM($BL1)&gt;$BJ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI1:BJ1048576 BM1:BO1048576">
-    <cfRule type="expression" dxfId="31" priority="36">
+    <cfRule type="expression" dxfId="46" priority="36">
       <formula>(($BI1-$BK1)+($BJ1-$BL1))&lt;SUM($BM1:$BO1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP1:BP1048576 BR1:BR1048576">
-    <cfRule type="expression" dxfId="30" priority="45">
+    <cfRule type="expression" dxfId="45" priority="45">
       <formula>AND(ROW($BR1)&gt;14,SUM($BR1)&gt;$BP1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ1:BQ1048576 BS1:BS1048576">
-    <cfRule type="expression" dxfId="29" priority="1135">
+    <cfRule type="expression" dxfId="44" priority="1135">
       <formula>AND(ROW($BS1)&gt;14,SUM($BS1)&gt;$BQ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP1:BQ1048576 BT1:BV1048576">
-    <cfRule type="expression" dxfId="28" priority="1136">
+    <cfRule type="expression" dxfId="43" priority="1136">
       <formula>(($BP1-$BR1)+($BQ1-$BS1))&lt;SUM($BT1:$BV1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="42" priority="2">
       <formula>AND(ISNUMBER($F1),SUM($F1)&gt;$C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 E1:E1048576">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="41" priority="1">
       <formula>AND(ISNUMBER($G1),SUM($G1)&gt;$E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J1048576 C1:E1048576">
-    <cfRule type="expression" dxfId="25" priority="4">
+    <cfRule type="expression" dxfId="40" priority="4">
       <formula>(($C1-$F1)+($E1-$G1))&lt;SUM($H1:$J1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1048576 N1:N1048576">
-    <cfRule type="expression" dxfId="24" priority="6">
+    <cfRule type="expression" dxfId="39" priority="6">
       <formula>AND(ROW($N1)&gt;14,SUM($N1)&gt;$K1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576 O1:O1048576">
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="38" priority="5">
       <formula>AND(ROW($O1)&gt;14,SUM($O1)&gt;$M1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:M1048576 P1:R1048576">
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="37" priority="8">
       <formula>(($K1-$N1)+($M1-$O1))&lt;SUM($P1:$R1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42544,70 +42618,70 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="CH1:CH1048576 CN1:CN1048576 CT1:CT1048576">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="36" priority="13">
       <formula>AND(ROW(CH1)&gt;14,UPPER(CH1)&lt;&gt;"CUSTOM",UPPER(CH1)&lt;&gt;"MAX",UPPER(CH1)&lt;&gt;"SUM",CH1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CV1:CV1048576">
-    <cfRule type="expression" dxfId="20" priority="10">
+    <cfRule type="expression" dxfId="35" priority="10">
       <formula>AND(ROW($CV1)&gt;14,OR(SUM($CV1)&gt;SUM($CQ1),SUM($CV1)&lt;SUM($CR1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ1:CJ1048576">
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="34" priority="11">
       <formula>AND(ROW(CJ1)&gt;14,OR(CJ1&gt;CF1,CJ1&lt;CG1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:CE1048576">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>AND(ROW(I1)&gt;14,OR(SUM(I1)&gt;1,SUM(I1)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CO1:CO1048576 CU1:CU1048576 CI1:CI1048576">
-    <cfRule type="expression" dxfId="17" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>AND(ROW(CI1)&gt;14,SUM(CI1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="31" priority="4">
       <formula>AND(ROW($H1)&gt;14,ABS(ROUND(SUM($H1),0)-ROUND(SUM($G1),0))&gt;2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="30" priority="6">
       <formula>AND(ROW($H1)&gt;14,ROUND(SUM($H1),0)&lt;&gt;ROUND(SUM($G1),0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP1:CP1048576">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="29" priority="14">
       <formula>AND(ROW($CP1)&gt;14,OR(SUM($CP1)&gt;SUM($CK1),SUM($CP1)&lt;SUM($CL1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ1:CU1048576">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="28" priority="7">
       <formula>AND(ROW($CQ1)&gt;14,$A1&lt;&gt;"",OR(SUM($CQ1)=0,$CS1&lt;=1,SUM($CQ1)=SUM($CR1),AND(SUM($G1)=SUM($CQ1),SUM($CK1)=0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF1:CI1048576">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="27" priority="8">
       <formula>AND(ROW($CF1)&gt;14,$A1&lt;&gt;"",OR(SUM($CP1)=0,SUM($CV1)=0,$CM1=0,$CS1=0,SUM($CF1)=SUM($CG1),SUM($G1)&gt;=SUM($CF1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CO1:CO1048576">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="26" priority="9">
       <formula>AND(ROW($CO1)&gt;14,$A1&lt;&gt;"",UPPER($CN1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CK1:CO1048576">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>AND(ROW($CK1)&gt;14,$A1&lt;&gt;"",OR(SUM($CK1)=0,$CM1&lt;=1,SUM($CK1)=SUM($CL1),AND(SUM($G1)=SUM($CK1),SUM($CQ1)=0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CU1:CU1048576">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>AND(ROW($CU1)&gt;14,$A1&lt;&gt;"",UPPER($CT1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CI1:CI1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>AND(ROW($CF1)&gt;14,$A1&lt;&gt;"",UPPER($CH1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42801,20 +42875,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4">
-    <cfRule type="containsText" dxfId="196" priority="3" operator="containsText" text="BLANK PRIORITIZATIONS">
+    <cfRule type="containsText" dxfId="203" priority="3" operator="containsText" text="BLANK PRIORITIZATIONS">
       <formula>NOT(ISERROR(SEARCH("BLANK PRIORITIZATIONS",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="expression" dxfId="195" priority="2">
+    <cfRule type="expression" dxfId="202" priority="2">
       <formula>AND(ROW(C1)&gt;14,$B1&lt;&gt;"",C1&lt;&gt;1,C1&lt;&gt;2,C1&lt;&gt;4,C1&lt;&gt;5,C1&lt;&gt;6,C1&lt;&gt;7,C1&lt;&gt;8,C1&lt;&gt;"M",C1&lt;&gt;"NA")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="194" priority="728">
+    <cfRule type="expression" dxfId="201" priority="728">
       <formula>AND(ROW($D1)&gt;14,$D1="",$B1&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="729">
+    <cfRule type="expression" dxfId="200" priority="729">
       <formula>AND(LEFT($B1,4)&lt;&gt;"_Mil",ROW($D1)&gt;14,$D1&lt;&gt;$C1,$B1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42831,7 +42905,7 @@
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46436,7 +46510,7 @@
         <v/>
       </c>
       <c r="AP15" s="201" t="str">
-        <f>IF($C15="&lt;01",HYPERLINK("",$AO15),IF(LEFT($B15,4)="_Mil",HYPERLINK("","*For DOD Military Use Only"),IFERROR(HYPERLINK("",ROUND($AN15*AK15,0)),HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add PEPFAR Contribution %"))))</f>
+        <f>IF($C15="&lt;01",HYPERLINK("",$AO15),IF(LEFT($B15,4)="_Mil",HYPERLINK("","*For DOD Military Use Only"),IFERROR(HYPERLINK("",ROUND($AN15*AK15,0)),HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN(AK15)),"&lt;- Add PEPFAR Contribution %"))))</f>
         <v>&lt;- Add PEPFAR Contribution %</v>
       </c>
       <c r="AQ15" s="144" t="str">
@@ -46456,7 +46530,7 @@
         <v>0.95</v>
       </c>
       <c r="AU15" s="201">
-        <f>IF(AND(LEFT($B15,4)="_Mil",SUM($AP15)=0),"",IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$T:$T,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF($AT15="",HYPERLINK("#Cascade!AT"&amp;ROW(AU15),"&lt;- Add VLS Rate"),HYPERLINK("",ROUND(SUM($AP15)/$AT15,0)))))</f>
+        <f>IF(AND(LEFT($B15,4)="_Mil",SUM($AP15)=0),"",IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$T:$T,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF($AT15="",HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN(AT15)),"&lt;- Add VLS Rate"),HYPERLINK("",ROUND(SUM($AP15)/$AT15,0)))))</f>
         <v>0</v>
       </c>
       <c r="AV15" s="144" t="str">
@@ -46508,11 +46582,11 @@
         <v>0.95</v>
       </c>
       <c r="BH15" s="199" t="str">
-        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$N:$N,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(AND($AK15="",LEFT($B15,4)&lt;&gt;"_Mil"),HYPERLINK("#Cascade!AK"&amp;ROW(AK15),"&lt;- Add PEPFAR Contribution %"),IF($AX15="",HYPERLINK("#Cascade!AZ"&amp;ROW(AX15),"&lt;- Add % New Infections Diagnosed &amp; Linked"),IF($BC15="",HYPERLINK("#Cascade!BC"&amp;ROW(BC15),"&lt;- Add Linkage"),IF(LEFT($B15,4)="_Mil",HYPERLINK("","*For DOD Military Use Only"),HYPERLINK("",ROUND(SUM($N15)*IF(LEFT($B15,4)="_Mil",1,$AK15)*$AX15*$BC15,0)))))))</f>
+        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$N:$N,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(AND($AK15="",LEFT($B15,4)&lt;&gt;"_Mil"),HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN($AK15)),"&lt;- Add PEPFAR Contribution %"),IF($AX15="",HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN($AX15)),"&lt;- Add % New Infections Diagnosed &amp; Linked"),IF($BC15="",HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN($BC15)),"&lt;- Add Linkage"),IF(LEFT($B15,4)="_Mil",HYPERLINK("","*For DOD Military Use Only"),HYPERLINK("",ROUND(SUM($N15)*IF(LEFT($B15,4)="_Mil",1,$AK15)*$AX15*$BC15,0)))))))</f>
         <v>&lt;- Add PEPFAR Contribution %</v>
       </c>
       <c r="BI15" s="199">
-        <f>IF($C15="&lt;01","",IF($BG15="",HYPERLINK("#Cascade!BG"&amp;ROW($BG15),"&lt;- Add VLT Coverage"),IF($BD15="",HYPERLINK("#Cascade!BD"&amp;ROW($BD15),"&lt;- Add Eligibility Rate"),HYPERLINK("",MAX(ROUND(((SUM($AU15)/SUM($BG15)-SUM($AG15))/SUM($BD15))-SUM($BH15),0),0)))))</f>
+        <f>IF($C15="&lt;01","",IF($BG15="",HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN($BG15)),"&lt;- Add VLT Coverage"),IF($BD15="",HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN($BD15)),"&lt;- Add Eligibility Rate"),HYPERLINK("",MAX(ROUND(((SUM($AU15)/SUM($BG15)-SUM($AG15))/SUM($BD15))-SUM($BH15),0),0)))))</f>
         <v>0</v>
       </c>
       <c r="BJ15" s="201">
@@ -46556,7 +46630,7 @@
         <v>0</v>
       </c>
       <c r="BT15" s="406" t="str">
-        <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add PEPFAR Contribution %"),HYPERLINK("",ROUND($BQ15/$AK15,0))))</f>
+        <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN($AK15)),"&lt;- Add PEPFAR Contribution %"),HYPERLINK("",ROUND($BQ15/$AK15,0))))</f>
         <v>&lt;- Add PEPFAR Contribution %</v>
       </c>
       <c r="BU15" s="230" t="str">
@@ -46585,7 +46659,7 @@
         <v/>
       </c>
       <c r="CB15" s="89" t="str">
-        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$L:$L,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(SUM($BY15)=0,"",IF($BC15="",HYPERLINK("#Cascade!BC"&amp;ROW($BC15),"&lt;- Add Linkage Rate"),HYPERLINK("",ROUND($BY15/$BC15,0)))))</f>
+        <f>IF($C15="&lt;01",HYPERLINK("",IFERROR(ROUND(INDEX(EID!$L:$L,MATCH($B15,EID!$B:$B,0))/2,0),0)),IF(SUM($BY15)=0,"",IF($BC15="",HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN($BC15)),"&lt;- Add Linkage Rate"),HYPERLINK("",ROUND($BY15/$BC15,0)))))</f>
         <v/>
       </c>
       <c r="CC15" s="89" t="str">
@@ -46668,7 +46742,7 @@
         <v/>
       </c>
       <c r="CY15" s="412" t="str">
-        <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!AK"&amp;ROW($AK15),"&lt;- Add % PEPFAR Contribution"),HYPERLINK("",IF($C15="&lt;01",0,SUM($P15))+ROUND(SUM($CB15)/$AK15,0))))</f>
+        <f>IF(LEFT($B15,4)="_Mil","",IF($AK15="",HYPERLINK("#Cascade!"&amp;ADDRESS(ROW(),COLUMN($AK15)),"&lt;- Add % PEPFAR Contribution"),HYPERLINK("",IF($C15="&lt;01",0,SUM($P15))+ROUND(SUM($CB15)/$AK15,0))))</f>
         <v>&lt;- Add % PEPFAR Contribution</v>
       </c>
       <c r="CZ15"/>
@@ -46683,120 +46757,120 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="BW1:BX1048576">
-    <cfRule type="expression" dxfId="192" priority="848">
+    <cfRule type="expression" dxfId="199" priority="848">
       <formula>AND(ISNUMBER(BW1),ROUND(BW1,2)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:Y1048576 AJ1:AN1048576 AQ1:AQ1048576 BE1:BE1048576 BT1:BV1048576 CY1:CY1048576 AV1:AW1048576 AY1:AZ1048576">
-    <cfRule type="expression" dxfId="191" priority="103">
+    <cfRule type="expression" dxfId="198" priority="103">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ1:AT1048576 BI1:BI1048576 BM1:BM1048576 BO1:BP1048576 BW1:BX1048576 BZ1:CA1048576 CC1:CG1048576 CI1:CN1048576 CP1:CX1048576 AV1:BG1048576">
-    <cfRule type="expression" dxfId="190" priority="95">
+    <cfRule type="expression" dxfId="197" priority="95">
       <formula>$C1="&lt;01"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO1:BP1048576">
-    <cfRule type="expression" dxfId="189" priority="80">
+    <cfRule type="expression" dxfId="196" priority="80">
       <formula>AND(ISNUMBER(BO1),ROUND(BO1,2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO1:AO1048576 CH1:CH1048576 CO1:CO1048576">
-    <cfRule type="expression" dxfId="188" priority="7">
+    <cfRule type="expression" dxfId="195" priority="7">
       <formula>AND(ROW(AO1)&gt;14,$B1&lt;&gt;"",NOT($C1="&lt;01"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA1:CA1048576">
-    <cfRule type="expression" dxfId="187" priority="2577">
+    <cfRule type="expression" dxfId="194" priority="2577">
       <formula>AND(ISNUMBER($CA1),$CA1&lt;&gt;$BZ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576 L1:L1048576 AJ1:AM1048576 AQ1:AT1048576 AV1:AV1048576 AX1:BG1048576 BL1:BM1048576 BO1:BP1048576 BU1:BW1048576 BZ1:CA1048576 CJ1:CS1048576 CX1:CX1048576">
-    <cfRule type="expression" dxfId="186" priority="6">
+    <cfRule type="expression" dxfId="193" priority="6">
       <formula>AND(ISNUMBER(J1),OR(ROUND(J1,2)&lt;0,ROUND(J1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ1:AT1048576 AV1:AV1048576 AX1:AY1048576 BA1:BC1048576 BE1:BG1048576">
-    <cfRule type="expression" dxfId="185" priority="12">
+    <cfRule type="expression" dxfId="192" priority="12">
       <formula>AND(ISNUMBER(AQ1),ROUND(AQ1,2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU1:BV1048576">
-    <cfRule type="expression" dxfId="184" priority="10">
+    <cfRule type="expression" dxfId="191" priority="10">
       <formula>AND(ISNUMBER(BU1),ROUND(BU1,2)&lt;ROUND(90%*90%,2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM1:BM1048576">
-    <cfRule type="expression" dxfId="183" priority="8">
+    <cfRule type="expression" dxfId="190" priority="8">
       <formula>AND(ISNUMBER(BM1),ROUND(BM1,2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CN1:CN1048576 CG1:CG1048576">
-    <cfRule type="expression" dxfId="182" priority="96">
+    <cfRule type="expression" dxfId="189" priority="96">
       <formula>AND(ROW(CG1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Male")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL1:AM1048576">
-    <cfRule type="expression" dxfId="181" priority="13">
+    <cfRule type="expression" dxfId="188" priority="13">
       <formula>AND(ISNUMBER(AL1),ROUND(AL1,2)&lt;POWER(0.95,3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD1:BD1048576">
-    <cfRule type="expression" dxfId="180" priority="2952">
+    <cfRule type="expression" dxfId="187" priority="2952">
       <formula>AND(ISNUMBER(BD1),ROUND(BD1,2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:AI1048576 AN1:AP1048576 AU1:AU1048576 AW1:AW1048576 AZ1:AZ1048576 BH1:BK1048576 BN1:BN1048576 BQ1:BT1048576 BX1:BY1048576 CB1:CI1048576 CT1:CW1048576 CY1:CY1048576">
-    <cfRule type="expression" dxfId="179" priority="1">
+    <cfRule type="expression" dxfId="186" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CG1:CG1048576 CN1:CN1048576">
-    <cfRule type="expression" dxfId="178" priority="2429">
+    <cfRule type="expression" dxfId="185" priority="2429">
       <formula>AND(ROW(CG1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09",$C1="10-14"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ1:CQ1048576">
-    <cfRule type="expression" dxfId="177" priority="5">
+    <cfRule type="expression" dxfId="184" priority="5">
       <formula>AND(ISNUMBER($CC1),$CC1&gt;0,CQ1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 J1:J1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576">
-    <cfRule type="expression" dxfId="176" priority="104">
+    <cfRule type="expression" dxfId="183" priority="104">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&gt;=40%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="105">
+    <cfRule type="expression" dxfId="182" priority="105">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&gt;=20%,G1&lt;40%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="107">
+    <cfRule type="expression" dxfId="181" priority="107">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&lt;20%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD1:CE1048576 CK1:CL1048576">
-    <cfRule type="expression" dxfId="173" priority="29">
+    <cfRule type="expression" dxfId="180" priority="29">
       <formula>AND(ROW(CD1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="93">
+    <cfRule type="expression" dxfId="179" priority="93">
       <formula>AND(ROW(CD1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CB1:CP1048576">
-    <cfRule type="expression" dxfId="171" priority="2964">
+    <cfRule type="expression" dxfId="178" priority="2964">
       <formula>AND(ROW(CB1)&gt;14,$B1&lt;&gt;"",OR(SUM($CI1)&lt;0,ROUND(SUM($CP1),2)&lt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="3289">
+    <cfRule type="expression" dxfId="177" priority="3289">
       <formula>AND(ROW($CI1)&gt;14,$B1&lt;&gt;"",$C1="&lt;01",OR(SUM($CI1)&lt;&gt;0,ROUND(SUM($CP1),2)&lt;&gt;0,SUM($CC1:$CG1)&lt;&gt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="3290">
+    <cfRule type="expression" dxfId="176" priority="3290">
       <formula>AND(ROW($A1)&gt;14,$B1&lt;&gt;"",OR(ISERROR($CI1),ISERROR($CP1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CR1:CS1048576">
-    <cfRule type="expression" dxfId="168" priority="3291">
+    <cfRule type="expression" dxfId="175" priority="3291">
       <formula>AND(ISNUMBER($CC1),$CC1&lt;&gt;0,SUM(CR1)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="3292">
+    <cfRule type="expression" dxfId="174" priority="3292">
       <formula>AND(OR($C1="15-19",$C1="20-24",$C1="25-29",$C1="30-34",$C1="35-39",$C1="40-44",$C1="45-49",$C1="50-54",$C1="55-59",$C1="60-64",$C1="65+"),CR1&lt;20%,CR1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46822,10 +46896,10 @@
   <dimension ref="A1:BE15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="14" topLeftCell="AS15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AY15" sqref="AY15"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48840,71 +48914,71 @@
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="166" priority="46">
+    <cfRule type="expression" dxfId="173" priority="46">
       <formula>AND(ISNUMBER($T1),ROUND($T1,2)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL1:AL1048576 AU1:AU1048576">
-    <cfRule type="expression" dxfId="165" priority="23">
+    <cfRule type="expression" dxfId="172" priority="23">
       <formula>AND(ISNUMBER(AL1),ROUND(AL1,2)&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576">
-    <cfRule type="expression" dxfId="164" priority="48">
+    <cfRule type="expression" dxfId="171" priority="48">
       <formula>AND(ISNUMBER(AA1),ROUND(AA1,2)&gt;=0.75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Y1048576">
-    <cfRule type="expression" dxfId="163" priority="14">
+    <cfRule type="expression" dxfId="170" priority="14">
       <formula>AND(ISNUMBER($Y1),$Y1&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY1:BE1048576">
-    <cfRule type="expression" dxfId="162" priority="7">
+    <cfRule type="expression" dxfId="169" priority="7">
       <formula>AND(ROW($BE1)&gt;14,ROUND($BE1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="16">
+    <cfRule type="expression" dxfId="168" priority="16">
       <formula>AND(ROW($BE1)&gt;14,ISERROR($BE1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AC1048576">
-    <cfRule type="expression" dxfId="160" priority="3">
+    <cfRule type="expression" dxfId="167" priority="3">
       <formula>AND(ROW($AA1)&gt;14,SUM($AD1)&gt;0,SUM($AA1)&lt;=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="4">
+    <cfRule type="expression" dxfId="166" priority="4">
       <formula>AND(ROW($AC1)&gt;14,SUM($AD1)&gt;0,SUM($AC1)&lt;=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="13">
+    <cfRule type="expression" dxfId="165" priority="13">
       <formula>AND(ROW($AC1)&gt;14,ROUND($AC1,2)&gt;10%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="expression" dxfId="157" priority="1282">
+    <cfRule type="expression" dxfId="164" priority="1282">
       <formula>AND(ROW($U1)&gt;14,ISNUMBER($U1),$S1&gt;$L1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:R1048576 V1:X1048576 AH1:AK1048576 AO1:AQ1048576">
-    <cfRule type="expression" dxfId="156" priority="2178">
+    <cfRule type="expression" dxfId="163" priority="2178">
       <formula>AND(ROW(F1)&gt;14,LEFT($B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:K1048576 V1:W1048576 Y1:AC1048576 AL1:AL1048576 AS1:AU1048576 BA1:BE1048576">
-    <cfRule type="expression" dxfId="155" priority="6">
+    <cfRule type="expression" dxfId="162" priority="6">
       <formula>AND(ISNUMBER(H1),OR(ROUND(H1,2)&lt;0,ROUND(H1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 I1:I1048576 L1:S1048576 U1:U1048576 X1:X1048576 AD1:AK1048576 AM1:AR1048576 AV1:AZ1048576">
-    <cfRule type="expression" dxfId="154" priority="1">
+    <cfRule type="expression" dxfId="161" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT1:AT1048576">
-    <cfRule type="expression" dxfId="153" priority="5">
+    <cfRule type="expression" dxfId="160" priority="5">
       <formula>AND(ROW($AT1)&gt;14,SUM($AR1)&gt;0,SUM($AT1)&lt;=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="expression" dxfId="152" priority="2">
+    <cfRule type="expression" dxfId="159" priority="2">
       <formula>AND(ROW($W1)&gt;14,LEFT($B1,4)&lt;&gt;"_Mil",SUM($U1)&gt;0,SUM($W1)&lt;=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48937,10 +49011,10 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="14" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="14" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49664,47 +49738,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576 M1:M1048576 S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="151" priority="23">
+    <cfRule type="expression" dxfId="158" priority="23">
       <formula>AND(ISNUMBER(E1),ROUND(E1,2)&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="150" priority="22">
+    <cfRule type="expression" dxfId="157" priority="22">
       <formula>AND(ISNUMBER(D1),ROUND(D1,2)&lt;0.8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1048576 H1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="149" priority="5">
+    <cfRule type="expression" dxfId="156" priority="5">
       <formula>AND(ISNUMBER(D1),OR(ROUND(D1,2)&gt;1,ROUND(D1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="expression" dxfId="148" priority="1267">
+    <cfRule type="expression" dxfId="155" priority="1267">
       <formula>AND(SUM(G1)&gt;0,SUM(K1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="147" priority="2151">
+    <cfRule type="expression" dxfId="154" priority="2151">
       <formula>AND(SUM(F1)&gt;0,SUM(I1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1048576">
-    <cfRule type="expression" dxfId="146" priority="13">
+    <cfRule type="expression" dxfId="153" priority="13">
       <formula>AND(ISNUMBER($D1),ROUND($E1,2)&lt;ROUND($D1,2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576 F1:G1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576">
-    <cfRule type="expression" dxfId="145" priority="4">
+    <cfRule type="expression" dxfId="152" priority="4">
       <formula>AND(ISNUMBER(C1),C1&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="expression" dxfId="144" priority="3">
+    <cfRule type="expression" dxfId="151" priority="3">
       <formula>AND(ISNUMBER(O1),ROUND(O1,2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="expression" dxfId="143" priority="2">
+    <cfRule type="expression" dxfId="150" priority="2">
       <formula>AND(ISNUMBER(Q1),ROUND(Q1,2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49728,10 +49802,10 @@
   <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="14" topLeftCell="M15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:AB1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50665,72 +50739,72 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="142" priority="20">
+    <cfRule type="expression" dxfId="149" priority="20">
       <formula>AND(ISNUMBER(G1),G1&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="expression" dxfId="141" priority="672">
+    <cfRule type="expression" dxfId="148" priority="672">
       <formula>AND(ISNUMBER($Q1),ROUND(SUM($Q1),2)&gt;ROUND(SUM($I1),2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="140" priority="4">
+    <cfRule type="expression" dxfId="147" priority="4">
       <formula>AND(ISNUMBER($J1),SUM($J1)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="139" priority="687">
+    <cfRule type="expression" dxfId="146" priority="687">
       <formula>AND(ISNUMBER(S1),S1&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Z1048576">
-    <cfRule type="expression" dxfId="138" priority="11">
+    <cfRule type="expression" dxfId="145" priority="11">
       <formula>AND(ROW(Y1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="12">
+    <cfRule type="expression" dxfId="144" priority="12">
       <formula>AND(ROW(Y1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576">
-    <cfRule type="expression" dxfId="136" priority="9">
+    <cfRule type="expression" dxfId="143" priority="9">
       <formula>AND(ROW(AA1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09",$C1="10-14"))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="10">
+    <cfRule type="expression" dxfId="142" priority="10">
       <formula>AND(ROW(AA1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Male")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:AB1048576">
-    <cfRule type="expression" dxfId="134" priority="2">
+    <cfRule type="expression" dxfId="141" priority="2">
       <formula>AND(ROW($AB1)&gt;14,ROUND($AB1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="8">
+    <cfRule type="expression" dxfId="140" priority="8">
       <formula>AND(ROW($AB1)&gt;14,ISERROR($AB1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:N1048576 S1:S1048576 W1:AB1048576">
-    <cfRule type="expression" dxfId="132" priority="1">
+    <cfRule type="expression" dxfId="139" priority="1">
       <formula>AND(ISNUMBER(J1),OR(ROUND(J1,2)&gt;1,ROUND(J1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="expression" dxfId="131" priority="14">
+    <cfRule type="expression" dxfId="138" priority="14">
       <formula>AND(ROW($N1)&gt;14,$N1="",SUM($O1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="15">
+    <cfRule type="expression" dxfId="137" priority="15">
       <formula>AND(ISNUMBER($N1),SUM($N1)&gt;10%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="expression" dxfId="129" priority="5">
+    <cfRule type="expression" dxfId="136" priority="5">
       <formula>AND(ROW($L1)&gt;14,$L1="",SUM($O1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="7">
+    <cfRule type="expression" dxfId="135" priority="7">
       <formula>AND(ISNUMBER($L1),ROUND(SUM($L1),2)&gt;=0.75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:I1048576 O1:R1048576 T1:U1048576">
-    <cfRule type="expression" dxfId="127" priority="3">
+    <cfRule type="expression" dxfId="134" priority="3">
       <formula>AND(ISNUMBER(F1),F1&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -50756,10 +50830,10 @@
   <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="14" topLeftCell="W15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AG15" sqref="AG15"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -51991,63 +52065,63 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="expression" dxfId="126" priority="17">
+    <cfRule type="expression" dxfId="133" priority="17">
       <formula>AND(ISNUMBER($O1),OR(ROUND($O1,2)&lt;0.8,ROUND($O1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576">
-    <cfRule type="expression" dxfId="125" priority="6">
+    <cfRule type="expression" dxfId="132" priority="6">
       <formula>AND(ROW($Z1)&gt;14,$Z1="",SUM($AA1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="7">
+    <cfRule type="expression" dxfId="131" priority="7">
       <formula>AND(ROW($Z1)&gt;14,ROUND(SUM($Z1),2)&gt;0.01)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AK1048576">
-    <cfRule type="expression" dxfId="123" priority="4">
+    <cfRule type="expression" dxfId="130" priority="4">
       <formula>AND(ISNUMBER($AK1),ROUND($AK1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="19">
+    <cfRule type="expression" dxfId="129" priority="19">
       <formula>AND(ISNUMBER($AK1),ISERROR($AK1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="expression" dxfId="121" priority="11">
+    <cfRule type="expression" dxfId="128" priority="11">
       <formula>AND(ISNUMBER($P1),$P1&lt;$M1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="expression" dxfId="120" priority="20">
+    <cfRule type="expression" dxfId="127" priority="20">
       <formula>AND(ROW($V1)&gt;14,$E1&lt;&gt;"",LEFT($B1,4)&lt;&gt;"_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE1:AE1048576">
-    <cfRule type="expression" dxfId="119" priority="2164">
+    <cfRule type="expression" dxfId="126" priority="2164">
       <formula>AND(ISNUMBER($AE1),ROUND($AE1,2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M1048576">
-    <cfRule type="expression" dxfId="118" priority="27">
+    <cfRule type="expression" dxfId="125" priority="27">
       <formula>AND(ISNUMBER($L1),ISNUMBER($M1),$M1&lt;$L1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:Q1048576 T1:U1048576">
-    <cfRule type="expression" dxfId="117" priority="16">
+    <cfRule type="expression" dxfId="124" priority="16">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:X1048576">
-    <cfRule type="expression" dxfId="116" priority="5">
+    <cfRule type="expression" dxfId="123" priority="5">
       <formula>AND(ROW($X1)&gt;14,$X1="",SUM($AA1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 I1:I1048576 L1:M1048576 P1:S1048576 AA1:AD1048576 AF1:AG1048576">
-    <cfRule type="expression" dxfId="115" priority="2">
+    <cfRule type="expression" dxfId="122" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:K1048576 N1:O1048576 T1:U1048576 W1:Z1048576 AE1:AE1048576 AH1:AK1048576">
-    <cfRule type="expression" dxfId="114" priority="1">
+    <cfRule type="expression" dxfId="121" priority="1">
       <formula>AND(ISNUMBER(H1),OR(ROUND(H1,2)&lt;0,ROUND(H1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53476,45 +53550,38 @@
         <v/>
       </c>
       <c r="R15" s="96"/>
-      <c r="S15" s="230" t="str">
-        <f>IF(SUM($Q15)=0,"",100%)</f>
-        <v/>
-      </c>
-      <c r="T15" s="20" t="str">
-        <f>IF(SUM($P15)=0,"",98%)</f>
-        <v/>
-      </c>
-      <c r="U15" s="20" t="str">
-        <f>IF(SUM($P15)=0,"",98%)</f>
-        <v/>
+      <c r="S15" s="230">
+        <v>1</v>
+      </c>
+      <c r="T15" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="U15" s="20">
+        <v>0.98</v>
       </c>
       <c r="V15" s="56" t="str">
         <f>IF(SUM($P15)=0,"",ROUND(($P15-($O15*$T15))/$U15,0))</f>
         <v/>
       </c>
-      <c r="W15" s="146" t="str">
-        <f>IF(SUM($V15)=0,"",70%)</f>
-        <v/>
-      </c>
-      <c r="X15" s="39" t="str">
-        <f>IF(SUM($V15)=0,"",100%)</f>
-        <v/>
+      <c r="W15" s="146">
+        <v>0.7</v>
+      </c>
+      <c r="X15" s="39">
+        <v>0.95</v>
       </c>
       <c r="Y15" s="56" t="str">
         <f>IF(SUM($V15,$O15)=0,"",ROUND(($V15*$W15+$O15)*$X15,0))</f>
         <v/>
       </c>
-      <c r="Z15" s="146" t="str">
-        <f>IF(SUM($Y15)=0,"",95%)</f>
-        <v/>
+      <c r="Z15" s="146">
+        <v>0.95</v>
       </c>
       <c r="AA15" s="56" t="str">
         <f>IF(SUM($Y15)=0,"",ROUND($Y15*$Z15,0))</f>
         <v/>
       </c>
-      <c r="AB15" s="144" t="str">
-        <f>IF(SUM($V15)=0,"",0%)</f>
-        <v/>
+      <c r="AB15" s="144">
+        <v>0</v>
       </c>
       <c r="AC15" s="59" t="str">
         <f>IF(OR(SUM($V15)=0,SUM($AB15)=0),"",ROUND($V15*$AB15,0))</f>
@@ -53526,9 +53593,8 @@
       </c>
       <c r="AE15" s="59"/>
       <c r="AF15" s="59"/>
-      <c r="AG15" s="20" t="str">
-        <f>IF(SUM($AD15)=0,"",95%)</f>
-        <v/>
+      <c r="AG15" s="20">
+        <v>0.95</v>
       </c>
       <c r="AH15" s="20"/>
       <c r="AI15" s="56" t="str">
@@ -53539,9 +53605,8 @@
         <f>IF(SUM($AI15)=0,"",ROUND($AI15/$AH15-$AI15,0))</f>
         <v/>
       </c>
-      <c r="AK15" s="144" t="str">
-        <f>IF(SUM($AI15)=0,"",100%)</f>
-        <v/>
+      <c r="AK15" s="144">
+        <v>1</v>
       </c>
       <c r="AL15" s="56" t="str">
         <f>IF(SUM($AI15)=0,"",ROUND($AI15*$AK15,0))</f>
@@ -53551,63 +53616,58 @@
       <c r="AN15" s="56"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="X1:X1048576">
-    <cfRule type="expression" dxfId="113" priority="31">
-      <formula>AND(ISNUMBER($X1),ROUND(SUM($Y1),0)&gt;0,ROUND(SUM($X1),2)&lt;1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z1:Z1048576">
-    <cfRule type="expression" dxfId="112" priority="32">
+  <conditionalFormatting sqref="X1:X1048576 Z1:Z1048576">
+    <cfRule type="expression" dxfId="22" priority="32">
       <formula>AND(ISNUMBER($Z1),SUM($Y1)&gt;0,ROUND(SUM($Z1),2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK1:AK1048576">
-    <cfRule type="expression" dxfId="111" priority="30">
+    <cfRule type="expression" dxfId="21" priority="30">
       <formula>AND(ISNUMBER($AK1),SUM($AI1)&gt;0,ROUND(SUM($AK1),2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G1048576">
-    <cfRule type="expression" dxfId="110" priority="17">
+    <cfRule type="expression" dxfId="20" priority="17">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="expression" dxfId="109" priority="11">
+    <cfRule type="expression" dxfId="19" priority="11">
       <formula>AND(ISNUMBER($W1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($W1),2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AG1048576">
-    <cfRule type="expression" dxfId="108" priority="10">
+    <cfRule type="expression" dxfId="18" priority="10">
       <formula>AND(ISNUMBER($AG1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($AG1),2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="expression" dxfId="107" priority="8">
+    <cfRule type="expression" dxfId="17" priority="8">
       <formula>AND(ISNUMBER($U1),SUM($V1)&gt;0,ROUND(SUM($U1),2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="106" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>AND(ISNUMBER($S1),ROUND(SUM($S1),2)&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB1:AB1048576">
-    <cfRule type="expression" dxfId="105" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>AND(ISNUMBER($AB1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($AB1),2)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:F1048576 H1:R1048576 V1:V1048576 Y1:Y1048576 AA1:AA1048576 AC1:AF1048576 AI1:AJ1048576 AL1:AN1048576">
-    <cfRule type="expression" dxfId="104" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>AND(ISNUMBER(E1),ROUND(E1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 S1:U1048576 W1:X1048576 Z1:Z1048576 AB1:AB1048576 AG1:AH1048576 AK1:AK1048576">
-    <cfRule type="expression" dxfId="103" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>AND(ISNUMBER(G1),OR(ROUND(G1,2)&lt;0,ROUND(G1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="102" priority="7">
+    <cfRule type="expression" dxfId="12" priority="7">
       <formula>AND(ISNUMBER($T1),SUM($P1)&gt;0,ROUND(SUM($T1),2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Address formula issues in COP22 DP template
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_Data_Pack_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54521DAF-CB1E-CE47-B92C-68958AD80A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9709E852-F92F-9C41-895B-4414505BC284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10480" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -8147,233 +8147,7 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="3" xr:uid="{EBDE175B-1152-3C44-B18E-2B948C595077}"/>
   </cellStyles>
-  <dxfs count="204">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="192">
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -9329,6 +9103,114 @@
       <fill>
         <patternFill patternType="darkUp">
           <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13528,67 +13410,67 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="N1:N1048576 U1:U1048576 BW1:BW1048576">
-    <cfRule type="expression" dxfId="120" priority="25">
+    <cfRule type="expression" dxfId="97" priority="25">
       <formula>OR($D1="Female",$C1="01-04",$C1="05-09",$C1="10-14")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:X1048576 AK1:AP1048576">
-    <cfRule type="expression" dxfId="119" priority="355">
+    <cfRule type="expression" dxfId="96" priority="355">
       <formula>AND(ROW(W1)&gt;14,$B1&lt;&gt;"",$C1&lt;&gt;"01-04")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA1:CC1048576">
-    <cfRule type="expression" dxfId="118" priority="197">
+    <cfRule type="expression" dxfId="95" priority="197">
       <formula>OR($C1="01-04",$C1="05-09")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1048576 R1:S1048576 BT1:BU1048576">
-    <cfRule type="expression" dxfId="117" priority="34">
+    <cfRule type="expression" dxfId="94" priority="34">
       <formula>OR($D1="Male",$C1="01-04",$C1="05-09")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ1:BQ1048576">
-    <cfRule type="expression" dxfId="116" priority="680">
+    <cfRule type="expression" dxfId="93" priority="680">
       <formula>AND(ISNUMBER($BQ1),ROUND(SUM($BQ1),0)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH1:AH1048576 AQ1:AQ1048576 AT1:AT1048576 AW1:AW1048576 AZ1:AZ1048576">
-    <cfRule type="expression" dxfId="115" priority="30">
+    <cfRule type="expression" dxfId="92" priority="30">
       <formula>AND(ISNUMBER(AH1),OR(AND($F1&gt;=0.7,ROUND(AH1,2)&lt;0.1),AND($F1&lt;0.7,ROUND(AH1,2)&lt;0.05)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ1:AJ1048576 AM1:AM1048576 AP1:AP1048576 AS1:AS1048576 AV1:AV1048576 AY1:AY1048576 BB1:BB1048576 BH1:BH1048576 BN1:BN1048576 BK1:BK1048576 BE1:BE1048576">
-    <cfRule type="containsText" dxfId="114" priority="26" operator="containsText" text="ENTER YIELD!">
+    <cfRule type="containsText" dxfId="91" priority="26" operator="containsText" text="ENTER YIELD!">
       <formula>NOT(ISERROR(SEARCH("ENTER YIELD!",AJ1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF1:AF1048576">
-    <cfRule type="expression" dxfId="113" priority="2165">
+    <cfRule type="expression" dxfId="90" priority="2165">
       <formula>AND(ISNUMBER($AF1),ROUND(SUM($F1),2)&gt;=80%,(SUM($H1)*SUM($AF1))&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:AG1048576">
-    <cfRule type="expression" dxfId="112" priority="2168">
+    <cfRule type="expression" dxfId="89" priority="2168">
       <formula>AND(ISNUMBER($AG1),ROUND($AG1,2)&lt;&gt;1,ROUND($H1,0)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM1:BN1048576">
-    <cfRule type="expression" dxfId="111" priority="2170">
+    <cfRule type="expression" dxfId="88" priority="2170">
       <formula>AND(ISNUMBER(BM1),SUM($F1)&gt;=80%,SUM(BM1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="expression" dxfId="110" priority="5">
+    <cfRule type="expression" dxfId="87" priority="5">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 P1:AH1048576 AK1:AK1048576 AN1:AN1048576 AQ1:AQ1048576 AT1:AT1048576 AW1:AW1048576 AZ1:AZ1048576 BC1:BC1048576 BF1:BF1048576 BI1:BI1048576 BL1:BL1048576 BZ1:BZ1048576">
-    <cfRule type="expression" dxfId="109" priority="2">
+    <cfRule type="expression" dxfId="86" priority="2">
       <formula>AND(ISNUMBER(F1),OR(ROUND(F1,2)&lt;0,ROUND(F1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:O1048576 AI1:AJ1048576 AL1:AM1048576 AO1:AP1048576 AR1:AS1048576 AU1:AV1048576 AX1:AY1048576 BA1:BB1048576 BD1:BE1048576 BG1:BH1048576 BJ1:BK1048576 BM1:BY1048576 CA1:CA1048576 CC1:CC1048576">
-    <cfRule type="expression" dxfId="108" priority="1">
+    <cfRule type="expression" dxfId="85" priority="1">
       <formula>AND(ISNUMBER(H1),ROUND(H1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13999,17 +13881,17 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="107" priority="6">
+    <cfRule type="expression" dxfId="84" priority="6">
       <formula>AND(ISNUMBER($J1),ROUND($J1,2)&lt;0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J1048576">
-    <cfRule type="expression" dxfId="106" priority="2">
+    <cfRule type="expression" dxfId="83" priority="2">
       <formula>AND(ISNUMBER(I1),OR(ROUND(I1,2)&gt;1,ROUND(I1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:H1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="105" priority="1">
+    <cfRule type="expression" dxfId="82" priority="1">
       <formula>AND(ISNUMBER(A1),ROUND(A1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15460,25 +15342,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:I1048576">
-    <cfRule type="expression" dxfId="104" priority="6">
+    <cfRule type="expression" dxfId="81" priority="6">
       <formula>$D1="Male"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M1048576">
-    <cfRule type="expression" dxfId="103" priority="9">
+    <cfRule type="expression" dxfId="80" priority="9">
       <formula>$D1="Female"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 J1:J1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:Z1048576 AB1:AB1048576 AD1:AD1048576 AF1:AF1048576 AH1:AH1048576 AL1:AL1048576">
-    <cfRule type="expression" dxfId="102" priority="2">
+    <cfRule type="expression" dxfId="79" priority="2">
       <formula>AND(ISNUMBER(F1),OR(ROUND(F1,2)&gt;1,ROUND(F1,2)&lt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="4">
+    <cfRule type="expression" dxfId="78" priority="4">
       <formula>AND(ISNUMBER(F1),ROUND(F1,2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576 Y1:Y1048576 AA1:AA1048576 AC1:AC1048576 AE1:AE1048576 AG1:AG1048576 AI1:AK1048576">
-    <cfRule type="expression" dxfId="100" priority="1">
+    <cfRule type="expression" dxfId="77" priority="1">
       <formula>AND(ISNUMBER(G1),ROUND(G1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16497,47 +16379,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="V1:V1048576 Y1:Y1048576">
-    <cfRule type="expression" dxfId="99" priority="7">
+    <cfRule type="expression" dxfId="76" priority="7">
       <formula>AND(ISNUMBER(V1),ROUND(SUM(V1),2)&lt;90%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:K1048576 U1:V1048576 Y1:Y1048576">
-    <cfRule type="expression" dxfId="98" priority="3">
+    <cfRule type="expression" dxfId="75" priority="3">
       <formula>AND(ISNUMBER(H1),OR(ROUND(SUM(H1),2)&gt;1,ROUND(SUM(H1),2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:J1048576">
-    <cfRule type="expression" dxfId="97" priority="2164">
+    <cfRule type="expression" dxfId="74" priority="2164">
       <formula>AND(SUM($F1)&lt;&gt;0,H1="",ROW(H1)&gt;14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="96" priority="2166">
+    <cfRule type="expression" dxfId="73" priority="2166">
       <formula>AND(SUM($G1)&gt;0,I1="",ROW(I1)&gt;14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="95" priority="4">
+    <cfRule type="expression" dxfId="72" priority="4">
       <formula>AND(ISNUMBER(H1),ROUND(SUM(H1),2)&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 L1:P1048576">
-    <cfRule type="expression" dxfId="94" priority="1">
+    <cfRule type="expression" dxfId="71" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:X1048576 Z1:AA1048576">
-    <cfRule type="expression" dxfId="93" priority="3284">
+    <cfRule type="expression" dxfId="70" priority="3284">
       <formula>AND(ISNUMBER(C1),ROUND(SUM(C1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1048576">
-    <cfRule type="expression" dxfId="92" priority="3286">
+    <cfRule type="expression" dxfId="69" priority="3286">
       <formula>AND(ISNUMBER(A1),ROUND(SUM(A1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576 T1:T1048576">
-    <cfRule type="expression" dxfId="91" priority="3287">
+    <cfRule type="expression" dxfId="68" priority="3287">
       <formula>AND(ISNUMBER(A1),ROUND(SUM(A1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16805,7 +16687,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576">
-    <cfRule type="expression" dxfId="90" priority="2">
+    <cfRule type="expression" dxfId="67" priority="2">
       <formula>AND(ISNUMBER(D1),ROUND(D1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17560,7 +17442,7 @@
         <v/>
       </c>
       <c r="S15" s="56" t="str">
-        <f>IF(SUM($O15)=0,"",($O15*$M15)-$R15)</f>
+        <f>IF(SUM($O15)=0,"",ROUND($O15*$M15,0)-$R15)</f>
         <v/>
       </c>
       <c r="T15" s="144" t="str">
@@ -17574,42 +17456,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="T1:U1048576">
-    <cfRule type="expression" dxfId="89" priority="26">
+    <cfRule type="expression" dxfId="66" priority="26">
       <formula>OR($C1="18-20",$C1="18+")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="expression" dxfId="88" priority="24">
+    <cfRule type="expression" dxfId="65" priority="24">
       <formula>AND(ISNUMBER($N1),ROUND(SUM($N1),2)&lt;20%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576 P1:P1048576">
-    <cfRule type="expression" dxfId="87" priority="18">
+    <cfRule type="expression" dxfId="64" priority="18">
       <formula>AND($B1&lt;&gt;"",ROW(K1)&gt;14,NOT(AND($D1="Female",$G1="Y",OR($C1="10-14",$C1="15-17"))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576 L1:L1048576">
-    <cfRule type="expression" dxfId="86" priority="17">
+    <cfRule type="expression" dxfId="63" priority="17">
       <formula>AND($E1&lt;&gt;"",ROW(L1)&gt;14,NOT(OR($C1="05-09",$C1="10-14")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="85" priority="4">
+    <cfRule type="expression" dxfId="62" priority="4">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:I1048576 O1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="84" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:N1048576 T1:T1048576">
-    <cfRule type="expression" dxfId="83" priority="1">
+    <cfRule type="expression" dxfId="60" priority="1">
       <formula>AND(ISNUMBER(K1),OR(ROUND(SUM(K1),2)&lt;0,ROUND(SUM(K1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="82" priority="25">
+    <cfRule type="expression" dxfId="59" priority="25">
       <formula>AND(ISNUMBER($T1),SUM($R1,$S1)&gt;0,ROUND(SUM($T1),2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17908,7 +17790,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:H1048576 C1:D1048576">
-    <cfRule type="expression" dxfId="81" priority="2">
+    <cfRule type="expression" dxfId="58" priority="2">
       <formula>AND(ISNUMBER(C1),ROUND(SUM(C1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18631,7 +18513,7 @@
         <v/>
       </c>
       <c r="U15" s="56" t="str">
-        <f>IF(SUM($Q15)=0,"",SUM($Q15)*(1+$T15))</f>
+        <f>IF(SUM($Q15)=0,"",ROUND(SUM($Q15)*(1+$T15),0))</f>
         <v/>
       </c>
       <c r="V15" s="56" t="str">
@@ -18645,32 +18527,32 @@
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="expression" dxfId="80" priority="14">
+    <cfRule type="expression" dxfId="57" priority="14">
       <formula>AND(ISNUMBER(V1),SUM($V1)&gt;SUM($U1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1048576">
-    <cfRule type="expression" dxfId="79" priority="6">
+    <cfRule type="expression" dxfId="56" priority="6">
       <formula>AND(ROW(H1)&gt;14,$C1="10-14")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="expression" dxfId="78" priority="3">
+    <cfRule type="expression" dxfId="55" priority="3">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576 F1:N1048576">
-    <cfRule type="expression" dxfId="77" priority="2">
+    <cfRule type="expression" dxfId="54" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1048576">
-    <cfRule type="expression" dxfId="76" priority="1">
+    <cfRule type="expression" dxfId="53" priority="1">
       <formula>AND(ISNUMBER(R1),OR(ROUND(SUM(R1),2)&lt;0,ROUND(SUM(R1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="75" priority="2997">
+    <cfRule type="expression" dxfId="52" priority="2997">
       <formula>AND(ROUND(SUM($S1),2)&lt;60%,SUM($U1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19176,20 +19058,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:I1048576">
-    <cfRule type="expression" dxfId="74" priority="3">
+    <cfRule type="expression" dxfId="51" priority="3">
       <formula>AND(ROW(H1)&gt;14,$E1&lt;&gt;"",NOT(OR($C1="15-19",$C1="20-24",$C1="25-29")))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="4">
+    <cfRule type="expression" dxfId="50" priority="4">
       <formula>AND(ROW(H1)&gt;14,$E1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="72" priority="2">
+    <cfRule type="expression" dxfId="49" priority="2">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:O1048576">
-    <cfRule type="expression" dxfId="71" priority="1">
+    <cfRule type="expression" dxfId="48" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19585,32 +19467,32 @@
         <v/>
       </c>
       <c r="J15" s="56" t="str">
-        <f>IF(SUM($F15)=0,"",$F15*(1+SUM($I15)))</f>
+        <f>IF(SUM($F15)=0,"",ROUND($F15*(1+SUM($I15)),0))</f>
         <v/>
       </c>
       <c r="K15" s="56" t="str">
-        <f>IF(SUM($H15)=0,"",SUM($J15)/$H15)</f>
+        <f>IF(SUM($H15)=0,"",ROUND(SUM($J15)/$H15,0))</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576 G1:H1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="70" priority="7">
+    <cfRule type="expression" dxfId="47" priority="7">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="69" priority="3">
+    <cfRule type="expression" dxfId="46" priority="3">
       <formula>AND(ISNUMBER(H1),H1&lt;&gt;G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K1048576 E1:F1048576">
-    <cfRule type="expression" dxfId="68" priority="2">
+    <cfRule type="expression" dxfId="45" priority="2">
       <formula>AND(ISNUMBER(E1),ROUND(SUM(E1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="expression" dxfId="67" priority="1">
+    <cfRule type="expression" dxfId="44" priority="1">
       <formula>AND(ISNUMBER(G1),OR(ROUND(SUM(G1),2)&lt;0,ROUND(SUM(G1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33534,7 +33416,7 @@
   <dimension ref="A1:BV63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="14" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="14" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
@@ -35810,152 +35692,152 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="66" priority="10">
+    <cfRule type="expression" dxfId="43" priority="10">
       <formula>AND(ROW($U1)&gt;14,SUM($U1)&gt;$S1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576 V1:V1048576">
-    <cfRule type="expression" dxfId="65" priority="9">
+    <cfRule type="expression" dxfId="42" priority="9">
       <formula>AND(ROW($V1)&gt;14,SUM($V1)&gt;$T1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:T1048576 W1:Y1048576">
-    <cfRule type="expression" dxfId="64" priority="12">
+    <cfRule type="expression" dxfId="41" priority="12">
       <formula>(($S1-$U1)+($T1-$V1))&lt;SUM($W1:$Y1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576 AB1:AB1048576">
-    <cfRule type="expression" dxfId="63" priority="13">
+    <cfRule type="expression" dxfId="40" priority="13">
       <formula>AND(ROW($AB1)&gt;14,SUM($AB1)&gt;$Z1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576 AC1:AC1048576">
-    <cfRule type="expression" dxfId="62" priority="14">
+    <cfRule type="expression" dxfId="39" priority="14">
       <formula>AND(ROW($AC1)&gt;14,SUM($AC1)&gt;$AA1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:AA1048576 AD1:AF1048576">
-    <cfRule type="expression" dxfId="61" priority="16">
+    <cfRule type="expression" dxfId="38" priority="16">
       <formula>(($Z1-$AB1)+($AA1-$AC1))&lt;SUM($AD1:$AF1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AG1048576 AI1:AI1048576">
-    <cfRule type="expression" dxfId="60" priority="17">
+    <cfRule type="expression" dxfId="37" priority="17">
       <formula>AND(ROW($AI1)&gt;14,SUM($AI1)&gt;$AG1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH1:AH1048576 AJ1:AJ1048576">
-    <cfRule type="expression" dxfId="59" priority="18">
+    <cfRule type="expression" dxfId="36" priority="18">
       <formula>AND(ROW($AJ1)&gt;14,SUM($AJ1)&gt;$AH1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AH1048576 AK1:AM1048576">
-    <cfRule type="expression" dxfId="58" priority="20">
+    <cfRule type="expression" dxfId="35" priority="20">
       <formula>(($AG1-$AI1)+($AH1-$AJ1))&lt;SUM($AK1:$AM1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN1:AN1048576 AP1:AP1048576">
-    <cfRule type="expression" dxfId="57" priority="21">
+    <cfRule type="expression" dxfId="34" priority="21">
       <formula>AND(ROW($AP1)&gt;14,SUM($AP1)&gt;$AN1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO1:AO1048576 AQ1:AQ1048576">
-    <cfRule type="expression" dxfId="56" priority="22">
+    <cfRule type="expression" dxfId="33" priority="22">
       <formula>AND(ROW($AQ1)&gt;14,SUM($AQ1)&gt;$AO1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN1:AO1048576 AR1:AT1048576">
-    <cfRule type="expression" dxfId="55" priority="24">
+    <cfRule type="expression" dxfId="32" priority="24">
       <formula>(($AN1-$AP1)+($AO1-$AQ1))&lt;SUM($AR1:$AT1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU1:AU1048576 AW1:AW1048576">
-    <cfRule type="expression" dxfId="54" priority="25">
+    <cfRule type="expression" dxfId="31" priority="25">
       <formula>AND(ROW($AW1)&gt;14,SUM($AW1)&gt;$AU1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV1:AV1048576 AX1:AX1048576">
-    <cfRule type="expression" dxfId="53" priority="26">
+    <cfRule type="expression" dxfId="30" priority="26">
       <formula>AND(ROW($AX1)&gt;14,SUM($AX1)&gt;$AV1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU1:AV1048576 AY1:BA1048576">
-    <cfRule type="expression" dxfId="52" priority="28">
+    <cfRule type="expression" dxfId="29" priority="28">
       <formula>(($AU1-$AW1)+($AV1-$AX1))&lt;SUM($AY1:$BA1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB1:BB1048576 BD1:BD1048576">
-    <cfRule type="expression" dxfId="51" priority="29">
+    <cfRule type="expression" dxfId="28" priority="29">
       <formula>AND(ROW($BD1)&gt;14,SUM($BD1)&gt;$BB1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC1:BC1048576 BE1:BE1048576">
-    <cfRule type="expression" dxfId="50" priority="30">
+    <cfRule type="expression" dxfId="27" priority="30">
       <formula>AND(ROW($BE1)&gt;14,SUM($BE1)&gt;$BC1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB1:BC1048576 BF1:BH1048576">
-    <cfRule type="expression" dxfId="49" priority="32">
+    <cfRule type="expression" dxfId="26" priority="32">
       <formula>(($BB1-$BD1)+($BC1-$BE1))&lt;SUM($BF1:$BH1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI1:BI1048576 BK1:BK1048576">
-    <cfRule type="expression" dxfId="48" priority="33">
+    <cfRule type="expression" dxfId="25" priority="33">
       <formula>AND(ROW($BK1)&gt;14,SUM($BK1)&gt;$BI1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL1:BL1048576 BJ1:BJ1048576">
-    <cfRule type="expression" dxfId="47" priority="34">
+    <cfRule type="expression" dxfId="24" priority="34">
       <formula>AND(ROW($BL1)&gt;14,SUM($BL1)&gt;$BJ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI1:BJ1048576 BM1:BO1048576">
-    <cfRule type="expression" dxfId="46" priority="36">
+    <cfRule type="expression" dxfId="23" priority="36">
       <formula>(($BI1-$BK1)+($BJ1-$BL1))&lt;SUM($BM1:$BO1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP1:BP1048576 BR1:BR1048576">
-    <cfRule type="expression" dxfId="45" priority="45">
+    <cfRule type="expression" dxfId="22" priority="45">
       <formula>AND(ROW($BR1)&gt;14,SUM($BR1)&gt;$BP1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ1:BQ1048576 BS1:BS1048576">
-    <cfRule type="expression" dxfId="44" priority="1135">
+    <cfRule type="expression" dxfId="21" priority="1135">
       <formula>AND(ROW($BS1)&gt;14,SUM($BS1)&gt;$BQ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP1:BQ1048576 BT1:BV1048576">
-    <cfRule type="expression" dxfId="43" priority="1136">
+    <cfRule type="expression" dxfId="20" priority="1136">
       <formula>(($BP1-$BR1)+($BQ1-$BS1))&lt;SUM($BT1:$BV1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="42" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>AND(ISNUMBER($F1),SUM($F1)&gt;$C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 E1:E1048576">
-    <cfRule type="expression" dxfId="41" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>AND(ISNUMBER($G1),SUM($G1)&gt;$E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J1048576 C1:E1048576">
-    <cfRule type="expression" dxfId="40" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>(($C1-$F1)+($E1-$G1))&lt;SUM($H1:$J1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1048576 N1:N1048576">
-    <cfRule type="expression" dxfId="39" priority="6">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>AND(ROW($N1)&gt;14,SUM($N1)&gt;$K1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576 O1:O1048576">
-    <cfRule type="expression" dxfId="38" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>AND(ROW($O1)&gt;14,SUM($O1)&gt;$M1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:M1048576 P1:R1048576">
-    <cfRule type="expression" dxfId="37" priority="8">
+    <cfRule type="expression" dxfId="14" priority="8">
       <formula>(($K1-$N1)+($M1-$O1))&lt;SUM($P1:$R1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42618,70 +42500,70 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="CH1:CH1048576 CN1:CN1048576 CT1:CT1048576">
-    <cfRule type="expression" dxfId="36" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>AND(ROW(CH1)&gt;14,UPPER(CH1)&lt;&gt;"CUSTOM",UPPER(CH1)&lt;&gt;"MAX",UPPER(CH1)&lt;&gt;"SUM",CH1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CV1:CV1048576">
-    <cfRule type="expression" dxfId="35" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>AND(ROW($CV1)&gt;14,OR(SUM($CV1)&gt;SUM($CQ1),SUM($CV1)&lt;SUM($CR1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ1:CJ1048576">
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>AND(ROW(CJ1)&gt;14,OR(CJ1&gt;CF1,CJ1&lt;CG1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:CE1048576">
-    <cfRule type="expression" dxfId="33" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>AND(ROW(I1)&gt;14,OR(SUM(I1)&gt;1,SUM(I1)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CO1:CO1048576 CU1:CU1048576 CI1:CI1048576">
-    <cfRule type="expression" dxfId="32" priority="12">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>AND(ROW(CI1)&gt;14,SUM(CI1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="31" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>AND(ROW($H1)&gt;14,ABS(ROUND(SUM($H1),0)-ROUND(SUM($G1),0))&gt;2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>AND(ROW($H1)&gt;14,ROUND(SUM($H1),0)&lt;&gt;ROUND(SUM($G1),0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP1:CP1048576">
-    <cfRule type="expression" dxfId="29" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>AND(ROW($CP1)&gt;14,OR(SUM($CP1)&gt;SUM($CK1),SUM($CP1)&lt;SUM($CL1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ1:CU1048576">
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>AND(ROW($CQ1)&gt;14,$A1&lt;&gt;"",OR(SUM($CQ1)=0,$CS1&lt;=1,SUM($CQ1)=SUM($CR1),AND(SUM($G1)=SUM($CQ1),SUM($CK1)=0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF1:CI1048576">
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>AND(ROW($CF1)&gt;14,$A1&lt;&gt;"",OR(SUM($CP1)=0,SUM($CV1)=0,$CM1=0,$CS1=0,SUM($CF1)=SUM($CG1),SUM($G1)&gt;=SUM($CF1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CO1:CO1048576">
-    <cfRule type="expression" dxfId="26" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>AND(ROW($CO1)&gt;14,$A1&lt;&gt;"",UPPER($CN1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CK1:CO1048576">
-    <cfRule type="expression" dxfId="25" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>AND(ROW($CK1)&gt;14,$A1&lt;&gt;"",OR(SUM($CK1)=0,$CM1&lt;=1,SUM($CK1)=SUM($CL1),AND(SUM($G1)=SUM($CK1),SUM($CQ1)=0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CU1:CU1048576">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(ROW($CU1)&gt;14,$A1&lt;&gt;"",UPPER($CT1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CI1:CI1048576">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(ROW($CF1)&gt;14,$A1&lt;&gt;"",UPPER($CH1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42875,20 +42757,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4">
-    <cfRule type="containsText" dxfId="203" priority="3" operator="containsText" text="BLANK PRIORITIZATIONS">
+    <cfRule type="containsText" dxfId="191" priority="3" operator="containsText" text="BLANK PRIORITIZATIONS">
       <formula>NOT(ISERROR(SEARCH("BLANK PRIORITIZATIONS",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="expression" dxfId="202" priority="2">
+    <cfRule type="expression" dxfId="190" priority="2">
       <formula>AND(ROW(C1)&gt;14,$B1&lt;&gt;"",C1&lt;&gt;1,C1&lt;&gt;2,C1&lt;&gt;4,C1&lt;&gt;5,C1&lt;&gt;6,C1&lt;&gt;7,C1&lt;&gt;8,C1&lt;&gt;"M",C1&lt;&gt;"NA")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="201" priority="728">
+    <cfRule type="expression" dxfId="189" priority="728">
       <formula>AND(ROW($D1)&gt;14,$D1="",$B1&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="729">
+    <cfRule type="expression" dxfId="188" priority="729">
       <formula>AND(LEFT($B1,4)&lt;&gt;"_Mil",ROW($D1)&gt;14,$D1&lt;&gt;$C1,$B1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46757,120 +46639,120 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="BW1:BX1048576">
-    <cfRule type="expression" dxfId="199" priority="848">
+    <cfRule type="expression" dxfId="187" priority="848">
       <formula>AND(ISNUMBER(BW1),ROUND(BW1,2)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:Y1048576 AJ1:AN1048576 AQ1:AQ1048576 BE1:BE1048576 BT1:BV1048576 CY1:CY1048576 AV1:AW1048576 AY1:AZ1048576">
-    <cfRule type="expression" dxfId="198" priority="103">
+    <cfRule type="expression" dxfId="186" priority="103">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ1:AT1048576 BI1:BI1048576 BM1:BM1048576 BO1:BP1048576 BW1:BX1048576 BZ1:CA1048576 CC1:CG1048576 CI1:CN1048576 CP1:CX1048576 AV1:BG1048576">
-    <cfRule type="expression" dxfId="197" priority="95">
+    <cfRule type="expression" dxfId="185" priority="95">
       <formula>$C1="&lt;01"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO1:BP1048576">
-    <cfRule type="expression" dxfId="196" priority="80">
+    <cfRule type="expression" dxfId="184" priority="80">
       <formula>AND(ISNUMBER(BO1),ROUND(BO1,2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO1:AO1048576 CH1:CH1048576 CO1:CO1048576">
-    <cfRule type="expression" dxfId="195" priority="7">
+    <cfRule type="expression" dxfId="183" priority="7">
       <formula>AND(ROW(AO1)&gt;14,$B1&lt;&gt;"",NOT($C1="&lt;01"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA1:CA1048576">
-    <cfRule type="expression" dxfId="194" priority="2577">
+    <cfRule type="expression" dxfId="182" priority="2577">
       <formula>AND(ISNUMBER($CA1),$CA1&lt;&gt;$BZ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576 L1:L1048576 AJ1:AM1048576 AQ1:AT1048576 AV1:AV1048576 AX1:BG1048576 BL1:BM1048576 BO1:BP1048576 BU1:BW1048576 BZ1:CA1048576 CJ1:CS1048576 CX1:CX1048576">
-    <cfRule type="expression" dxfId="193" priority="6">
+    <cfRule type="expression" dxfId="181" priority="6">
       <formula>AND(ISNUMBER(J1),OR(ROUND(J1,2)&lt;0,ROUND(J1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ1:AT1048576 AV1:AV1048576 AX1:AY1048576 BA1:BC1048576 BE1:BG1048576">
-    <cfRule type="expression" dxfId="192" priority="12">
+    <cfRule type="expression" dxfId="180" priority="12">
       <formula>AND(ISNUMBER(AQ1),ROUND(AQ1,2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU1:BV1048576">
-    <cfRule type="expression" dxfId="191" priority="10">
+    <cfRule type="expression" dxfId="179" priority="10">
       <formula>AND(ISNUMBER(BU1),ROUND(BU1,2)&lt;ROUND(90%*90%,2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM1:BM1048576">
-    <cfRule type="expression" dxfId="190" priority="8">
+    <cfRule type="expression" dxfId="178" priority="8">
       <formula>AND(ISNUMBER(BM1),ROUND(BM1,2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CN1:CN1048576 CG1:CG1048576">
-    <cfRule type="expression" dxfId="189" priority="96">
+    <cfRule type="expression" dxfId="177" priority="96">
       <formula>AND(ROW(CG1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Male")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL1:AM1048576">
-    <cfRule type="expression" dxfId="188" priority="13">
+    <cfRule type="expression" dxfId="176" priority="13">
       <formula>AND(ISNUMBER(AL1),ROUND(AL1,2)&lt;POWER(0.95,3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD1:BD1048576">
-    <cfRule type="expression" dxfId="187" priority="2952">
+    <cfRule type="expression" dxfId="175" priority="2952">
       <formula>AND(ISNUMBER(BD1),ROUND(BD1,2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:AI1048576 AN1:AP1048576 AU1:AU1048576 AW1:AW1048576 AZ1:AZ1048576 BH1:BK1048576 BN1:BN1048576 BQ1:BT1048576 BX1:BY1048576 CB1:CI1048576 CT1:CW1048576 CY1:CY1048576">
-    <cfRule type="expression" dxfId="186" priority="1">
+    <cfRule type="expression" dxfId="174" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CG1:CG1048576 CN1:CN1048576">
-    <cfRule type="expression" dxfId="185" priority="2429">
+    <cfRule type="expression" dxfId="173" priority="2429">
       <formula>AND(ROW(CG1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09",$C1="10-14"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ1:CQ1048576">
-    <cfRule type="expression" dxfId="184" priority="5">
+    <cfRule type="expression" dxfId="172" priority="5">
       <formula>AND(ISNUMBER($CC1),$CC1&gt;0,CQ1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 J1:J1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576">
-    <cfRule type="expression" dxfId="183" priority="104">
+    <cfRule type="expression" dxfId="171" priority="104">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&gt;=40%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="105">
+    <cfRule type="expression" dxfId="170" priority="105">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&gt;=20%,G1&lt;40%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="107">
+    <cfRule type="expression" dxfId="169" priority="107">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&lt;20%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD1:CE1048576 CK1:CL1048576">
-    <cfRule type="expression" dxfId="180" priority="29">
+    <cfRule type="expression" dxfId="168" priority="29">
       <formula>AND(ROW(CD1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="93">
+    <cfRule type="expression" dxfId="167" priority="93">
       <formula>AND(ROW(CD1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CB1:CP1048576">
-    <cfRule type="expression" dxfId="178" priority="2964">
+    <cfRule type="expression" dxfId="166" priority="2964">
       <formula>AND(ROW(CB1)&gt;14,$B1&lt;&gt;"",OR(SUM($CI1)&lt;0,ROUND(SUM($CP1),2)&lt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="3289">
+    <cfRule type="expression" dxfId="165" priority="3289">
       <formula>AND(ROW($CI1)&gt;14,$B1&lt;&gt;"",$C1="&lt;01",OR(SUM($CI1)&lt;&gt;0,ROUND(SUM($CP1),2)&lt;&gt;0,SUM($CC1:$CG1)&lt;&gt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="3290">
+    <cfRule type="expression" dxfId="164" priority="3290">
       <formula>AND(ROW($A1)&gt;14,$B1&lt;&gt;"",OR(ISERROR($CI1),ISERROR($CP1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CR1:CS1048576">
-    <cfRule type="expression" dxfId="175" priority="3291">
+    <cfRule type="expression" dxfId="163" priority="3291">
       <formula>AND(ISNUMBER($CC1),$CC1&lt;&gt;0,SUM(CR1)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="3292">
+    <cfRule type="expression" dxfId="162" priority="3292">
       <formula>AND(OR($C1="15-19",$C1="20-24",$C1="25-29",$C1="30-34",$C1="35-39",$C1="40-44",$C1="45-49",$C1="50-54",$C1="55-59",$C1="60-64",$C1="65+"),CR1&lt;20%,CR1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48914,71 +48796,71 @@
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="173" priority="46">
+    <cfRule type="expression" dxfId="161" priority="46">
       <formula>AND(ISNUMBER($T1),ROUND($T1,2)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL1:AL1048576 AU1:AU1048576">
-    <cfRule type="expression" dxfId="172" priority="23">
+    <cfRule type="expression" dxfId="160" priority="23">
       <formula>AND(ISNUMBER(AL1),ROUND(AL1,2)&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576">
-    <cfRule type="expression" dxfId="171" priority="48">
+    <cfRule type="expression" dxfId="159" priority="48">
       <formula>AND(ISNUMBER(AA1),ROUND(AA1,2)&gt;=0.75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Y1048576">
-    <cfRule type="expression" dxfId="170" priority="14">
+    <cfRule type="expression" dxfId="158" priority="14">
       <formula>AND(ISNUMBER($Y1),$Y1&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY1:BE1048576">
-    <cfRule type="expression" dxfId="169" priority="7">
+    <cfRule type="expression" dxfId="157" priority="7">
       <formula>AND(ROW($BE1)&gt;14,ROUND($BE1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="16">
+    <cfRule type="expression" dxfId="156" priority="16">
       <formula>AND(ROW($BE1)&gt;14,ISERROR($BE1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AC1048576">
-    <cfRule type="expression" dxfId="167" priority="3">
+    <cfRule type="expression" dxfId="155" priority="3">
       <formula>AND(ROW($AA1)&gt;14,SUM($AD1)&gt;0,SUM($AA1)&lt;=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="4">
+    <cfRule type="expression" dxfId="154" priority="4">
       <formula>AND(ROW($AC1)&gt;14,SUM($AD1)&gt;0,SUM($AC1)&lt;=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="13">
+    <cfRule type="expression" dxfId="153" priority="13">
       <formula>AND(ROW($AC1)&gt;14,ROUND($AC1,2)&gt;10%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="expression" dxfId="164" priority="1282">
+    <cfRule type="expression" dxfId="152" priority="1282">
       <formula>AND(ROW($U1)&gt;14,ISNUMBER($U1),$S1&gt;$L1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:R1048576 V1:X1048576 AH1:AK1048576 AO1:AQ1048576">
-    <cfRule type="expression" dxfId="163" priority="2178">
+    <cfRule type="expression" dxfId="151" priority="2178">
       <formula>AND(ROW(F1)&gt;14,LEFT($B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:K1048576 V1:W1048576 Y1:AC1048576 AL1:AL1048576 AS1:AU1048576 BA1:BE1048576">
-    <cfRule type="expression" dxfId="162" priority="6">
+    <cfRule type="expression" dxfId="150" priority="6">
       <formula>AND(ISNUMBER(H1),OR(ROUND(H1,2)&lt;0,ROUND(H1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 I1:I1048576 L1:S1048576 U1:U1048576 X1:X1048576 AD1:AK1048576 AM1:AR1048576 AV1:AZ1048576">
-    <cfRule type="expression" dxfId="161" priority="1">
+    <cfRule type="expression" dxfId="149" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT1:AT1048576">
-    <cfRule type="expression" dxfId="160" priority="5">
+    <cfRule type="expression" dxfId="148" priority="5">
       <formula>AND(ROW($AT1)&gt;14,SUM($AR1)&gt;0,SUM($AT1)&lt;=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="expression" dxfId="159" priority="2">
+    <cfRule type="expression" dxfId="147" priority="2">
       <formula>AND(ROW($W1)&gt;14,LEFT($B1,4)&lt;&gt;"_Mil",SUM($U1)&gt;0,SUM($W1)&lt;=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49738,47 +49620,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576 M1:M1048576 S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="158" priority="23">
+    <cfRule type="expression" dxfId="146" priority="23">
       <formula>AND(ISNUMBER(E1),ROUND(E1,2)&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="157" priority="22">
+    <cfRule type="expression" dxfId="145" priority="22">
       <formula>AND(ISNUMBER(D1),ROUND(D1,2)&lt;0.8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1048576 H1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="156" priority="5">
+    <cfRule type="expression" dxfId="144" priority="5">
       <formula>AND(ISNUMBER(D1),OR(ROUND(D1,2)&gt;1,ROUND(D1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="expression" dxfId="155" priority="1267">
+    <cfRule type="expression" dxfId="143" priority="1267">
       <formula>AND(SUM(G1)&gt;0,SUM(K1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="154" priority="2151">
+    <cfRule type="expression" dxfId="142" priority="2151">
       <formula>AND(SUM(F1)&gt;0,SUM(I1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1048576">
-    <cfRule type="expression" dxfId="153" priority="13">
+    <cfRule type="expression" dxfId="141" priority="13">
       <formula>AND(ISNUMBER($D1),ROUND($E1,2)&lt;ROUND($D1,2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576 F1:G1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576">
-    <cfRule type="expression" dxfId="152" priority="4">
+    <cfRule type="expression" dxfId="140" priority="4">
       <formula>AND(ISNUMBER(C1),C1&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="expression" dxfId="151" priority="3">
+    <cfRule type="expression" dxfId="139" priority="3">
       <formula>AND(ISNUMBER(O1),ROUND(O1,2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="expression" dxfId="150" priority="2">
+    <cfRule type="expression" dxfId="138" priority="2">
       <formula>AND(ISNUMBER(Q1),ROUND(Q1,2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -50663,7 +50545,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="56">
-        <f>SUM($F15)*(1+$G15)</f>
+        <f>ROUND(SUM($F15)*(1+$G15),0)</f>
         <v>0</v>
       </c>
       <c r="J15" s="230">
@@ -50739,72 +50621,72 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="149" priority="20">
+    <cfRule type="expression" dxfId="137" priority="20">
       <formula>AND(ISNUMBER(G1),G1&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="expression" dxfId="148" priority="672">
+    <cfRule type="expression" dxfId="136" priority="672">
       <formula>AND(ISNUMBER($Q1),ROUND(SUM($Q1),2)&gt;ROUND(SUM($I1),2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="147" priority="4">
+    <cfRule type="expression" dxfId="135" priority="4">
       <formula>AND(ISNUMBER($J1),SUM($J1)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="146" priority="687">
+    <cfRule type="expression" dxfId="134" priority="687">
       <formula>AND(ISNUMBER(S1),S1&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Z1048576">
-    <cfRule type="expression" dxfId="145" priority="11">
+    <cfRule type="expression" dxfId="133" priority="11">
       <formula>AND(ROW(Y1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="12">
+    <cfRule type="expression" dxfId="132" priority="12">
       <formula>AND(ROW(Y1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576">
-    <cfRule type="expression" dxfId="143" priority="9">
+    <cfRule type="expression" dxfId="131" priority="9">
       <formula>AND(ROW(AA1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09",$C1="10-14"))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="10">
+    <cfRule type="expression" dxfId="130" priority="10">
       <formula>AND(ROW(AA1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Male")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:AB1048576">
-    <cfRule type="expression" dxfId="141" priority="2">
+    <cfRule type="expression" dxfId="129" priority="2">
       <formula>AND(ROW($AB1)&gt;14,ROUND($AB1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="8">
+    <cfRule type="expression" dxfId="128" priority="8">
       <formula>AND(ROW($AB1)&gt;14,ISERROR($AB1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:N1048576 S1:S1048576 W1:AB1048576">
-    <cfRule type="expression" dxfId="139" priority="1">
+    <cfRule type="expression" dxfId="127" priority="1">
       <formula>AND(ISNUMBER(J1),OR(ROUND(J1,2)&gt;1,ROUND(J1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="expression" dxfId="138" priority="14">
+    <cfRule type="expression" dxfId="126" priority="14">
       <formula>AND(ROW($N1)&gt;14,$N1="",SUM($O1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="15">
+    <cfRule type="expression" dxfId="125" priority="15">
       <formula>AND(ISNUMBER($N1),SUM($N1)&gt;10%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="expression" dxfId="136" priority="5">
+    <cfRule type="expression" dxfId="124" priority="5">
       <formula>AND(ROW($L1)&gt;14,$L1="",SUM($O1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="7">
+    <cfRule type="expression" dxfId="123" priority="7">
       <formula>AND(ISNUMBER($L1),ROUND(SUM($L1),2)&gt;=0.75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:I1048576 O1:R1048576 T1:U1048576">
-    <cfRule type="expression" dxfId="134" priority="3">
+    <cfRule type="expression" dxfId="122" priority="3">
       <formula>AND(ISNUMBER(F1),F1&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52065,63 +51947,63 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="expression" dxfId="133" priority="17">
+    <cfRule type="expression" dxfId="121" priority="17">
       <formula>AND(ISNUMBER($O1),OR(ROUND($O1,2)&lt;0.8,ROUND($O1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576">
-    <cfRule type="expression" dxfId="132" priority="6">
+    <cfRule type="expression" dxfId="120" priority="6">
       <formula>AND(ROW($Z1)&gt;14,$Z1="",SUM($AA1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="7">
+    <cfRule type="expression" dxfId="119" priority="7">
       <formula>AND(ROW($Z1)&gt;14,ROUND(SUM($Z1),2)&gt;0.01)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AK1048576">
-    <cfRule type="expression" dxfId="130" priority="4">
+    <cfRule type="expression" dxfId="118" priority="4">
       <formula>AND(ISNUMBER($AK1),ROUND($AK1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="19">
+    <cfRule type="expression" dxfId="117" priority="19">
       <formula>AND(ISNUMBER($AK1),ISERROR($AK1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="expression" dxfId="128" priority="11">
+    <cfRule type="expression" dxfId="116" priority="11">
       <formula>AND(ISNUMBER($P1),$P1&lt;$M1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="expression" dxfId="127" priority="20">
+    <cfRule type="expression" dxfId="115" priority="20">
       <formula>AND(ROW($V1)&gt;14,$E1&lt;&gt;"",LEFT($B1,4)&lt;&gt;"_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE1:AE1048576">
-    <cfRule type="expression" dxfId="126" priority="2164">
+    <cfRule type="expression" dxfId="114" priority="2164">
       <formula>AND(ISNUMBER($AE1),ROUND($AE1,2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M1048576">
-    <cfRule type="expression" dxfId="125" priority="27">
+    <cfRule type="expression" dxfId="113" priority="27">
       <formula>AND(ISNUMBER($L1),ISNUMBER($M1),$M1&lt;$L1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:Q1048576 T1:U1048576">
-    <cfRule type="expression" dxfId="124" priority="16">
+    <cfRule type="expression" dxfId="112" priority="16">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:X1048576">
-    <cfRule type="expression" dxfId="123" priority="5">
+    <cfRule type="expression" dxfId="111" priority="5">
       <formula>AND(ROW($X1)&gt;14,$X1="",SUM($AA1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 I1:I1048576 L1:M1048576 P1:S1048576 AA1:AD1048576 AF1:AG1048576">
-    <cfRule type="expression" dxfId="122" priority="2">
+    <cfRule type="expression" dxfId="110" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:K1048576 N1:O1048576 T1:U1048576 W1:Z1048576 AE1:AE1048576 AH1:AK1048576">
-    <cfRule type="expression" dxfId="121" priority="1">
+    <cfRule type="expression" dxfId="109" priority="1">
       <formula>AND(ISNUMBER(H1),OR(ROUND(H1,2)&lt;0,ROUND(H1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53617,57 +53499,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="X1:X1048576 Z1:Z1048576">
-    <cfRule type="expression" dxfId="22" priority="32">
+    <cfRule type="expression" dxfId="108" priority="32">
       <formula>AND(ISNUMBER($Z1),SUM($Y1)&gt;0,ROUND(SUM($Z1),2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK1:AK1048576">
-    <cfRule type="expression" dxfId="21" priority="30">
+    <cfRule type="expression" dxfId="107" priority="30">
       <formula>AND(ISNUMBER($AK1),SUM($AI1)&gt;0,ROUND(SUM($AK1),2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G1048576">
-    <cfRule type="expression" dxfId="20" priority="17">
+    <cfRule type="expression" dxfId="106" priority="17">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="105" priority="11">
       <formula>AND(ISNUMBER($W1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($W1),2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AG1048576">
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="104" priority="10">
       <formula>AND(ISNUMBER($AG1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($AG1),2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="103" priority="8">
       <formula>AND(ISNUMBER($U1),SUM($V1)&gt;0,ROUND(SUM($U1),2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="102" priority="4">
       <formula>AND(ISNUMBER($S1),ROUND(SUM($S1),2)&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB1:AB1048576">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="101" priority="5">
       <formula>AND(ISNUMBER($AB1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($AB1),2)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:F1048576 H1:R1048576 V1:V1048576 Y1:Y1048576 AA1:AA1048576 AC1:AF1048576 AI1:AJ1048576 AL1:AN1048576">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="100" priority="2">
       <formula>AND(ISNUMBER(E1),ROUND(E1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 S1:U1048576 W1:X1048576 Z1:Z1048576 AB1:AB1048576 AG1:AH1048576 AK1:AK1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="99" priority="1">
       <formula>AND(ISNUMBER(G1),OR(ROUND(G1,2)&lt;0,ROUND(G1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="98" priority="7">
       <formula>AND(ISNUMBER($T1),SUM($P1)&gt;0,ROUND(SUM($T1),2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Addresses DP-501 (EID 12 mo % to 100%)
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_Data_Pack_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9709E852-F92F-9C41-895B-4414505BC284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543D680C-2610-984C-BAC0-3E7933CB736C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
@@ -49557,8 +49557,7 @@
         <v>0.95</v>
       </c>
       <c r="E15" s="20">
-        <f>MAX(95%,SUM($D15))</f>
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F15" s="56">
         <f>ROUND(SUM($C15)*$D15,0)</f>

</xml_diff>

<commit_message>
Address cond fmtng for Index yields <10% instead of 20%
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_Data_Pack_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543D680C-2610-984C-BAC0-3E7933CB736C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6314B4-AC33-2D4A-AF0A-1BE11FAD4A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>To estimate PEPFAR's share of Host Country VLS, the Data Pack looks first at PEPFAR TX_PVLS (N) vs. Host Country PVLS. If Host Country PVLS is not provided, the Data Pack looks next at TX_CURR vs. Host Country ART.</t>
+          <t>To estimate PEPFAR's Contribution to the HIV Response in the Host Country, the Data Pack compares PEPFAR TX_CURR vs. Host Country ART.</t>
         </r>
       </text>
     </comment>
@@ -639,7 +639,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">HTS_INDEX yields &lt;20% for 15+ yr olds. Encourage testing strategies that prioritize testing among high yield populations, or work to increase yields through more refined identification methods.
+          <t xml:space="preserve">HTS_INDEX yields &lt;10% for 15+ yr olds. Encourage testing strategies that prioritize testing among high yield populations, or work to increase yields through more refined identification methods.
 </t>
         </r>
         <r>
@@ -692,7 +692,8 @@
             <rFont val="Tahoma"/>
             <family val="34"/>
           </rPr>
-          <t>HTS_INDEX yields &lt;20% for 15+ yr olds. Encourage testing strategies that prioritize testing among high yield populations, or work to increase yields through more refined identification methods.</t>
+          <t xml:space="preserve">HTS_INDEX yields &lt;10% for 15+ yr olds. Encourage testing strategies that prioritize testing among high yield populations, or work to increase yields through more refined identification methods.
+</t>
         </r>
         <r>
           <rPr>
@@ -8147,7 +8148,499 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="3" xr:uid="{EBDE175B-1152-3C44-B18E-2B948C595077}"/>
   </cellStyles>
-  <dxfs count="192">
+  <dxfs count="218">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -9770,252 +10263,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -10343,7 +10590,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13410,67 +13657,67 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="N1:N1048576 U1:U1048576 BW1:BW1048576">
-    <cfRule type="expression" dxfId="97" priority="25">
+    <cfRule type="expression" dxfId="149" priority="25">
       <formula>OR($D1="Female",$C1="01-04",$C1="05-09",$C1="10-14")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:X1048576 AK1:AP1048576">
-    <cfRule type="expression" dxfId="96" priority="355">
+    <cfRule type="expression" dxfId="148" priority="355">
       <formula>AND(ROW(W1)&gt;14,$B1&lt;&gt;"",$C1&lt;&gt;"01-04")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA1:CC1048576">
-    <cfRule type="expression" dxfId="95" priority="197">
+    <cfRule type="expression" dxfId="147" priority="197">
       <formula>OR($C1="01-04",$C1="05-09")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1048576 R1:S1048576 BT1:BU1048576">
-    <cfRule type="expression" dxfId="94" priority="34">
+    <cfRule type="expression" dxfId="146" priority="34">
       <formula>OR($D1="Male",$C1="01-04",$C1="05-09")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ1:BQ1048576">
-    <cfRule type="expression" dxfId="93" priority="680">
+    <cfRule type="expression" dxfId="145" priority="680">
       <formula>AND(ISNUMBER($BQ1),ROUND(SUM($BQ1),0)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH1:AH1048576 AQ1:AQ1048576 AT1:AT1048576 AW1:AW1048576 AZ1:AZ1048576">
-    <cfRule type="expression" dxfId="92" priority="30">
+    <cfRule type="expression" dxfId="144" priority="30">
       <formula>AND(ISNUMBER(AH1),OR(AND($F1&gt;=0.7,ROUND(AH1,2)&lt;0.1),AND($F1&lt;0.7,ROUND(AH1,2)&lt;0.05)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ1:AJ1048576 AM1:AM1048576 AP1:AP1048576 AS1:AS1048576 AV1:AV1048576 AY1:AY1048576 BB1:BB1048576 BH1:BH1048576 BN1:BN1048576 BK1:BK1048576 BE1:BE1048576">
-    <cfRule type="containsText" dxfId="91" priority="26" operator="containsText" text="ENTER YIELD!">
+    <cfRule type="containsText" dxfId="143" priority="26" operator="containsText" text="ENTER YIELD!">
       <formula>NOT(ISERROR(SEARCH("ENTER YIELD!",AJ1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF1:AF1048576">
-    <cfRule type="expression" dxfId="90" priority="2165">
+    <cfRule type="expression" dxfId="142" priority="2165">
       <formula>AND(ISNUMBER($AF1),ROUND(SUM($F1),2)&gt;=80%,(SUM($H1)*SUM($AF1))&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:AG1048576">
-    <cfRule type="expression" dxfId="89" priority="2168">
+    <cfRule type="expression" dxfId="141" priority="2168">
       <formula>AND(ISNUMBER($AG1),ROUND($AG1,2)&lt;&gt;1,ROUND($H1,0)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM1:BN1048576">
-    <cfRule type="expression" dxfId="88" priority="2170">
+    <cfRule type="expression" dxfId="140" priority="2170">
       <formula>AND(ISNUMBER(BM1),SUM($F1)&gt;=80%,SUM(BM1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="expression" dxfId="87" priority="5">
+    <cfRule type="expression" dxfId="139" priority="5">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 P1:AH1048576 AK1:AK1048576 AN1:AN1048576 AQ1:AQ1048576 AT1:AT1048576 AW1:AW1048576 AZ1:AZ1048576 BC1:BC1048576 BF1:BF1048576 BI1:BI1048576 BL1:BL1048576 BZ1:BZ1048576">
-    <cfRule type="expression" dxfId="86" priority="2">
+    <cfRule type="expression" dxfId="138" priority="2">
       <formula>AND(ISNUMBER(F1),OR(ROUND(F1,2)&lt;0,ROUND(F1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:O1048576 AI1:AJ1048576 AL1:AM1048576 AO1:AP1048576 AR1:AS1048576 AU1:AV1048576 AX1:AY1048576 BA1:BB1048576 BD1:BE1048576 BG1:BH1048576 BJ1:BK1048576 BM1:BY1048576 CA1:CA1048576 CC1:CC1048576">
-    <cfRule type="expression" dxfId="85" priority="1">
+    <cfRule type="expression" dxfId="137" priority="1">
       <formula>AND(ISNUMBER(H1),ROUND(H1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13881,17 +14128,17 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="84" priority="6">
+    <cfRule type="expression" dxfId="136" priority="6">
       <formula>AND(ISNUMBER($J1),ROUND($J1,2)&lt;0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J1048576">
-    <cfRule type="expression" dxfId="83" priority="2">
+    <cfRule type="expression" dxfId="135" priority="2">
       <formula>AND(ISNUMBER(I1),OR(ROUND(I1,2)&gt;1,ROUND(I1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:H1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="82" priority="1">
+    <cfRule type="expression" dxfId="134" priority="1">
       <formula>AND(ISNUMBER(A1),ROUND(A1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15342,25 +15589,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:I1048576">
-    <cfRule type="expression" dxfId="81" priority="6">
+    <cfRule type="expression" dxfId="133" priority="6">
       <formula>$D1="Male"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M1048576">
-    <cfRule type="expression" dxfId="80" priority="9">
+    <cfRule type="expression" dxfId="132" priority="9">
       <formula>$D1="Female"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 J1:J1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:Z1048576 AB1:AB1048576 AD1:AD1048576 AF1:AF1048576 AH1:AH1048576 AL1:AL1048576">
-    <cfRule type="expression" dxfId="79" priority="2">
+    <cfRule type="expression" dxfId="131" priority="2">
       <formula>AND(ISNUMBER(F1),OR(ROUND(F1,2)&gt;1,ROUND(F1,2)&lt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="4">
+    <cfRule type="expression" dxfId="130" priority="4">
       <formula>AND(ISNUMBER(F1),ROUND(F1,2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576 Y1:Y1048576 AA1:AA1048576 AC1:AC1048576 AE1:AE1048576 AG1:AG1048576 AI1:AK1048576">
-    <cfRule type="expression" dxfId="77" priority="1">
+    <cfRule type="expression" dxfId="129" priority="1">
       <formula>AND(ISNUMBER(G1),ROUND(G1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16379,47 +16626,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="V1:V1048576 Y1:Y1048576">
-    <cfRule type="expression" dxfId="76" priority="7">
+    <cfRule type="expression" dxfId="128" priority="7">
       <formula>AND(ISNUMBER(V1),ROUND(SUM(V1),2)&lt;90%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:K1048576 U1:V1048576 Y1:Y1048576">
-    <cfRule type="expression" dxfId="75" priority="3">
+    <cfRule type="expression" dxfId="127" priority="3">
       <formula>AND(ISNUMBER(H1),OR(ROUND(SUM(H1),2)&gt;1,ROUND(SUM(H1),2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:J1048576">
-    <cfRule type="expression" dxfId="74" priority="2164">
+    <cfRule type="expression" dxfId="126" priority="2164">
       <formula>AND(SUM($F1)&lt;&gt;0,H1="",ROW(H1)&gt;14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="73" priority="2166">
+    <cfRule type="expression" dxfId="125" priority="2166">
       <formula>AND(SUM($G1)&gt;0,I1="",ROW(I1)&gt;14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="72" priority="4">
+    <cfRule type="expression" dxfId="124" priority="4">
       <formula>AND(ISNUMBER(H1),ROUND(SUM(H1),2)&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 L1:P1048576">
-    <cfRule type="expression" dxfId="71" priority="1">
+    <cfRule type="expression" dxfId="123" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:X1048576 Z1:AA1048576">
-    <cfRule type="expression" dxfId="70" priority="3284">
+    <cfRule type="expression" dxfId="122" priority="3284">
       <formula>AND(ISNUMBER(C1),ROUND(SUM(C1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1048576">
-    <cfRule type="expression" dxfId="69" priority="3286">
+    <cfRule type="expression" dxfId="121" priority="3286">
       <formula>AND(ISNUMBER(A1),ROUND(SUM(A1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576 T1:T1048576">
-    <cfRule type="expression" dxfId="68" priority="3287">
+    <cfRule type="expression" dxfId="120" priority="3287">
       <formula>AND(ISNUMBER(A1),ROUND(SUM(A1),2)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16687,7 +16934,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576">
-    <cfRule type="expression" dxfId="67" priority="2">
+    <cfRule type="expression" dxfId="119" priority="2">
       <formula>AND(ISNUMBER(D1),ROUND(D1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17456,42 +17703,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="T1:U1048576">
-    <cfRule type="expression" dxfId="66" priority="26">
+    <cfRule type="expression" dxfId="118" priority="26">
       <formula>OR($C1="18-20",$C1="18+")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="expression" dxfId="65" priority="24">
+    <cfRule type="expression" dxfId="117" priority="24">
       <formula>AND(ISNUMBER($N1),ROUND(SUM($N1),2)&lt;20%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576 P1:P1048576">
-    <cfRule type="expression" dxfId="64" priority="18">
+    <cfRule type="expression" dxfId="116" priority="18">
       <formula>AND($B1&lt;&gt;"",ROW(K1)&gt;14,NOT(AND($D1="Female",$G1="Y",OR($C1="10-14",$C1="15-17"))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576 L1:L1048576">
-    <cfRule type="expression" dxfId="63" priority="17">
+    <cfRule type="expression" dxfId="115" priority="17">
       <formula>AND($E1&lt;&gt;"",ROW(L1)&gt;14,NOT(OR($C1="05-09",$C1="10-14")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="62" priority="4">
+    <cfRule type="expression" dxfId="114" priority="4">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:I1048576 O1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="61" priority="2">
+    <cfRule type="expression" dxfId="113" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:N1048576 T1:T1048576">
-    <cfRule type="expression" dxfId="60" priority="1">
+    <cfRule type="expression" dxfId="112" priority="1">
       <formula>AND(ISNUMBER(K1),OR(ROUND(SUM(K1),2)&lt;0,ROUND(SUM(K1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="59" priority="25">
+    <cfRule type="expression" dxfId="111" priority="25">
       <formula>AND(ISNUMBER($T1),SUM($R1,$S1)&gt;0,ROUND(SUM($T1),2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17790,7 +18037,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:H1048576 C1:D1048576">
-    <cfRule type="expression" dxfId="58" priority="2">
+    <cfRule type="expression" dxfId="110" priority="2">
       <formula>AND(ISNUMBER(C1),ROUND(SUM(C1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18527,32 +18774,32 @@
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="expression" dxfId="57" priority="14">
+    <cfRule type="expression" dxfId="109" priority="14">
       <formula>AND(ISNUMBER(V1),SUM($V1)&gt;SUM($U1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1048576">
-    <cfRule type="expression" dxfId="56" priority="6">
+    <cfRule type="expression" dxfId="108" priority="6">
       <formula>AND(ROW(H1)&gt;14,$C1="10-14")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="expression" dxfId="55" priority="3">
+    <cfRule type="expression" dxfId="107" priority="3">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576 F1:N1048576">
-    <cfRule type="expression" dxfId="54" priority="2">
+    <cfRule type="expression" dxfId="106" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1048576">
-    <cfRule type="expression" dxfId="53" priority="1">
+    <cfRule type="expression" dxfId="105" priority="1">
       <formula>AND(ISNUMBER(R1),OR(ROUND(SUM(R1),2)&lt;0,ROUND(SUM(R1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="52" priority="2997">
+    <cfRule type="expression" dxfId="104" priority="2997">
       <formula>AND(ROUND(SUM($S1),2)&lt;60%,SUM($U1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19058,20 +19305,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:I1048576">
-    <cfRule type="expression" dxfId="51" priority="3">
+    <cfRule type="expression" dxfId="103" priority="3">
       <formula>AND(ROW(H1)&gt;14,$E1&lt;&gt;"",NOT(OR($C1="15-19",$C1="20-24",$C1="25-29")))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="4">
+    <cfRule type="expression" dxfId="102" priority="4">
       <formula>AND(ROW(H1)&gt;14,$E1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="49" priority="2">
+    <cfRule type="expression" dxfId="101" priority="2">
       <formula>AND(ROW(F1)&gt;14,LEFT(B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:O1048576">
-    <cfRule type="expression" dxfId="48" priority="1">
+    <cfRule type="expression" dxfId="100" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(SUM(F1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19477,22 +19724,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576 G1:H1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="47" priority="7">
+    <cfRule type="expression" dxfId="99" priority="7">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="46" priority="3">
+    <cfRule type="expression" dxfId="98" priority="3">
       <formula>AND(ISNUMBER(H1),H1&lt;&gt;G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K1048576 E1:F1048576">
-    <cfRule type="expression" dxfId="45" priority="2">
+    <cfRule type="expression" dxfId="97" priority="2">
       <formula>AND(ISNUMBER(E1),ROUND(SUM(E1),0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="expression" dxfId="44" priority="1">
+    <cfRule type="expression" dxfId="96" priority="1">
       <formula>AND(ISNUMBER(G1),OR(ROUND(SUM(G1),2)&lt;0,ROUND(SUM(G1),2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35692,152 +35939,152 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="43" priority="10">
+    <cfRule type="expression" dxfId="95" priority="10">
       <formula>AND(ROW($U1)&gt;14,SUM($U1)&gt;$S1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576 V1:V1048576">
-    <cfRule type="expression" dxfId="42" priority="9">
+    <cfRule type="expression" dxfId="94" priority="9">
       <formula>AND(ROW($V1)&gt;14,SUM($V1)&gt;$T1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:T1048576 W1:Y1048576">
-    <cfRule type="expression" dxfId="41" priority="12">
+    <cfRule type="expression" dxfId="93" priority="12">
       <formula>(($S1-$U1)+($T1-$V1))&lt;SUM($W1:$Y1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576 AB1:AB1048576">
-    <cfRule type="expression" dxfId="40" priority="13">
+    <cfRule type="expression" dxfId="92" priority="13">
       <formula>AND(ROW($AB1)&gt;14,SUM($AB1)&gt;$Z1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576 AC1:AC1048576">
-    <cfRule type="expression" dxfId="39" priority="14">
+    <cfRule type="expression" dxfId="91" priority="14">
       <formula>AND(ROW($AC1)&gt;14,SUM($AC1)&gt;$AA1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:AA1048576 AD1:AF1048576">
-    <cfRule type="expression" dxfId="38" priority="16">
+    <cfRule type="expression" dxfId="90" priority="16">
       <formula>(($Z1-$AB1)+($AA1-$AC1))&lt;SUM($AD1:$AF1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AG1048576 AI1:AI1048576">
-    <cfRule type="expression" dxfId="37" priority="17">
+    <cfRule type="expression" dxfId="89" priority="17">
       <formula>AND(ROW($AI1)&gt;14,SUM($AI1)&gt;$AG1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH1:AH1048576 AJ1:AJ1048576">
-    <cfRule type="expression" dxfId="36" priority="18">
+    <cfRule type="expression" dxfId="88" priority="18">
       <formula>AND(ROW($AJ1)&gt;14,SUM($AJ1)&gt;$AH1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AH1048576 AK1:AM1048576">
-    <cfRule type="expression" dxfId="35" priority="20">
+    <cfRule type="expression" dxfId="87" priority="20">
       <formula>(($AG1-$AI1)+($AH1-$AJ1))&lt;SUM($AK1:$AM1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN1:AN1048576 AP1:AP1048576">
-    <cfRule type="expression" dxfId="34" priority="21">
+    <cfRule type="expression" dxfId="86" priority="21">
       <formula>AND(ROW($AP1)&gt;14,SUM($AP1)&gt;$AN1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO1:AO1048576 AQ1:AQ1048576">
-    <cfRule type="expression" dxfId="33" priority="22">
+    <cfRule type="expression" dxfId="85" priority="22">
       <formula>AND(ROW($AQ1)&gt;14,SUM($AQ1)&gt;$AO1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN1:AO1048576 AR1:AT1048576">
-    <cfRule type="expression" dxfId="32" priority="24">
+    <cfRule type="expression" dxfId="84" priority="24">
       <formula>(($AN1-$AP1)+($AO1-$AQ1))&lt;SUM($AR1:$AT1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU1:AU1048576 AW1:AW1048576">
-    <cfRule type="expression" dxfId="31" priority="25">
+    <cfRule type="expression" dxfId="83" priority="25">
       <formula>AND(ROW($AW1)&gt;14,SUM($AW1)&gt;$AU1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV1:AV1048576 AX1:AX1048576">
-    <cfRule type="expression" dxfId="30" priority="26">
+    <cfRule type="expression" dxfId="82" priority="26">
       <formula>AND(ROW($AX1)&gt;14,SUM($AX1)&gt;$AV1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU1:AV1048576 AY1:BA1048576">
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="81" priority="28">
       <formula>(($AU1-$AW1)+($AV1-$AX1))&lt;SUM($AY1:$BA1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB1:BB1048576 BD1:BD1048576">
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="80" priority="29">
       <formula>AND(ROW($BD1)&gt;14,SUM($BD1)&gt;$BB1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC1:BC1048576 BE1:BE1048576">
-    <cfRule type="expression" dxfId="27" priority="30">
+    <cfRule type="expression" dxfId="79" priority="30">
       <formula>AND(ROW($BE1)&gt;14,SUM($BE1)&gt;$BC1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB1:BC1048576 BF1:BH1048576">
-    <cfRule type="expression" dxfId="26" priority="32">
+    <cfRule type="expression" dxfId="78" priority="32">
       <formula>(($BB1-$BD1)+($BC1-$BE1))&lt;SUM($BF1:$BH1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI1:BI1048576 BK1:BK1048576">
-    <cfRule type="expression" dxfId="25" priority="33">
+    <cfRule type="expression" dxfId="77" priority="33">
       <formula>AND(ROW($BK1)&gt;14,SUM($BK1)&gt;$BI1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL1:BL1048576 BJ1:BJ1048576">
-    <cfRule type="expression" dxfId="24" priority="34">
+    <cfRule type="expression" dxfId="76" priority="34">
       <formula>AND(ROW($BL1)&gt;14,SUM($BL1)&gt;$BJ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI1:BJ1048576 BM1:BO1048576">
-    <cfRule type="expression" dxfId="23" priority="36">
+    <cfRule type="expression" dxfId="75" priority="36">
       <formula>(($BI1-$BK1)+($BJ1-$BL1))&lt;SUM($BM1:$BO1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP1:BP1048576 BR1:BR1048576">
-    <cfRule type="expression" dxfId="22" priority="45">
+    <cfRule type="expression" dxfId="74" priority="45">
       <formula>AND(ROW($BR1)&gt;14,SUM($BR1)&gt;$BP1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ1:BQ1048576 BS1:BS1048576">
-    <cfRule type="expression" dxfId="21" priority="1135">
+    <cfRule type="expression" dxfId="73" priority="1135">
       <formula>AND(ROW($BS1)&gt;14,SUM($BS1)&gt;$BQ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP1:BQ1048576 BT1:BV1048576">
-    <cfRule type="expression" dxfId="20" priority="1136">
+    <cfRule type="expression" dxfId="72" priority="1136">
       <formula>(($BP1-$BR1)+($BQ1-$BS1))&lt;SUM($BT1:$BV1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="71" priority="2">
       <formula>AND(ISNUMBER($F1),SUM($F1)&gt;$C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 E1:E1048576">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="70" priority="1">
       <formula>AND(ISNUMBER($G1),SUM($G1)&gt;$E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J1048576 C1:E1048576">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="69" priority="4">
       <formula>(($C1-$F1)+($E1-$G1))&lt;SUM($H1:$J1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1048576 N1:N1048576">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="68" priority="6">
       <formula>AND(ROW($N1)&gt;14,SUM($N1)&gt;$K1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576 O1:O1048576">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="67" priority="5">
       <formula>AND(ROW($O1)&gt;14,SUM($O1)&gt;$M1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:M1048576 P1:R1048576">
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="66" priority="8">
       <formula>(($K1-$N1)+($M1-$O1))&lt;SUM($P1:$R1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42500,70 +42747,70 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="CH1:CH1048576 CN1:CN1048576 CT1:CT1048576">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="65" priority="13">
       <formula>AND(ROW(CH1)&gt;14,UPPER(CH1)&lt;&gt;"CUSTOM",UPPER(CH1)&lt;&gt;"MAX",UPPER(CH1)&lt;&gt;"SUM",CH1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CV1:CV1048576">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="64" priority="10">
       <formula>AND(ROW($CV1)&gt;14,OR(SUM($CV1)&gt;SUM($CQ1),SUM($CV1)&lt;SUM($CR1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ1:CJ1048576">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="63" priority="11">
       <formula>AND(ROW(CJ1)&gt;14,OR(CJ1&gt;CF1,CJ1&lt;CG1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:CE1048576">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="62" priority="3">
       <formula>AND(ROW(I1)&gt;14,OR(SUM(I1)&gt;1,SUM(I1)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CO1:CO1048576 CU1:CU1048576 CI1:CI1048576">
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="61" priority="12">
       <formula>AND(ROW(CI1)&gt;14,SUM(CI1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="60" priority="4">
       <formula>AND(ROW($H1)&gt;14,ABS(ROUND(SUM($H1),0)-ROUND(SUM($G1),0))&gt;2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="59" priority="6">
       <formula>AND(ROW($H1)&gt;14,ROUND(SUM($H1),0)&lt;&gt;ROUND(SUM($G1),0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP1:CP1048576">
-    <cfRule type="expression" dxfId="6" priority="14">
+    <cfRule type="expression" dxfId="58" priority="14">
       <formula>AND(ROW($CP1)&gt;14,OR(SUM($CP1)&gt;SUM($CK1),SUM($CP1)&lt;SUM($CL1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ1:CU1048576">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="57" priority="7">
       <formula>AND(ROW($CQ1)&gt;14,$A1&lt;&gt;"",OR(SUM($CQ1)=0,$CS1&lt;=1,SUM($CQ1)=SUM($CR1),AND(SUM($G1)=SUM($CQ1),SUM($CK1)=0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF1:CI1048576">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="56" priority="8">
       <formula>AND(ROW($CF1)&gt;14,$A1&lt;&gt;"",OR(SUM($CP1)=0,SUM($CV1)=0,$CM1=0,$CS1=0,SUM($CF1)=SUM($CG1),SUM($G1)&gt;=SUM($CF1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CO1:CO1048576">
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="55" priority="9">
       <formula>AND(ROW($CO1)&gt;14,$A1&lt;&gt;"",UPPER($CN1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CK1:CO1048576">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="54" priority="5">
       <formula>AND(ROW($CK1)&gt;14,$A1&lt;&gt;"",OR(SUM($CK1)=0,$CM1&lt;=1,SUM($CK1)=SUM($CL1),AND(SUM($G1)=SUM($CK1),SUM($CQ1)=0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CU1:CU1048576">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="53" priority="2">
       <formula>AND(ROW($CU1)&gt;14,$A1&lt;&gt;"",UPPER($CT1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CI1:CI1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="52" priority="1">
       <formula>AND(ROW($CF1)&gt;14,$A1&lt;&gt;"",UPPER($CH1)&lt;&gt;"CUSTOM")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42757,20 +43004,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4">
-    <cfRule type="containsText" dxfId="191" priority="3" operator="containsText" text="BLANK PRIORITIZATIONS">
+    <cfRule type="containsText" dxfId="217" priority="3" operator="containsText" text="BLANK PRIORITIZATIONS">
       <formula>NOT(ISERROR(SEARCH("BLANK PRIORITIZATIONS",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="expression" dxfId="190" priority="2">
+    <cfRule type="expression" dxfId="216" priority="2">
       <formula>AND(ROW(C1)&gt;14,$B1&lt;&gt;"",C1&lt;&gt;1,C1&lt;&gt;2,C1&lt;&gt;4,C1&lt;&gt;5,C1&lt;&gt;6,C1&lt;&gt;7,C1&lt;&gt;8,C1&lt;&gt;"M",C1&lt;&gt;"NA")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="189" priority="728">
+    <cfRule type="expression" dxfId="215" priority="728">
       <formula>AND(ROW($D1)&gt;14,$D1="",$B1&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="729">
+    <cfRule type="expression" dxfId="214" priority="729">
       <formula>AND(LEFT($B1,4)&lt;&gt;"_Mil",ROW($D1)&gt;14,$D1&lt;&gt;$C1,$B1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42783,7 +43030,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:DE15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -46639,121 +46886,121 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="BW1:BX1048576">
-    <cfRule type="expression" dxfId="187" priority="848">
+    <cfRule type="expression" dxfId="51" priority="848">
       <formula>AND(ISNUMBER(BW1),ROUND(BW1,2)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:Y1048576 AJ1:AN1048576 AQ1:AQ1048576 BE1:BE1048576 BT1:BV1048576 CY1:CY1048576 AV1:AW1048576 AY1:AZ1048576">
-    <cfRule type="expression" dxfId="186" priority="103">
+    <cfRule type="expression" dxfId="50" priority="103">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ1:AT1048576 BI1:BI1048576 BM1:BM1048576 BO1:BP1048576 BW1:BX1048576 BZ1:CA1048576 CC1:CG1048576 CI1:CN1048576 CP1:CX1048576 AV1:BG1048576">
-    <cfRule type="expression" dxfId="185" priority="95">
+    <cfRule type="expression" dxfId="49" priority="95">
       <formula>$C1="&lt;01"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO1:BP1048576">
-    <cfRule type="expression" dxfId="184" priority="80">
+    <cfRule type="expression" dxfId="48" priority="80">
       <formula>AND(ISNUMBER(BO1),ROUND(BO1,2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO1:AO1048576 CH1:CH1048576 CO1:CO1048576">
-    <cfRule type="expression" dxfId="183" priority="7">
+    <cfRule type="expression" dxfId="47" priority="7">
       <formula>AND(ROW(AO1)&gt;14,$B1&lt;&gt;"",NOT($C1="&lt;01"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA1:CA1048576">
-    <cfRule type="expression" dxfId="182" priority="2577">
+    <cfRule type="expression" dxfId="46" priority="2577">
       <formula>AND(ISNUMBER($CA1),$CA1&lt;&gt;$BZ1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576 L1:L1048576 AJ1:AM1048576 AQ1:AT1048576 AV1:AV1048576 AX1:BG1048576 BL1:BM1048576 BO1:BP1048576 BU1:BW1048576 BZ1:CA1048576 CJ1:CS1048576 CX1:CX1048576">
-    <cfRule type="expression" dxfId="181" priority="6">
+    <cfRule type="expression" dxfId="45" priority="6">
       <formula>AND(ISNUMBER(J1),OR(ROUND(J1,2)&lt;0,ROUND(J1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ1:AT1048576 AV1:AV1048576 AX1:AY1048576 BA1:BC1048576 BE1:BG1048576">
-    <cfRule type="expression" dxfId="180" priority="12">
+    <cfRule type="expression" dxfId="44" priority="12">
       <formula>AND(ISNUMBER(AQ1),ROUND(AQ1,2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU1:BV1048576">
-    <cfRule type="expression" dxfId="179" priority="10">
+    <cfRule type="expression" dxfId="43" priority="10">
       <formula>AND(ISNUMBER(BU1),ROUND(BU1,2)&lt;ROUND(90%*90%,2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM1:BM1048576">
-    <cfRule type="expression" dxfId="178" priority="8">
+    <cfRule type="expression" dxfId="42" priority="8">
       <formula>AND(ISNUMBER(BM1),ROUND(BM1,2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CN1:CN1048576 CG1:CG1048576">
-    <cfRule type="expression" dxfId="177" priority="96">
+    <cfRule type="expression" dxfId="41" priority="96">
       <formula>AND(ROW(CG1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Male")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL1:AM1048576">
-    <cfRule type="expression" dxfId="176" priority="13">
+    <cfRule type="expression" dxfId="40" priority="13">
       <formula>AND(ISNUMBER(AL1),ROUND(AL1,2)&lt;POWER(0.95,3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD1:BD1048576">
-    <cfRule type="expression" dxfId="175" priority="2952">
+    <cfRule type="expression" dxfId="39" priority="2952">
       <formula>AND(ISNUMBER(BD1),ROUND(BD1,2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:AI1048576 AN1:AP1048576 AU1:AU1048576 AW1:AW1048576 AZ1:AZ1048576 BH1:BK1048576 BN1:BN1048576 BQ1:BT1048576 BX1:BY1048576 CB1:CI1048576 CT1:CW1048576 CY1:CY1048576">
-    <cfRule type="expression" dxfId="174" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CG1:CG1048576 CN1:CN1048576">
-    <cfRule type="expression" dxfId="173" priority="2429">
+    <cfRule type="expression" dxfId="37" priority="2429">
       <formula>AND(ROW(CG1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09",$C1="10-14"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ1:CQ1048576">
-    <cfRule type="expression" dxfId="172" priority="5">
+    <cfRule type="expression" dxfId="36" priority="5">
       <formula>AND(ISNUMBER($CC1),$CC1&gt;0,CQ1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:H1048576 J1:J1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576">
-    <cfRule type="expression" dxfId="171" priority="104">
+    <cfRule type="expression" dxfId="35" priority="104">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&gt;=40%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="105">
+    <cfRule type="expression" dxfId="34" priority="105">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&gt;=20%,G1&lt;40%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="107">
+    <cfRule type="expression" dxfId="33" priority="107">
       <formula>AND(ISNUMBER(G1),ISNUMBER(F1),G1&lt;20%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD1:CE1048576 CK1:CL1048576">
-    <cfRule type="expression" dxfId="168" priority="29">
+    <cfRule type="expression" dxfId="32" priority="29">
       <formula>AND(ROW(CD1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="93">
+    <cfRule type="expression" dxfId="31" priority="93">
       <formula>AND(ROW(CD1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CB1:CP1048576">
-    <cfRule type="expression" dxfId="166" priority="2964">
+    <cfRule type="expression" dxfId="30" priority="2964">
       <formula>AND(ROW(CB1)&gt;14,$B1&lt;&gt;"",OR(SUM($CI1)&lt;0,ROUND(SUM($CP1),2)&lt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="3289">
+    <cfRule type="expression" dxfId="29" priority="3289">
       <formula>AND(ROW($CI1)&gt;14,$B1&lt;&gt;"",$C1="&lt;01",OR(SUM($CI1)&lt;&gt;0,ROUND(SUM($CP1),2)&lt;&gt;0,SUM($CC1:$CG1)&lt;&gt;0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="3290">
+    <cfRule type="expression" dxfId="28" priority="3290">
       <formula>AND(ROW($A1)&gt;14,$B1&lt;&gt;"",OR(ISERROR($CI1),ISERROR($CP1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CR1:CS1048576">
-    <cfRule type="expression" dxfId="163" priority="3291">
+    <cfRule type="expression" dxfId="27" priority="3291">
       <formula>AND(ISNUMBER($CC1),$CC1&lt;&gt;0,SUM(CR1)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="3292">
-      <formula>AND(OR($C1="15-19",$C1="20-24",$C1="25-29",$C1="30-34",$C1="35-39",$C1="40-44",$C1="45-49",$C1="50-54",$C1="55-59",$C1="60-64",$C1="65+"),CR1&lt;20%,CR1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="26" priority="3292">
+      <formula>AND(OR($C1="15-19",$C1="20-24",$C1="25-29",$C1="30-34",$C1="35-39",$C1="40-44",$C1="45-49",$C1="50-54",$C1="55-59",$C1="60-64",$C1="65+"),CR1&lt;10%,CR1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -48796,71 +49043,71 @@
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="161" priority="46">
+    <cfRule type="expression" dxfId="213" priority="46">
       <formula>AND(ISNUMBER($T1),ROUND($T1,2)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL1:AL1048576 AU1:AU1048576">
-    <cfRule type="expression" dxfId="160" priority="23">
+    <cfRule type="expression" dxfId="212" priority="23">
       <formula>AND(ISNUMBER(AL1),ROUND(AL1,2)&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576">
-    <cfRule type="expression" dxfId="159" priority="48">
+    <cfRule type="expression" dxfId="211" priority="48">
       <formula>AND(ISNUMBER(AA1),ROUND(AA1,2)&gt;=0.75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Y1048576">
-    <cfRule type="expression" dxfId="158" priority="14">
+    <cfRule type="expression" dxfId="210" priority="14">
       <formula>AND(ISNUMBER($Y1),$Y1&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY1:BE1048576">
-    <cfRule type="expression" dxfId="157" priority="7">
+    <cfRule type="expression" dxfId="209" priority="7">
       <formula>AND(ROW($BE1)&gt;14,ROUND($BE1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="16">
+    <cfRule type="expression" dxfId="208" priority="16">
       <formula>AND(ROW($BE1)&gt;14,ISERROR($BE1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AC1048576">
-    <cfRule type="expression" dxfId="155" priority="3">
+    <cfRule type="expression" dxfId="207" priority="3">
       <formula>AND(ROW($AA1)&gt;14,SUM($AD1)&gt;0,SUM($AA1)&lt;=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="4">
+    <cfRule type="expression" dxfId="206" priority="4">
       <formula>AND(ROW($AC1)&gt;14,SUM($AD1)&gt;0,SUM($AC1)&lt;=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="13">
+    <cfRule type="expression" dxfId="205" priority="13">
       <formula>AND(ROW($AC1)&gt;14,ROUND($AC1,2)&gt;10%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="expression" dxfId="152" priority="1282">
+    <cfRule type="expression" dxfId="204" priority="1282">
       <formula>AND(ROW($U1)&gt;14,ISNUMBER($U1),$S1&gt;$L1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:R1048576 V1:X1048576 AH1:AK1048576 AO1:AQ1048576">
-    <cfRule type="expression" dxfId="151" priority="2178">
+    <cfRule type="expression" dxfId="203" priority="2178">
       <formula>AND(ROW(F1)&gt;14,LEFT($B1,4)="_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:K1048576 V1:W1048576 Y1:AC1048576 AL1:AL1048576 AS1:AU1048576 BA1:BE1048576">
-    <cfRule type="expression" dxfId="150" priority="6">
+    <cfRule type="expression" dxfId="202" priority="6">
       <formula>AND(ISNUMBER(H1),OR(ROUND(H1,2)&lt;0,ROUND(H1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 I1:I1048576 L1:S1048576 U1:U1048576 X1:X1048576 AD1:AK1048576 AM1:AR1048576 AV1:AZ1048576">
-    <cfRule type="expression" dxfId="149" priority="1">
+    <cfRule type="expression" dxfId="201" priority="1">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT1:AT1048576">
-    <cfRule type="expression" dxfId="148" priority="5">
+    <cfRule type="expression" dxfId="200" priority="5">
       <formula>AND(ROW($AT1)&gt;14,SUM($AR1)&gt;0,SUM($AT1)&lt;=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="expression" dxfId="147" priority="2">
+    <cfRule type="expression" dxfId="199" priority="2">
       <formula>AND(ROW($W1)&gt;14,LEFT($B1,4)&lt;&gt;"_Mil",SUM($U1)&gt;0,SUM($W1)&lt;=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49619,47 +49866,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576 M1:M1048576 S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="146" priority="23">
+    <cfRule type="expression" dxfId="198" priority="23">
       <formula>AND(ISNUMBER(E1),ROUND(E1,2)&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="145" priority="22">
+    <cfRule type="expression" dxfId="197" priority="22">
       <formula>AND(ISNUMBER(D1),ROUND(D1,2)&lt;0.8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1048576 H1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576">
-    <cfRule type="expression" dxfId="144" priority="5">
+    <cfRule type="expression" dxfId="196" priority="5">
       <formula>AND(ISNUMBER(D1),OR(ROUND(D1,2)&gt;1,ROUND(D1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="expression" dxfId="143" priority="1267">
+    <cfRule type="expression" dxfId="195" priority="1267">
       <formula>AND(SUM(G1)&gt;0,SUM(K1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="142" priority="2151">
+    <cfRule type="expression" dxfId="194" priority="2151">
       <formula>AND(SUM(F1)&gt;0,SUM(I1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1048576">
-    <cfRule type="expression" dxfId="141" priority="13">
+    <cfRule type="expression" dxfId="193" priority="13">
       <formula>AND(ISNUMBER($D1),ROUND($E1,2)&lt;ROUND($D1,2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576 F1:G1048576 L1:L1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576">
-    <cfRule type="expression" dxfId="140" priority="4">
+    <cfRule type="expression" dxfId="192" priority="4">
       <formula>AND(ISNUMBER(C1),C1&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="expression" dxfId="139" priority="3">
+    <cfRule type="expression" dxfId="191" priority="3">
       <formula>AND(ISNUMBER(O1),ROUND(O1,2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="expression" dxfId="138" priority="2">
+    <cfRule type="expression" dxfId="190" priority="2">
       <formula>AND(ISNUMBER(Q1),ROUND(Q1,2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -50620,72 +50867,72 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="137" priority="20">
+    <cfRule type="expression" dxfId="189" priority="20">
       <formula>AND(ISNUMBER(G1),G1&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="expression" dxfId="136" priority="672">
+    <cfRule type="expression" dxfId="188" priority="672">
       <formula>AND(ISNUMBER($Q1),ROUND(SUM($Q1),2)&gt;ROUND(SUM($I1),2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="135" priority="4">
+    <cfRule type="expression" dxfId="187" priority="4">
       <formula>AND(ISNUMBER($J1),SUM($J1)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="134" priority="687">
+    <cfRule type="expression" dxfId="186" priority="687">
       <formula>AND(ISNUMBER(S1),S1&lt;0.95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Z1048576">
-    <cfRule type="expression" dxfId="133" priority="11">
+    <cfRule type="expression" dxfId="185" priority="11">
       <formula>AND(ROW(Y1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Female")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="12">
+    <cfRule type="expression" dxfId="184" priority="12">
       <formula>AND(ROW(Y1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576">
-    <cfRule type="expression" dxfId="131" priority="9">
+    <cfRule type="expression" dxfId="183" priority="9">
       <formula>AND(ROW(AA1)&gt;14,$B1&lt;&gt;"",OR($C1="&lt;01",$C1="01-04",$C1="05-09",$C1="10-14"))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="10">
+    <cfRule type="expression" dxfId="182" priority="10">
       <formula>AND(ROW(AA1)&gt;14,$B1&lt;&gt;"",$D1&lt;&gt;"Male")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:AB1048576">
-    <cfRule type="expression" dxfId="129" priority="2">
+    <cfRule type="expression" dxfId="181" priority="2">
       <formula>AND(ROW($AB1)&gt;14,ROUND($AB1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="8">
+    <cfRule type="expression" dxfId="180" priority="8">
       <formula>AND(ROW($AB1)&gt;14,ISERROR($AB1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:N1048576 S1:S1048576 W1:AB1048576">
-    <cfRule type="expression" dxfId="127" priority="1">
+    <cfRule type="expression" dxfId="179" priority="1">
       <formula>AND(ISNUMBER(J1),OR(ROUND(J1,2)&gt;1,ROUND(J1,2)&lt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="expression" dxfId="126" priority="14">
+    <cfRule type="expression" dxfId="178" priority="14">
       <formula>AND(ROW($N1)&gt;14,$N1="",SUM($O1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="15">
+    <cfRule type="expression" dxfId="177" priority="15">
       <formula>AND(ISNUMBER($N1),SUM($N1)&gt;10%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="expression" dxfId="124" priority="5">
+    <cfRule type="expression" dxfId="176" priority="5">
       <formula>AND(ROW($L1)&gt;14,$L1="",SUM($O1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="7">
+    <cfRule type="expression" dxfId="175" priority="7">
       <formula>AND(ISNUMBER($L1),ROUND(SUM($L1),2)&gt;=0.75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 H1:I1048576 O1:R1048576 T1:U1048576">
-    <cfRule type="expression" dxfId="122" priority="3">
+    <cfRule type="expression" dxfId="174" priority="3">
       <formula>AND(ISNUMBER(F1),F1&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51946,63 +52193,63 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="expression" dxfId="121" priority="17">
+    <cfRule type="expression" dxfId="173" priority="17">
       <formula>AND(ISNUMBER($O1),OR(ROUND($O1,2)&lt;0.8,ROUND($O1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576">
-    <cfRule type="expression" dxfId="120" priority="6">
+    <cfRule type="expression" dxfId="172" priority="6">
       <formula>AND(ROW($Z1)&gt;14,$Z1="",SUM($AA1)&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="7">
+    <cfRule type="expression" dxfId="171" priority="7">
       <formula>AND(ROW($Z1)&gt;14,ROUND(SUM($Z1),2)&gt;0.01)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AK1048576">
-    <cfRule type="expression" dxfId="118" priority="4">
+    <cfRule type="expression" dxfId="170" priority="4">
       <formula>AND(ISNUMBER($AK1),ROUND($AK1,2)&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="19">
+    <cfRule type="expression" dxfId="169" priority="19">
       <formula>AND(ISNUMBER($AK1),ISERROR($AK1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="expression" dxfId="116" priority="11">
+    <cfRule type="expression" dxfId="168" priority="11">
       <formula>AND(ISNUMBER($P1),$P1&lt;$M1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="expression" dxfId="115" priority="20">
+    <cfRule type="expression" dxfId="167" priority="20">
       <formula>AND(ROW($V1)&gt;14,$E1&lt;&gt;"",LEFT($B1,4)&lt;&gt;"_Mil")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE1:AE1048576">
-    <cfRule type="expression" dxfId="114" priority="2164">
+    <cfRule type="expression" dxfId="166" priority="2164">
       <formula>AND(ISNUMBER($AE1),ROUND($AE1,2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M1048576">
-    <cfRule type="expression" dxfId="113" priority="27">
+    <cfRule type="expression" dxfId="165" priority="27">
       <formula>AND(ISNUMBER($L1),ISNUMBER($M1),$M1&lt;$L1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:Q1048576 T1:U1048576">
-    <cfRule type="expression" dxfId="112" priority="16">
+    <cfRule type="expression" dxfId="164" priority="16">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:X1048576">
-    <cfRule type="expression" dxfId="111" priority="5">
+    <cfRule type="expression" dxfId="163" priority="5">
       <formula>AND(ROW($X1)&gt;14,$X1="",SUM($AA1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 I1:I1048576 L1:M1048576 P1:S1048576 AA1:AD1048576 AF1:AG1048576">
-    <cfRule type="expression" dxfId="110" priority="2">
+    <cfRule type="expression" dxfId="162" priority="2">
       <formula>AND(ISNUMBER(F1),ROUND(F1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 J1:K1048576 N1:O1048576 T1:U1048576 W1:Z1048576 AE1:AE1048576 AH1:AK1048576">
-    <cfRule type="expression" dxfId="109" priority="1">
+    <cfRule type="expression" dxfId="161" priority="1">
       <formula>AND(ISNUMBER(H1),OR(ROUND(H1,2)&lt;0,ROUND(H1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53498,57 +53745,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="X1:X1048576 Z1:Z1048576">
-    <cfRule type="expression" dxfId="108" priority="32">
+    <cfRule type="expression" dxfId="160" priority="32">
       <formula>AND(ISNUMBER($Z1),SUM($Y1)&gt;0,ROUND(SUM($Z1),2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK1:AK1048576">
-    <cfRule type="expression" dxfId="107" priority="30">
+    <cfRule type="expression" dxfId="159" priority="30">
       <formula>AND(ISNUMBER($AK1),SUM($AI1)&gt;0,ROUND(SUM($AK1),2)&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G1048576">
-    <cfRule type="expression" dxfId="106" priority="17">
+    <cfRule type="expression" dxfId="158" priority="17">
       <formula>LEFT($B1,4)="_Mil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="expression" dxfId="105" priority="11">
+    <cfRule type="expression" dxfId="157" priority="11">
       <formula>AND(ISNUMBER($W1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($W1),2)&lt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AG1048576">
-    <cfRule type="expression" dxfId="104" priority="10">
+    <cfRule type="expression" dxfId="156" priority="10">
       <formula>AND(ISNUMBER($AG1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($AG1),2)&lt;95%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="expression" dxfId="103" priority="8">
+    <cfRule type="expression" dxfId="155" priority="8">
       <formula>AND(ISNUMBER($U1),SUM($V1)&gt;0,ROUND(SUM($U1),2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="expression" dxfId="102" priority="4">
+    <cfRule type="expression" dxfId="154" priority="4">
       <formula>AND(ISNUMBER($S1),ROUND(SUM($S1),2)&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB1:AB1048576">
-    <cfRule type="expression" dxfId="101" priority="5">
+    <cfRule type="expression" dxfId="153" priority="5">
       <formula>AND(ISNUMBER($AB1),ROUND(SUM($V1),0)&gt;0,ROUND(SUM($AB1),2)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:F1048576 H1:R1048576 V1:V1048576 Y1:Y1048576 AA1:AA1048576 AC1:AF1048576 AI1:AJ1048576 AL1:AN1048576">
-    <cfRule type="expression" dxfId="100" priority="2">
+    <cfRule type="expression" dxfId="152" priority="2">
       <formula>AND(ISNUMBER(E1),ROUND(E1,0)&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 S1:U1048576 W1:X1048576 Z1:Z1048576 AB1:AB1048576 AG1:AH1048576 AK1:AK1048576">
-    <cfRule type="expression" dxfId="99" priority="1">
+    <cfRule type="expression" dxfId="151" priority="1">
       <formula>AND(ISNUMBER(G1),OR(ROUND(G1,2)&lt;0,ROUND(G1,2)&gt;1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="expression" dxfId="98" priority="7">
+    <cfRule type="expression" dxfId="150" priority="7">
       <formula>AND(ISNUMBER($T1),SUM($P1)&gt;0,ROUND(SUM($T1),2)&lt;98%)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>